<commit_message>
Adding eplus urban building type measure and updating gemfile to use cli for dencity.
</commit_message>
<xml_diff>
--- a/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
+++ b/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="784">
   <si>
     <t>type</t>
   </si>
@@ -2079,9 +2079,6 @@
     <t>Experiment Type</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -2133,9 +2130,6 @@
     <t>discrete</t>
   </si>
   <si>
-    <t>142484'</t>
-  </si>
-  <si>
     <t>|'142484','116245','142872','43254','1459','134032','143122','15204','155513','181948','142238','191582','185054','208359','113178','192702','236371','190013','6434','231850','128469','172662','222162','122347','158690','202694','56659','85635','3571','83186','227340','41962','217309','52660','161648','184642','3847','2373','62625','65373','58283','58911','237783','79514','110389','144568','5955','78754','96419','83574','223270','148046','191859','33879','52936','106804','221612','61663','207542','213989','49369','116055','151927','8514','100535','187338','207180','50936','11886','20763','230376','134949','151680','152016','164646','206572','178897','181797','183160','206869','187675','200594','222412','223723','233024','234608','235990','240241','203425','186746','215740','227893','230795','147716','150821','151683','155087','173389','208781','221871','236646','134575','138298','141692','146223','147538','148715','154723','155770','159371','166226','166447','185614','190700','200435','203431','209303','211686','225506','226857','231874','236181','134829','153445','188330','195998','215567','236722','240378','136118','144038','145786','156369','160789','166893','177498','184217','197688','212943','223606','224837','225080','228898','229908','234747','236146','236944','139179','140483','141333','141742','149927','150157','153100','157664','160763','164828','165203','166177','167379','169768','170121','170176','171097','172136','172760','174951','176543','188603','188635','192839','194021','194266','196939','199268','207526','207791','209874','210350','216983','219655','221577','225998','231823','233786','139210','139560','140971','148938','153385','156024','156566','157189','161540','162805','165776','181190','183554','184555','185691','187767','192580','196291','200692','203271','205426','209161','212361','212521','214551','220751','221103','222785','226178','234948','236366','238464','140303','155940','171027','184033','193357','206646','228561','240057','158140','159829','168276','181627','181985','194704','199802','200515','214462','220549','224670','231114','231559','238379','239180','139056','146495','160004','163839','170485','174902','176024','181799','188941','190575','192751','195570','212682','215390','222246','227246','232402','233696','238260','238366','138674','140217','149213','151733','155395','156878','157846','182991','197481','200860','204224','212394','215129','151466','157857','205201','208419','222958','224064','238013','142841','145861','145877','146423','165161','166962','171677','197554','199848','218849','219161','221310','234670','235539','239758','136089','138309','139280','139552','139972','140112','141291','145092','146832','147765','148030','149426','151459','151615','153585','154644','155425','156031','162031','158373','161939','163262','164664','168617','169885','169922','171070','173586','177972','178711','179427','179543','181848','183383','186074','186323','186484','186645','188930','189510','194658','197850','198151','204452','208462','210041','210801','211161','213948','214599','217006','220057','222119','229206','229762','236497','237377','240264','139906','142689','144492','161710','171251','173347','182732','199171','199748','218496','157559','161139','162145','175894','177668','179093','191030','211557','217141','218850','140479','152927','154431','154464','159986','179970','179999','184576','180201','187575','189920','190567','192647','207120','208849','212153','214562','218163','229721','229883','230166','233318','235390','135669','136042','146188','146794','150655','155019','159866','160735','164404','165424','172541','186414','176530','178186','181487','185242','190676','193814','196736','206032','212641','224220','224416','225635','233901','234701','237931','138231','141323','144648','145555','150780','150899','152839','156034','156206','157204','163155','164382','164577','166037','167180','171781','172656','175940','176083','176527','177893','179370','179380','180506','180928','181312','186261','186821','188752','188829','192028','192253','195430','196757','197324','204858','202564','203048','209777','209943','211983','215123','215882','217903','219176','227481','232103','234356','239047','144314','152718','161890','173232','184010','185603','189087','192262','195632','202699','223098','223836','224922','229421','140000','140062','168535','175315','179702','193716','211405','226429','212193','229689','156794','159799','163819','179634','181429','190947','205996','211049','224660','134586','140179','140897','148743','148792','153916','155447','161638','161681','163049','163218','186378','169820','177857','178398','182872','183800','188456','191281','191863','194747','199020','201060','205442','210315','214715','217037','218199','228236','229366','230278','230745','238378','238645','141358','141807','146429','151549','163349','159431','163012','176825','178193','189427','189930','191574','194472','196651','199478','205863','225950','231182','146349','161436','187104','191021','191734','194086','197836','203209','230430','136919','147914','150225','151174','151776','166433','170224','177521','185308','192052','200711','206227','210308','222863','222913','231145','236127','137197','140158','146957','148680','158508','167413','181146','188059','195832','215406','219282','221742','228771','230227','233235','137687','139905','148683','153540','154931','160185','161507','168943','175576','190299','194794','211649','213228','218327','227520','137733','143531','145229','152035','156082','162358','162560','166563','167482','174906','177785','179581','181727','184831','187591','188181','192875','197918','203955','205171','206049','211102','211511','140460','182042','185846','186059','194978','202325','207738','210823','213539','224910','143750','146664','157155','171037','185610','214994','222640','236462','135958','145554','152220','154793','155394','157781','173632','179192','190668','186750','191225','206920','218691','219325','221114','135888','137520','140523','142060','144519','145787','146424','147199','147684','154270','160406','161101','161838','163303','163875','164094','164561','166429','168479','168736','169732','172313','172383','175207','176225','178036','182775','186511','187648','188736','190841','194156','195367','195774','204083','210774','212113','214198','216378','218821','220433','232024','232440','235333','236582','239376','200511','200703','216368','216854','220985','221684','221834','221849','222135','223137','223721','224158','224504','226166','226297','226695','229251','230716','230761','234635','234895','235308','236196','237124','237960','238930','239976','240032','122105','168573','96922','144185','151931','156986','190213','217362','164013','104780','121861','167901','184630','124937','185146','193248','195079','77300','80971','86658','131929','204467','143637','203758','81361','106807','80313','131985','159184','212516','219061','143680','199109','200379','210667','213357','88336','90589','160050','187722','190416','196196','216274','108357','158067','191814','209748','218028','168409','88808','91652','107419','120394','130934','176535','186299','215284','72338','150378','155290','156516','157947','216010','219839','96387','103082','120734','122770','146527','147644','184966','107876','175298','184668','149130','150004','156304','174164','189171','84614','88533','90706','156563','179208','199464','80947','84283','85985','96257','101054','108605','122529','133615','137288','152785','169737','172060','218831','219358','83489','92916','108429','117211','119645','150610','149445','170454','184703','189645','190838','191674','214057','92414','115798','119426','128986','140277','154095','155957','160911','181632','126037','142972','305','557','784','3098','3672','4208','6537','7626','8122','9776','13779','16415','17391','17442','17741','18019','18138','20033','22734','23111','25358','26767','27364','27864','29168','30409','34851','35629','40383','37821','37934','38939','41644','42197','42305','42734','43507','43919','44444','44863','47006','47204','48052','59307','50573','53776','57248','58083','58533','62498','64663','65211','65916','66016','66723','67740','70467','73642','77256','78947','78958','79333','80104','80443','80717','81835','82425','82968','84578','87717','91015','91765','93806','96354','99101','99674','99978','103749','103853','104550','104801','105053','105736','105868','110303','110562','111378','111785','114642','117175','118705','123784','127336','127500','128766','129848','132134','132751','132950','133166','133776','131234','3671','4081','135435','12530','14875','25798','27308','30244','36571','41743','43437','44422','50607','55895','60525','66798','68600','68660','80402','82849','84693','92321','96066','107805','113252','116607','124001','130014','133034','132020','133819','1614','9787','15251','16859','18125','18253','21029','22044','24430','25821','30558','35912','39172','43686','44759','48274','48348','48952','49643','52210','55580','56230','56407','57930','57995','63830','65413','138646','71351','77608','102025','83878','84727','85039','89242','90596','91378','93895','94043','100388','101217','105518','106584','108694','111679','115046','114720','115805','118622','118763','119139','124080','128823','131551','132161','132761','132835','968','2145','2916','3901','7554','8131','8405','8875','9938','11008','11260','11633','14409','23443','27408','28907','29640','37909','38528','40120','60775','41112','42345','43161','44010','45630','46261','48335','54169','56205','57845','62892','65927','71052','72573','72609','72949','74596','74997','76347','77748','77875','78079','78374','79904','80019','80515','80904','81473','84188','102028','85108','92610','96690','98837','102417','103518','106075','106994','107133','107743','108418','109053','111513','114441','152173','120001','120466','124740','127774','129389','131553','133568','142275','128616','132155','124431','1835','4852','5970','5985','6412','6955','7065','7703','8979','9049','9917','10941','11426','13336','15743','15897','16700','17972','19474','21410','22635','23082','27277','29120','30449','31299','36733','37519','37960','38880','39273','43509','46157','46514','46973','50361','51850','53952','54531','57203','58449','62391','62627','62868','63596','138384','65272','67241','68865','69075','72535','73049','74789','75400','77048','79462','81655','86241','88606','88789','89145','89600','92602','94657','94900','95113','102086','95695','96505','100305','100408','100617','100621','100751','103105','105168','105373','105472','106890','110314','110661','111108','111294','112819','113515','117619','119304','120316','120521','120528','120659','124907','126403','129765','131946','132840','153878','5','803','2639','5453','5594','129144','8608','8891','11318','12098','12783','17960','18400','18679','20839','23247','23479','23920','25659','26382','28634','31791','33691','36559','37647','37686','38127','38824','38946','40172','43126','44441','45829','46984','47544','49109','49486','52170','128455','57399','58303','63100','63763','64448','64981','65895','128047','66289','67269','67319','69236','70023','71428','71681','74427','75660','75870','76389','77814','78152','81308','80554','127991','82858','83539','84011','88645','89138','89758','92226','94088','95964','97567','98652','100307','101113','102703','104239','105170','106108','106842','106907','109530','110458','114806','114884','114941','115031','116830','118122','120000','121285','9024','128624','129618','130084','132992','2029','2594','3371','6931','7325','8446','8837','10917','12757','13544','14020','17641','17956','19344','21647','22075','39354','24708','24967','29565','29572','30608','31214','32653','33914','34278','36147','38435','41529','44877','47239','48848','48908','51292','52433','52552','52699','52792','54130','56588','57681','58385','58941','59934','127472','60452','127483','65780','66892','67721','69590','69747','69880','70898','72508','74337','78317','79008','81699','82051','82348','83068','84196','86674','89038','90018','91299','92325','125673','93518','125382','98274','125485','99009','101785','102137','103741','104396','105700','108474','110143','110357','111635','111934','114266','114681','114932','115534','115558','115652','117848','118484','119292','119814','120456','120690','120792','120862','122837','135325','127676','130746','131123','128759','147482','410','5228','5975','6468','8136','13556','16203','20203','20467','21150','21907','22013','26278','27384','28663','30270','31941','32840','34162','34185','36119','36564','37307','39104','40441','40582','40730','42225','43182','165199','44991','45563','47205','47802','47968','48521','49230','50162','50277','50444','51280','52168','52448','52481','56748','56800','58053','59263','62004','62247','129542','67862','69687','71172','71990','72411','76910','77416','77546','77682','77727','78398','79894','80675','80810','80992','82166','83753','85062','86962','92315','92427','92523','92902','95432','95584','95785','97993','100258','100690','102284','105619','106758','107672','108087','109880','110472','111717','112523','112736','113947','113997','115209','122112','124359','14836','125933','127753','128203','132010','133802','124746','133064','702','993','6457','21267','10924','13381','13702','14265','15358','17782','23246','136398','27031','27425','28252','28150','30523','32050','32794','34635','37771','42823','43177','44655','44946','50684','51410','52005','54919','57085','57408','58220','60140','61380','63650','65512','65768','66317','66554','69854','72617','78633','79523','81468','81491','83427','91756','96136','96855','97081','100090','102016','102598','104110','105600','108651','110916','112024','112880','115349','118644','120519','120620','125661','127864','133420','133679','128793','142913','695','1246','2337','2381','5433','6404','9099','12276','12445','15932','16437','18599','18694','19546','23452','24768','24853','25034','27398','29763','30553','30873','31089','32097','33330','35456','36250','38608','39878','39971','43997','44686','46746','48757','49548','51685','53099','55437','56752','57444','60121','60700','61369','62358','62488','65092','66489','68384','70108','71437','72317','73435','73473','73739','77910','79614','79642','79938','81816','85132','86501','125627','92088','94531','96151','97450','97565','98395','98685','99514','100416','102728','103441','104698','104791','106740','110263','114814','117587','118545','121913','122957','124070','44859','124737','125596','127468','129489','131601','132011','132164','132591','133995','491','1399','2081','2862','3644','8115','8243','10811','11263','11424','11719','11796','13725','15619','16293','16539','17174','17205','18091','20814','22654','22827','24036','24600','25372','25896','26193','31569','31609','34670','35309','36605','37242','38197','39556','41210','43805','45478','46290','49485','137039','52305','53306','55623','61885','62154','66046','68178','68628','138866','72758','73840','73874','76640','76899','76986','79001','82142','82154','84763','87844','88049','90041','96272','96322','96382','97760','151361','103104','104357','107505','109315','140742','111571','113776','118599','121132','122174','122645','124115','125147','130751','130878','131980','133071','19139','7261','14110','21560','22495','26053','30648','33822','56583','60119','66404','70003','152800','6606','8501','9780','10791','18497','31565','31907','33368','34016','152742','128863','3339','4710','33487','33792','46435','133428','13178','26532','32979','15772','16282','51793','57564','6748','16936','3677','41404','5822','33857','49341','2304','19946','24390','24511','25682','27128','29635','30854','39651','40001','60083','17282','6692','16854','57771','58654','31013','66104','34221','12254','1699','205556','228564','307','55322','63500','135226','74906','25543','79455','8943','13840','63758','126538','39978','42682','103425','103524','84214','150486','160656','171007','209726','218420','219742','239709','125991','10377','28083','37582','77648','79389','99671','130006','154107','156027','161958','166132','210035','235727','218240','123749','5478','137832','35344','187863','206624','43631','72385','169785','191531','55395','81857','84341','123836','57050','128123','101599','200268','94207','113663','152212','143036','3114','36257','49550','123115','147724','230563','64794','98026','124601','153827','199381','211130'|</t>
   </si>
   <si>
@@ -2148,15 +2142,6 @@
     <t>standard_report_legacy.total_energy</t>
   </si>
   <si>
-    <t>Total Energy</t>
-  </si>
-  <si>
-    <t>total_energy_intensity</t>
-  </si>
-  <si>
-    <t>EUI</t>
-  </si>
-  <si>
     <t>URBANopt Testing</t>
   </si>
   <si>
@@ -2200,6 +2185,213 @@
   </si>
   <si>
     <t>../../weather</t>
+  </si>
+  <si>
+    <t>Total Site Energy Intensity</t>
+  </si>
+  <si>
+    <t>Site EUI</t>
+  </si>
+  <si>
+    <t>total_site_energy_intensity</t>
+  </si>
+  <si>
+    <t>Total Source Energy Intensity</t>
+  </si>
+  <si>
+    <t>Source EUI</t>
+  </si>
+  <si>
+    <t>total_source_energy_intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.total_source_energy</t>
+  </si>
+  <si>
+    <t>Total Natural Gas Intensity</t>
+  </si>
+  <si>
+    <t>NG EUI</t>
+  </si>
+  <si>
+    <t>total_natural_gas_intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.total_natural_gas</t>
+  </si>
+  <si>
+    <t>Total Electricity Intensity</t>
+  </si>
+  <si>
+    <t>Elec EUI</t>
+  </si>
+  <si>
+    <t>total_electricity_intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.total_electricity</t>
+  </si>
+  <si>
+    <t>Natural Gas Heating Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.heating_natural_gas</t>
+  </si>
+  <si>
+    <t>Cooling Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.cooling_electricity</t>
+  </si>
+  <si>
+    <t>Interior Lighting Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.interior_lighting_electricity</t>
+  </si>
+  <si>
+    <t>Exterior Lighting Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.exterior_lighting_electricity</t>
+  </si>
+  <si>
+    <t>Equipment Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.interior_equipment_electricity</t>
+  </si>
+  <si>
+    <t>Equipment Natural Gas Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.interior_equipment_natural_gas</t>
+  </si>
+  <si>
+    <t>Experior Equipment Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.exterior_equipment_electricity</t>
+  </si>
+  <si>
+    <t>Fans Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.fans_electricity</t>
+  </si>
+  <si>
+    <t>Pumps Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.pumps_electricity</t>
+  </si>
+  <si>
+    <t>Heat Rejection Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.heat_rejection_electricity</t>
+  </si>
+  <si>
+    <t>Humidification Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.humidification_electricity</t>
+  </si>
+  <si>
+    <t>Water Systems Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.water_systems_electricity</t>
+  </si>
+  <si>
+    <t>Water Systems Natural Gas Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.water_systems_natural_gas</t>
+  </si>
+  <si>
+    <t>Refrigeration Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.refrigeration_electricity</t>
+  </si>
+  <si>
+    <t>Electricity Cooling</t>
+  </si>
+  <si>
+    <t>standard_reports.electricity_cooling_ip</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>Electricity Fans</t>
+  </si>
+  <si>
+    <t>standard_reports.electricity_fans_ip</t>
+  </si>
+  <si>
+    <t>Electricity Heating</t>
+  </si>
+  <si>
+    <t>standard_reports.electricity_heating_ip</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>standard_reports.electricity_ip</t>
+  </si>
+  <si>
+    <t>Electricity Pumps</t>
+  </si>
+  <si>
+    <t>standard_reports.electricity_pumps_ip</t>
+  </si>
+  <si>
+    <t>Natural Gas Heating</t>
+  </si>
+  <si>
+    <t>standard_reports.natural_gas_heating_ip</t>
+  </si>
+  <si>
+    <t>MBtu</t>
+  </si>
+  <si>
+    <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>standard_reports.natural_gas_ip</t>
+  </si>
+  <si>
+    <t>Electric Peak Demand</t>
+  </si>
+  <si>
+    <t>report_out_peak_demand.electric_peak_demand</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>Natural Gas Peak Demand</t>
+  </si>
+  <si>
+    <t>report_out_peak_demand.natural_gas_peak_demand</t>
+  </si>
+  <si>
+    <t>jrobert1</t>
+  </si>
+  <si>
+    <t>UrbanBuildingTypeEPlus</t>
+  </si>
+  <si>
+    <t>urban_building_type_e_plus</t>
+  </si>
+  <si>
+    <t>ExportTimeSeriesDatatoCSV</t>
+  </si>
+  <si>
+    <t>164646'</t>
   </si>
 </sst>
 </file>
@@ -3875,7 +4067,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3972,9 +4164,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3983,6 +4172,10 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5788,9 +5981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
-    </sheetView>
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5838,7 +6029,7 @@
         <v>457</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>679</v>
+        <v>779</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>458</v>
@@ -5849,7 +6040,7 @@
         <v>470</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>611</v>
@@ -5860,7 +6051,7 @@
         <v>471</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>473</v>
@@ -5960,7 +6151,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>472</v>
@@ -5971,7 +6162,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>612</v>
@@ -6315,7 +6506,7 @@
         <v>28</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6341,13 +6532,13 @@
         <v>31</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>449</v>
@@ -6371,13 +6562,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
     </row>
   </sheetData>
@@ -6413,9 +6604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6469,14 +6658,14 @@
       <c r="R1" s="33"/>
       <c r="S1" s="30"/>
       <c r="T1" s="30"/>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
@@ -6597,13 +6786,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E4" s="39" t="s">
         <v>67</v>
@@ -6630,17 +6819,17 @@
       <c r="Y4" s="39"/>
       <c r="Z4" s="39"/>
     </row>
-    <row r="5" spans="1:26" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15" t="s">
@@ -6648,7 +6837,7 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -6675,10 +6864,10 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="42" t="s">
@@ -6686,34 +6875,34 @@
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="45" t="s">
+        <v>783</v>
+      </c>
+      <c r="J6" s="42" t="s">
+        <v>696</v>
+      </c>
+      <c r="K6" s="43">
+        <v>0</v>
+      </c>
+      <c r="L6" s="43">
+        <v>0</v>
+      </c>
+      <c r="M6" s="43">
+        <v>0</v>
+      </c>
+      <c r="N6" s="43">
+        <v>0</v>
+      </c>
+      <c r="O6" s="43">
+        <v>0</v>
+      </c>
+      <c r="P6" s="43" t="s">
         <v>697</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="Q6" s="43" t="s">
         <v>698</v>
       </c>
-      <c r="K6" s="43">
-        <v>0</v>
-      </c>
-      <c r="L6" s="43">
-        <v>0</v>
-      </c>
-      <c r="M6" s="43">
-        <v>0</v>
-      </c>
-      <c r="N6" s="43">
-        <v>0</v>
-      </c>
-      <c r="O6" s="43">
-        <v>0</v>
-      </c>
-      <c r="P6" s="43" t="s">
-        <v>699</v>
-      </c>
-      <c r="Q6" s="43" t="s">
-        <v>700</v>
-      </c>
       <c r="R6" s="42" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="S6" s="42"/>
       <c r="T6" s="42"/>
@@ -6725,131 +6914,131 @@
       <c r="Z6" s="42"/>
     </row>
     <row r="7" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="b">
+      <c r="A7" s="48" t="b">
         <v>1</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
+        <v>708</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>708</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>708</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="48"/>
+    </row>
+    <row r="8" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="46"/>
+      <c r="B8" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46" t="s">
+        <v>711</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>709</v>
+      </c>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46" t="s">
+        <v>714</v>
+      </c>
+      <c r="J8" s="46"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="46"/>
+      <c r="V8" s="46"/>
+      <c r="W8" s="46"/>
+      <c r="X8" s="46"/>
+      <c r="Y8" s="46"/>
+      <c r="Z8" s="46"/>
+    </row>
+    <row r="9" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="46"/>
+      <c r="B9" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46" t="s">
+        <v>712</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>710</v>
+      </c>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46" t="s">
         <v>713</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>713</v>
-      </c>
-      <c r="D7" s="49" t="s">
-        <v>713</v>
-      </c>
-      <c r="E7" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="49"/>
-      <c r="S7" s="49"/>
-      <c r="T7" s="49"/>
-      <c r="U7" s="49"/>
-      <c r="V7" s="49"/>
-      <c r="W7" s="49"/>
-      <c r="X7" s="49"/>
-      <c r="Y7" s="49"/>
-      <c r="Z7" s="49"/>
-    </row>
-    <row r="8" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47" t="s">
-        <v>716</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>714</v>
-      </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47" t="s">
-        <v>719</v>
-      </c>
-      <c r="J8" s="47"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="47"/>
-      <c r="V8" s="47"/>
-      <c r="W8" s="47"/>
-      <c r="X8" s="47"/>
-      <c r="Y8" s="47"/>
-      <c r="Z8" s="47"/>
-    </row>
-    <row r="9" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47" t="s">
-        <v>717</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>715</v>
-      </c>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47" t="s">
-        <v>718</v>
-      </c>
-      <c r="J9" s="47"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47"/>
-      <c r="V9" s="47"/>
-      <c r="W9" s="47"/>
-      <c r="X9" s="47"/>
-      <c r="Y9" s="47"/>
-      <c r="Z9" s="47"/>
-    </row>
-    <row r="10" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="46"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="46"/>
+      <c r="Y9" s="46"/>
+      <c r="Z9" s="46"/>
+    </row>
+    <row r="10" spans="1:26" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="b">
         <v>1</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E10" s="39" t="s">
         <v>67</v>
@@ -6876,61 +7065,81 @@
       <c r="Y10" s="39"/>
       <c r="Z10" s="39"/>
     </row>
-    <row r="11" spans="1:26" s="22" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-    </row>
-    <row r="12" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
+    <row r="11" spans="1:26" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>780</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>781</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>780</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="48"/>
+      <c r="W11" s="48"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="48"/>
+      <c r="Z11" s="48"/>
+    </row>
+    <row r="12" spans="1:26" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>782</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>782</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>782</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>232</v>
+      </c>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="48"/>
     </row>
     <row r="13" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
@@ -7072,7 +7281,7 @@
       <c r="Y17" s="15"/>
       <c r="Z17" s="15"/>
     </row>
-    <row r="18" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -7100,7 +7309,7 @@
       <c r="Y18" s="15"/>
       <c r="Z18" s="15"/>
     </row>
-    <row r="19" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -7128,7 +7337,7 @@
       <c r="Y19" s="15"/>
       <c r="Z19" s="15"/>
     </row>
-    <row r="20" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -7156,7 +7365,7 @@
       <c r="Y20" s="15"/>
       <c r="Z20" s="15"/>
     </row>
-    <row r="21" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -7184,7 +7393,7 @@
       <c r="Y21" s="15"/>
       <c r="Z21" s="15"/>
     </row>
-    <row r="22" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -7212,7 +7421,7 @@
       <c r="Y22" s="15"/>
       <c r="Z22" s="15"/>
     </row>
-    <row r="23" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -7240,7 +7449,7 @@
       <c r="Y23" s="15"/>
       <c r="Z23" s="15"/>
     </row>
-    <row r="24" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -7268,7 +7477,7 @@
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
     </row>
-    <row r="25" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -7296,7 +7505,7 @@
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
     </row>
-    <row r="26" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -7324,7 +7533,7 @@
       <c r="Y26" s="15"/>
       <c r="Z26" s="15"/>
     </row>
-    <row r="27" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -7352,7 +7561,7 @@
       <c r="Y27" s="15"/>
       <c r="Z27" s="15"/>
     </row>
-    <row r="28" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -7380,7 +7589,7 @@
       <c r="Y28" s="15"/>
       <c r="Z28" s="15"/>
     </row>
-    <row r="29" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -7408,7 +7617,7 @@
       <c r="Y29" s="15"/>
       <c r="Z29" s="15"/>
     </row>
-    <row r="30" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -7436,7 +7645,7 @@
       <c r="Y30" s="15"/>
       <c r="Z30" s="15"/>
     </row>
-    <row r="31" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -7464,7 +7673,7 @@
       <c r="Y31" s="15"/>
       <c r="Z31" s="15"/>
     </row>
-    <row r="32" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -7492,7 +7701,7 @@
       <c r="Y32" s="15"/>
       <c r="Z32" s="15"/>
     </row>
-    <row r="33" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -7520,7 +7729,7 @@
       <c r="Y33" s="15"/>
       <c r="Z33" s="15"/>
     </row>
-    <row r="34" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -7548,7 +7757,7 @@
       <c r="Y34" s="15"/>
       <c r="Z34" s="15"/>
     </row>
-    <row r="35" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -7576,7 +7785,7 @@
       <c r="Y35" s="15"/>
       <c r="Z35" s="15"/>
     </row>
-    <row r="36" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -7604,7 +7813,7 @@
       <c r="Y36" s="15"/>
       <c r="Z36" s="15"/>
     </row>
-    <row r="37" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -7632,7 +7841,7 @@
       <c r="Y37" s="15"/>
       <c r="Z37" s="15"/>
     </row>
-    <row r="38" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -7660,7 +7869,7 @@
       <c r="Y38" s="15"/>
       <c r="Z38" s="15"/>
     </row>
-    <row r="39" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -7688,7 +7897,7 @@
       <c r="Y39" s="15"/>
       <c r="Z39" s="15"/>
     </row>
-    <row r="40" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -7716,7 +7925,7 @@
       <c r="Y40" s="15"/>
       <c r="Z40" s="15"/>
     </row>
-    <row r="41" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -8254,7 +8463,7 @@
     <mergeCell ref="U1:Z1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -8280,8 +8489,7 @@
     <col min="4" max="4" width="35.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" style="1" customWidth="1"/>
@@ -8383,17 +8591,21 @@
       </c>
       <c r="M3" s="35"/>
     </row>
-    <row r="4" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>646</v>
-      </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+        <v>715</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>716</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>717</v>
+      </c>
       <c r="D4" s="15" t="s">
-        <v>652</v>
+        <v>699</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>647</v>
+        <v>469</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>63</v>
@@ -8412,17 +8624,21 @@
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
     </row>
-    <row r="5" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>648</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+        <v>718</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>719</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>720</v>
+      </c>
       <c r="D5" s="15" t="s">
-        <v>653</v>
+        <v>721</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>647</v>
+        <v>469</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>63</v>
@@ -8441,28 +8657,32 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>649</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15" t="s">
-        <v>654</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="F6" s="15" t="s">
+    <row r="6" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
+        <v>722</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>723</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>724</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>725</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>469</v>
+      </c>
+      <c r="F6" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="15" t="b">
+      <c r="G6" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="I6" s="15" t="b">
+      <c r="I6" s="46" t="b">
         <v>0</v>
       </c>
       <c r="J6" s="15"/>
@@ -8470,28 +8690,32 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>650</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15" t="s">
-        <v>655</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>651</v>
-      </c>
-      <c r="F7" s="15" t="s">
+    <row r="7" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="46" t="s">
+        <v>726</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>727</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>728</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>729</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>469</v>
+      </c>
+      <c r="F7" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="15" t="b">
+      <c r="G7" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="I7" s="15" t="b">
+      <c r="I7" s="46" t="b">
         <v>0</v>
       </c>
       <c r="J7" s="15"/>
@@ -8499,18 +8723,14 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>702</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>704</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>703</v>
-      </c>
+        <v>730</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>701</v>
+        <v>731</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>469</v>
@@ -8519,355 +8739,777 @@
         <v>63</v>
       </c>
       <c r="G8" s="15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="15" t="b">
         <v>1</v>
       </c>
       <c r="I8" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" s="15">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
+    <row r="9" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>732</v>
+      </c>
+      <c r="B9" s="22"/>
       <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="D9" s="15" t="s">
+        <v>733</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+    <row r="10" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>734</v>
+      </c>
+      <c r="B10" s="22"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="D10" s="15" t="s">
+        <v>735</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
+    <row r="11" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>736</v>
+      </c>
+      <c r="B11" s="22"/>
       <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="D11" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
     </row>
-    <row r="12" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+    <row r="12" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>738</v>
+      </c>
+      <c r="B12" s="22"/>
       <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="D12" s="15" t="s">
+        <v>739</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
     </row>
-    <row r="13" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
+    <row r="13" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>740</v>
+      </c>
       <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>741</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
+    <row r="14" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>742</v>
+      </c>
       <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
+      <c r="D14" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
+    <row r="15" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>744</v>
+      </c>
       <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>745</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
+    <row r="16" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>746</v>
+      </c>
       <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
+      <c r="D16" s="15" t="s">
+        <v>747</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
+    <row r="17" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>748</v>
+      </c>
       <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
+      <c r="D17" s="15" t="s">
+        <v>749</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
+    <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>750</v>
+      </c>
       <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
+      <c r="D18" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
+    <row r="19" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>752</v>
+      </c>
+      <c r="B19" s="22"/>
       <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
+      <c r="D19" s="15" t="s">
+        <v>753</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
+    <row r="20" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>754</v>
+      </c>
+      <c r="B20" s="22"/>
       <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
+      <c r="D20" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
     </row>
-    <row r="21" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
+    <row r="21" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>756</v>
+      </c>
+      <c r="B21" s="22"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
+      <c r="D21" s="15" t="s">
+        <v>757</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
     </row>
-    <row r="22" spans="1:13" s="23" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
+    <row r="22" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>646</v>
+      </c>
+      <c r="B22" s="22"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
+      <c r="D22" s="15" t="s">
+        <v>652</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>647</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
     </row>
-    <row r="23" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="B23" s="22"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
+      <c r="D23" s="15" t="s">
+        <v>653</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>647</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
     </row>
-    <row r="24" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>649</v>
+      </c>
+      <c r="B24" s="22"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
+      <c r="D24" s="15" t="s">
+        <v>654</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>647</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
     </row>
-    <row r="25" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>650</v>
+      </c>
       <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
+      <c r="D25" s="15" t="s">
+        <v>655</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>651</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
       <c r="M25" s="15"/>
     </row>
-    <row r="26" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>758</v>
+      </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
+      <c r="D26" s="15" t="s">
+        <v>759</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>760</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="15" t="b">
+        <v>0</v>
+      </c>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
     </row>
-    <row r="27" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B27" s="22"/>
-    </row>
-    <row r="28" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B28" s="22"/>
-    </row>
-    <row r="29" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B29" s="22"/>
-    </row>
-    <row r="30" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B30" s="22"/>
-    </row>
-    <row r="31" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B31" s="22"/>
-    </row>
-    <row r="32" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B32" s="22"/>
-    </row>
-    <row r="33" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>761</v>
+      </c>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15" t="s">
+        <v>762</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>760</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>763</v>
+      </c>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15" t="s">
+        <v>764</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>760</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>765</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15" t="s">
+        <v>766</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>760</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>767</v>
+      </c>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15" t="s">
+        <v>768</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>760</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>769</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15" t="s">
+        <v>770</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>771</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>772</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15" t="s">
+        <v>773</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>771</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>774</v>
+      </c>
       <c r="B33" s="22"/>
-    </row>
-    <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C33" s="15"/>
+      <c r="D33" s="15" t="s">
+        <v>775</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>776</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>777</v>
+      </c>
       <c r="B34" s="22"/>
-    </row>
-    <row r="35" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C34" s="22"/>
+      <c r="D34" s="15" t="s">
+        <v>778</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>776</v>
+      </c>
+      <c r="F34" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" s="22"/>
     </row>
-    <row r="36" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="22"/>
     </row>
-    <row r="37" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" s="22"/>
     </row>
-    <row r="38" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" s="22"/>
     </row>
-    <row r="39" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="22"/>
     </row>
-    <row r="40" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" s="22"/>
     </row>
-    <row r="41" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" s="22"/>
     </row>
-    <row r="42" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" s="22"/>
     </row>
-    <row r="43" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" s="22"/>
     </row>
-    <row r="44" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" s="22"/>
     </row>
-    <row r="45" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" s="22"/>
     </row>
-    <row r="46" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" s="22"/>
     </row>
-    <row r="47" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="22"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" s="22"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
@@ -9435,7 +10077,7 @@
       </c>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10" t="s">
         <v>21</v>
@@ -9458,7 +10100,7 @@
       </c>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10" t="s">
         <v>21</v>
@@ -9481,7 +10123,7 @@
       </c>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="b">
         <v>0</v>
       </c>
@@ -9500,7 +10142,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10" t="s">
         <v>21</v>
@@ -9523,7 +10165,7 @@
       </c>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10" t="s">
         <v>21</v>
@@ -9546,7 +10188,7 @@
       </c>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10" t="s">
         <v>21</v>
@@ -9569,7 +10211,7 @@
       </c>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10" t="s">
         <v>21</v>
@@ -9592,7 +10234,7 @@
       </c>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10" t="s">
         <v>21</v>
@@ -9615,7 +10257,7 @@
       </c>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10" t="s">
         <v>21</v>
@@ -9638,7 +10280,7 @@
       </c>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10" t="s">
         <v>21</v>
@@ -9661,7 +10303,7 @@
       </c>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="10" t="s">
         <v>21</v>
@@ -9684,7 +10326,7 @@
       </c>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="10" t="s">
         <v>21</v>
@@ -9707,7 +10349,7 @@
       </c>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="b">
         <v>0</v>
       </c>
@@ -9726,7 +10368,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10" t="s">
         <v>21</v>
@@ -9747,7 +10389,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="10" t="s">
         <v>21</v>
@@ -9770,7 +10412,7 @@
       </c>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="10" t="s">
         <v>21</v>
@@ -9793,7 +10435,7 @@
       </c>
       <c r="I34" s="10"/>
     </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="10" t="s">
         <v>21</v>
@@ -9816,7 +10458,7 @@
       </c>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10" t="s">
         <v>21</v>
@@ -9839,7 +10481,7 @@
       </c>
       <c r="I36" s="10"/>
     </row>
-    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="10" t="s">
         <v>21</v>
@@ -9862,7 +10504,7 @@
       </c>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="10" t="s">
         <v>21</v>
@@ -9885,7 +10527,7 @@
       </c>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
         <v>21</v>
@@ -9908,7 +10550,7 @@
       </c>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
         <v>21</v>
@@ -9931,7 +10573,7 @@
       </c>
       <c r="I40" s="10"/>
     </row>
-    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="b">
         <v>0</v>
       </c>
@@ -9950,7 +10592,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="10" t="s">
         <v>21</v>
@@ -9971,7 +10613,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="10" t="s">
         <v>21</v>
@@ -9994,7 +10636,7 @@
       </c>
       <c r="I43" s="10"/>
     </row>
-    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="10" t="s">
         <v>21</v>
@@ -10017,7 +10659,7 @@
       </c>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="10" t="s">
         <v>21</v>
@@ -10040,7 +10682,7 @@
       </c>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="10" t="s">
         <v>21</v>
@@ -17413,7 +18055,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>549</v>
       </c>
@@ -17447,12 +18089,12 @@
         <v>665</v>
       </c>
       <c r="AD18" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="AE18" s="22"/>
       <c r="AF18" s="22"/>
     </row>
-    <row r="19" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>550</v>
       </c>
@@ -17511,16 +18153,16 @@
         <v>589</v>
       </c>
       <c r="AD19" s="22" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="AE19" s="22" t="b">
         <v>1</v>
       </c>
       <c r="AF19" s="22" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -17570,16 +18212,16 @@
         <v>670</v>
       </c>
       <c r="AD20" s="22" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AE20" s="22" t="b">
         <v>1</v>
       </c>
       <c r="AF20" s="22" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="21" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>543</v>
       </c>
@@ -17643,7 +18285,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="23" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>551</v>
       </c>
@@ -17672,7 +18314,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="24" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>553</v>
       </c>
@@ -17704,7 +18346,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="25" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>669</v>
       </c>
@@ -17736,7 +18378,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="26" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>664</v>
       </c>
@@ -17756,7 +18398,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="27" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>665</v>
       </c>
@@ -17779,9 +18421,9 @@
         <v>574</v>
       </c>
     </row>
-    <row r="28" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>559</v>
@@ -17802,7 +18444,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="29" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="L29" s="1" t="s">
         <v>540</v>
       </c>
@@ -17810,7 +18452,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="30" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="L30" s="1" t="s">
         <v>542</v>
       </c>
@@ -17821,7 +18463,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="31" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="L31" s="22" t="s">
         <v>667</v>
       </c>
@@ -17832,7 +18474,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="32" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="L32" t="s">
         <v>672</v>
       </c>

</xml_diff>

<commit_message>
Adding ddy and stat files for use with SetResidentialEPWfile measure, updating commercial building type measure to handle more building types, and adding Ry's dencity measures.
</commit_message>
<xml_diff>
--- a/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
+++ b/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2254" uniqueCount="784">
   <si>
     <t>type</t>
   </si>
@@ -2100,9 +2100,6 @@
     <t>1.14.4</t>
   </si>
   <si>
-    <t>../weather/USA_OR_Portland.726980_TMY2.epw</t>
-  </si>
-  <si>
     <t>UrbanGeometryCreation</t>
   </si>
   <si>
@@ -2133,12 +2130,6 @@
     <t>|'142484','116245','142872','43254','1459','134032','143122','15204','155513','181948','142238','191582','185054','208359','113178','192702','236371','190013','6434','231850','128469','172662','222162','122347','158690','202694','56659','85635','3571','83186','227340','41962','217309','52660','161648','184642','3847','2373','62625','65373','58283','58911','237783','79514','110389','144568','5955','78754','96419','83574','223270','148046','191859','33879','52936','106804','221612','61663','207542','213989','49369','116055','151927','8514','100535','187338','207180','50936','11886','20763','230376','134949','151680','152016','164646','206572','178897','181797','183160','206869','187675','200594','222412','223723','233024','234608','235990','240241','203425','186746','215740','227893','230795','147716','150821','151683','155087','173389','208781','221871','236646','134575','138298','141692','146223','147538','148715','154723','155770','159371','166226','166447','185614','190700','200435','203431','209303','211686','225506','226857','231874','236181','134829','153445','188330','195998','215567','236722','240378','136118','144038','145786','156369','160789','166893','177498','184217','197688','212943','223606','224837','225080','228898','229908','234747','236146','236944','139179','140483','141333','141742','149927','150157','153100','157664','160763','164828','165203','166177','167379','169768','170121','170176','171097','172136','172760','174951','176543','188603','188635','192839','194021','194266','196939','199268','207526','207791','209874','210350','216983','219655','221577','225998','231823','233786','139210','139560','140971','148938','153385','156024','156566','157189','161540','162805','165776','181190','183554','184555','185691','187767','192580','196291','200692','203271','205426','209161','212361','212521','214551','220751','221103','222785','226178','234948','236366','238464','140303','155940','171027','184033','193357','206646','228561','240057','158140','159829','168276','181627','181985','194704','199802','200515','214462','220549','224670','231114','231559','238379','239180','139056','146495','160004','163839','170485','174902','176024','181799','188941','190575','192751','195570','212682','215390','222246','227246','232402','233696','238260','238366','138674','140217','149213','151733','155395','156878','157846','182991','197481','200860','204224','212394','215129','151466','157857','205201','208419','222958','224064','238013','142841','145861','145877','146423','165161','166962','171677','197554','199848','218849','219161','221310','234670','235539','239758','136089','138309','139280','139552','139972','140112','141291','145092','146832','147765','148030','149426','151459','151615','153585','154644','155425','156031','162031','158373','161939','163262','164664','168617','169885','169922','171070','173586','177972','178711','179427','179543','181848','183383','186074','186323','186484','186645','188930','189510','194658','197850','198151','204452','208462','210041','210801','211161','213948','214599','217006','220057','222119','229206','229762','236497','237377','240264','139906','142689','144492','161710','171251','173347','182732','199171','199748','218496','157559','161139','162145','175894','177668','179093','191030','211557','217141','218850','140479','152927','154431','154464','159986','179970','179999','184576','180201','187575','189920','190567','192647','207120','208849','212153','214562','218163','229721','229883','230166','233318','235390','135669','136042','146188','146794','150655','155019','159866','160735','164404','165424','172541','186414','176530','178186','181487','185242','190676','193814','196736','206032','212641','224220','224416','225635','233901','234701','237931','138231','141323','144648','145555','150780','150899','152839','156034','156206','157204','163155','164382','164577','166037','167180','171781','172656','175940','176083','176527','177893','179370','179380','180506','180928','181312','186261','186821','188752','188829','192028','192253','195430','196757','197324','204858','202564','203048','209777','209943','211983','215123','215882','217903','219176','227481','232103','234356','239047','144314','152718','161890','173232','184010','185603','189087','192262','195632','202699','223098','223836','224922','229421','140000','140062','168535','175315','179702','193716','211405','226429','212193','229689','156794','159799','163819','179634','181429','190947','205996','211049','224660','134586','140179','140897','148743','148792','153916','155447','161638','161681','163049','163218','186378','169820','177857','178398','182872','183800','188456','191281','191863','194747','199020','201060','205442','210315','214715','217037','218199','228236','229366','230278','230745','238378','238645','141358','141807','146429','151549','163349','159431','163012','176825','178193','189427','189930','191574','194472','196651','199478','205863','225950','231182','146349','161436','187104','191021','191734','194086','197836','203209','230430','136919','147914','150225','151174','151776','166433','170224','177521','185308','192052','200711','206227','210308','222863','222913','231145','236127','137197','140158','146957','148680','158508','167413','181146','188059','195832','215406','219282','221742','228771','230227','233235','137687','139905','148683','153540','154931','160185','161507','168943','175576','190299','194794','211649','213228','218327','227520','137733','143531','145229','152035','156082','162358','162560','166563','167482','174906','177785','179581','181727','184831','187591','188181','192875','197918','203955','205171','206049','211102','211511','140460','182042','185846','186059','194978','202325','207738','210823','213539','224910','143750','146664','157155','171037','185610','214994','222640','236462','135958','145554','152220','154793','155394','157781','173632','179192','190668','186750','191225','206920','218691','219325','221114','135888','137520','140523','142060','144519','145787','146424','147199','147684','154270','160406','161101','161838','163303','163875','164094','164561','166429','168479','168736','169732','172313','172383','175207','176225','178036','182775','186511','187648','188736','190841','194156','195367','195774','204083','210774','212113','214198','216378','218821','220433','232024','232440','235333','236582','239376','200511','200703','216368','216854','220985','221684','221834','221849','222135','223137','223721','224158','224504','226166','226297','226695','229251','230716','230761','234635','234895','235308','236196','237124','237960','238930','239976','240032','122105','168573','96922','144185','151931','156986','190213','217362','164013','104780','121861','167901','184630','124937','185146','193248','195079','77300','80971','86658','131929','204467','143637','203758','81361','106807','80313','131985','159184','212516','219061','143680','199109','200379','210667','213357','88336','90589','160050','187722','190416','196196','216274','108357','158067','191814','209748','218028','168409','88808','91652','107419','120394','130934','176535','186299','215284','72338','150378','155290','156516','157947','216010','219839','96387','103082','120734','122770','146527','147644','184966','107876','175298','184668','149130','150004','156304','174164','189171','84614','88533','90706','156563','179208','199464','80947','84283','85985','96257','101054','108605','122529','133615','137288','152785','169737','172060','218831','219358','83489','92916','108429','117211','119645','150610','149445','170454','184703','189645','190838','191674','214057','92414','115798','119426','128986','140277','154095','155957','160911','181632','126037','142972','305','557','784','3098','3672','4208','6537','7626','8122','9776','13779','16415','17391','17442','17741','18019','18138','20033','22734','23111','25358','26767','27364','27864','29168','30409','34851','35629','40383','37821','37934','38939','41644','42197','42305','42734','43507','43919','44444','44863','47006','47204','48052','59307','50573','53776','57248','58083','58533','62498','64663','65211','65916','66016','66723','67740','70467','73642','77256','78947','78958','79333','80104','80443','80717','81835','82425','82968','84578','87717','91015','91765','93806','96354','99101','99674','99978','103749','103853','104550','104801','105053','105736','105868','110303','110562','111378','111785','114642','117175','118705','123784','127336','127500','128766','129848','132134','132751','132950','133166','133776','131234','3671','4081','135435','12530','14875','25798','27308','30244','36571','41743','43437','44422','50607','55895','60525','66798','68600','68660','80402','82849','84693','92321','96066','107805','113252','116607','124001','130014','133034','132020','133819','1614','9787','15251','16859','18125','18253','21029','22044','24430','25821','30558','35912','39172','43686','44759','48274','48348','48952','49643','52210','55580','56230','56407','57930','57995','63830','65413','138646','71351','77608','102025','83878','84727','85039','89242','90596','91378','93895','94043','100388','101217','105518','106584','108694','111679','115046','114720','115805','118622','118763','119139','124080','128823','131551','132161','132761','132835','968','2145','2916','3901','7554','8131','8405','8875','9938','11008','11260','11633','14409','23443','27408','28907','29640','37909','38528','40120','60775','41112','42345','43161','44010','45630','46261','48335','54169','56205','57845','62892','65927','71052','72573','72609','72949','74596','74997','76347','77748','77875','78079','78374','79904','80019','80515','80904','81473','84188','102028','85108','92610','96690','98837','102417','103518','106075','106994','107133','107743','108418','109053','111513','114441','152173','120001','120466','124740','127774','129389','131553','133568','142275','128616','132155','124431','1835','4852','5970','5985','6412','6955','7065','7703','8979','9049','9917','10941','11426','13336','15743','15897','16700','17972','19474','21410','22635','23082','27277','29120','30449','31299','36733','37519','37960','38880','39273','43509','46157','46514','46973','50361','51850','53952','54531','57203','58449','62391','62627','62868','63596','138384','65272','67241','68865','69075','72535','73049','74789','75400','77048','79462','81655','86241','88606','88789','89145','89600','92602','94657','94900','95113','102086','95695','96505','100305','100408','100617','100621','100751','103105','105168','105373','105472','106890','110314','110661','111108','111294','112819','113515','117619','119304','120316','120521','120528','120659','124907','126403','129765','131946','132840','153878','5','803','2639','5453','5594','129144','8608','8891','11318','12098','12783','17960','18400','18679','20839','23247','23479','23920','25659','26382','28634','31791','33691','36559','37647','37686','38127','38824','38946','40172','43126','44441','45829','46984','47544','49109','49486','52170','128455','57399','58303','63100','63763','64448','64981','65895','128047','66289','67269','67319','69236','70023','71428','71681','74427','75660','75870','76389','77814','78152','81308','80554','127991','82858','83539','84011','88645','89138','89758','92226','94088','95964','97567','98652','100307','101113','102703','104239','105170','106108','106842','106907','109530','110458','114806','114884','114941','115031','116830','118122','120000','121285','9024','128624','129618','130084','132992','2029','2594','3371','6931','7325','8446','8837','10917','12757','13544','14020','17641','17956','19344','21647','22075','39354','24708','24967','29565','29572','30608','31214','32653','33914','34278','36147','38435','41529','44877','47239','48848','48908','51292','52433','52552','52699','52792','54130','56588','57681','58385','58941','59934','127472','60452','127483','65780','66892','67721','69590','69747','69880','70898','72508','74337','78317','79008','81699','82051','82348','83068','84196','86674','89038','90018','91299','92325','125673','93518','125382','98274','125485','99009','101785','102137','103741','104396','105700','108474','110143','110357','111635','111934','114266','114681','114932','115534','115558','115652','117848','118484','119292','119814','120456','120690','120792','120862','122837','135325','127676','130746','131123','128759','147482','410','5228','5975','6468','8136','13556','16203','20203','20467','21150','21907','22013','26278','27384','28663','30270','31941','32840','34162','34185','36119','36564','37307','39104','40441','40582','40730','42225','43182','165199','44991','45563','47205','47802','47968','48521','49230','50162','50277','50444','51280','52168','52448','52481','56748','56800','58053','59263','62004','62247','129542','67862','69687','71172','71990','72411','76910','77416','77546','77682','77727','78398','79894','80675','80810','80992','82166','83753','85062','86962','92315','92427','92523','92902','95432','95584','95785','97993','100258','100690','102284','105619','106758','107672','108087','109880','110472','111717','112523','112736','113947','113997','115209','122112','124359','14836','125933','127753','128203','132010','133802','124746','133064','702','993','6457','21267','10924','13381','13702','14265','15358','17782','23246','136398','27031','27425','28252','28150','30523','32050','32794','34635','37771','42823','43177','44655','44946','50684','51410','52005','54919','57085','57408','58220','60140','61380','63650','65512','65768','66317','66554','69854','72617','78633','79523','81468','81491','83427','91756','96136','96855','97081','100090','102016','102598','104110','105600','108651','110916','112024','112880','115349','118644','120519','120620','125661','127864','133420','133679','128793','142913','695','1246','2337','2381','5433','6404','9099','12276','12445','15932','16437','18599','18694','19546','23452','24768','24853','25034','27398','29763','30553','30873','31089','32097','33330','35456','36250','38608','39878','39971','43997','44686','46746','48757','49548','51685','53099','55437','56752','57444','60121','60700','61369','62358','62488','65092','66489','68384','70108','71437','72317','73435','73473','73739','77910','79614','79642','79938','81816','85132','86501','125627','92088','94531','96151','97450','97565','98395','98685','99514','100416','102728','103441','104698','104791','106740','110263','114814','117587','118545','121913','122957','124070','44859','124737','125596','127468','129489','131601','132011','132164','132591','133995','491','1399','2081','2862','3644','8115','8243','10811','11263','11424','11719','11796','13725','15619','16293','16539','17174','17205','18091','20814','22654','22827','24036','24600','25372','25896','26193','31569','31609','34670','35309','36605','37242','38197','39556','41210','43805','45478','46290','49485','137039','52305','53306','55623','61885','62154','66046','68178','68628','138866','72758','73840','73874','76640','76899','76986','79001','82142','82154','84763','87844','88049','90041','96272','96322','96382','97760','151361','103104','104357','107505','109315','140742','111571','113776','118599','121132','122174','122645','124115','125147','130751','130878','131980','133071','19139','7261','14110','21560','22495','26053','30648','33822','56583','60119','66404','70003','152800','6606','8501','9780','10791','18497','31565','31907','33368','34016','152742','128863','3339','4710','33487','33792','46435','133428','13178','26532','32979','15772','16282','51793','57564','6748','16936','3677','41404','5822','33857','49341','2304','19946','24390','24511','25682','27128','29635','30854','39651','40001','60083','17282','6692','16854','57771','58654','31013','66104','34221','12254','1699','205556','228564','307','55322','63500','135226','74906','25543','79455','8943','13840','63758','126538','39978','42682','103425','103524','84214','150486','160656','171007','209726','218420','219742','239709','125991','10377','28083','37582','77648','79389','99671','130006','154107','156027','161958','166132','210035','235727','218240','123749','5478','137832','35344','187863','206624','43631','72385','169785','191531','55395','81857','84341','123836','57050','128123','101599','200268','94207','113663','152212','143036','3114','36257','49550','123115','147724','230563','64794','98026','124601','153827','199381','211130'|</t>
   </si>
   <si>
-    <t>['142484','116245','142872','43254','1459','134032','143122','15204','155513','181948','142238','191582','185054','208359','113178','192702','236371','190013','6434','231850','128469','172662','222162','122347','158690','202694','56659','85635','3571','83186','227340','41962','217309','52660','161648','184642','3847','2373','62625','65373','58283','58911','237783','79514','110389','144568','5955','78754','96419','83574','223270','148046','191859','33879','52936','106804','221612','61663','207542','213989','49369','116055','151927','8514','100535','187338','207180','50936','11886','20763','230376','134949','151680','152016','164646','206572','178897','181797','183160','206869','187675','200594','222412','223723','233024','234608','235990','240241','203425','186746','215740','227893','230795','147716','150821','151683','155087','173389','208781','221871','236646','134575','138298','141692','146223','147538','148715','154723','155770','159371','166226','166447','185614','190700','200435','203431','209303','211686','225506','226857','231874','236181','134829','153445','188330','195998','215567','236722','240378','136118','144038','145786','156369','160789','166893','177498','184217','197688','212943','223606','224837','225080','228898','229908','234747','236146','236944','139179','140483','141333','141742','149927','150157','153100','157664','160763','164828','165203','166177','167379','169768','170121','170176','171097','172136','172760','174951','176543','188603','188635','192839','194021','194266','196939','199268','207526','207791','209874','210350','216983','219655','221577','225998','231823','233786','139210','139560','140971','148938','153385','156024','156566','157189','161540','162805','165776','181190','183554','184555','185691','187767','192580','196291','200692','203271','205426','209161','212361','212521','214551','220751','221103','222785','226178','234948','236366','238464','140303','155940','171027','184033','193357','206646','228561','240057','158140','159829','168276','181627','181985','194704','199802','200515','214462','220549','224670','231114','231559','238379','239180','139056','146495','160004','163839','170485','174902','176024','181799','188941','190575','192751','195570','212682','215390','222246','227246','232402','233696','238260','238366','138674','140217','149213','151733','155395','156878','157846','182991','197481','200860','204224','212394','215129','151466','157857','205201','208419','222958','224064','238013','142841','145861','145877','146423','165161','166962','171677','197554','199848','218849','219161','221310','234670','235539','239758','136089','138309','139280','139552','139972','140112','141291','145092','146832','147765','148030','149426','151459','151615','153585','154644','155425','156031','162031','158373','161939','163262','164664','168617','169885','169922','171070','173586','177972','178711','179427','179543','181848','183383','186074','186323','186484','186645','188930','189510','194658','197850','198151','204452','208462','210041','210801','211161','213948','214599','217006','220057','222119','229206','229762','236497','237377','240264','139906','142689','144492','161710','171251','173347','182732','199171','199748','218496','157559','161139','162145','175894','177668','179093','191030','211557','217141','218850','140479','152927','154431','154464','159986','179970','179999','184576','180201','187575','189920','190567','192647','207120','208849','212153','214562','218163','229721','229883','230166','233318','235390','135669','136042','146188','146794','150655','155019','159866','160735','164404','165424','172541','186414','176530','178186','181487','185242','190676','193814','196736','206032','212641','224220','224416','225635','233901','234701','237931','138231','141323','144648','145555','150780','150899','152839','156034','156206','157204','163155','164382','164577','166037','167180','171781','172656','175940','176083','176527','177893','179370','179380','180506','180928','181312','186261','186821','188752','188829','192028','192253','195430','196757','197324','204858','202564','203048','209777','209943','211983','215123','215882','217903','219176','227481','232103','234356','239047','144314','152718','161890','173232','184010','185603','189087','192262','195632','202699','223098','223836','224922','229421','140000','140062','168535','175315','179702','193716','211405','226429','212193','229689','156794','159799','163819','179634','181429','190947','205996','211049','224660','134586','140179','140897','148743','148792','153916','155447','161638','161681','163049','163218','186378','169820','177857','178398','182872','183800','188456','191281','191863','194747','199020','201060','205442','210315','214715','217037','218199','228236','229366','230278','230745','238378','238645','141358','141807','146429','151549','163349','159431','163012','176825','178193','189427','189930','191574','194472','196651','199478','205863','225950','231182','146349','161436','187104','191021','191734','194086','197836','203209','230430','136919','147914','150225','151174','151776','166433','170224','177521','185308','192052','200711','206227','210308','222863','222913','231145','236127','137197','140158','146957','148680','158508','167413','181146','188059','195832','215406','219282','221742','228771','230227','233235','137687','139905','148683','153540','154931','160185','161507','168943','175576','190299','194794','211649','213228','218327','227520','137733','143531','145229','152035','156082','162358','162560','166563','167482','174906','177785','179581','181727','184831','187591','188181','192875','197918','203955','205171','206049','211102','211511','140460','182042','185846','186059','194978','202325','207738','210823','213539','224910','143750','146664','157155','171037','185610','214994','222640','236462','135958','145554','152220','154793','155394','157781','173632','179192','190668','186750','191225','206920','218691','219325','221114','135888','137520','140523','142060','144519','145787','146424','147199','147684','154270','160406','161101','161838','163303','163875','164094','164561','166429','168479','168736','169732','172313','172383','175207','176225','178036','182775','186511','187648','188736','190841','194156','195367','195774','204083','210774','212113','214198','216378','218821','220433','232024','232440','235333','236582','239376','200511','200703','216368','216854','220985','221684','221834','221849','222135','223137','223721','224158','224504','226166','226297','226695','229251','230716','230761','234635','234895','235308','236196','237124','237960','238930','239976','240032','122105','168573','96922','144185','151931','156986','190213','217362','164013','104780','121861','167901','184630','124937','185146','193248','195079','77300','80971','86658','131929','204467','143637','203758','81361','106807','80313','131985','159184','212516','219061','143680','199109','200379','210667','213357','88336','90589','160050','187722','190416','196196','216274','108357','158067','191814','209748','218028','168409','88808','91652','107419','120394','130934','176535','186299','215284','72338','150378','155290','156516','157947','216010','219839','96387','103082','120734','122770','146527','147644','184966','107876','175298','184668','149130','150004','156304','174164','189171','84614','88533','90706','156563','179208','199464','80947','84283','85985','96257','101054','108605','122529','133615','137288','152785','169737','172060','218831','219358','83489','92916','108429','117211','119645','150610','149445','170454','184703','189645','190838','191674','214057','92414','115798','119426','128986','140277','154095','155957','160911','181632','126037','142972','305','557','784','3098','3672','4208','6537','7626','8122','9776','13779','16415','17391','17442','17741','18019','18138','20033','22734','23111','25358','26767','27364','27864','29168','30409','34851','35629','40383','37821','37934','38939','41644','42197','42305','42734','43507','43919','44444','44863','47006','47204','48052','59307','50573','53776','57248','58083','58533','62498','64663','65211','65916','66016','66723','67740','70467','73642','77256','78947','78958','79333','80104','80443','80717','81835','82425','82968','84578','87717','91015','91765','93806','96354','99101','99674','99978','103749','103853','104550','104801','105053','105736','105868','110303','110562','111378','111785','114642','117175','118705','123784','127336','127500','128766','129848','132134','132751','132950','133166','133776','131234','3671','4081','135435','12530','14875','25798','27308','30244','36571','41743','43437','44422','50607','55895','60525','66798','68600','68660','80402','82849','84693','92321','96066','107805','113252','116607','124001','130014','133034','132020','133819','1614','9787','15251','16859','18125','18253','21029','22044','24430','25821','30558','35912','39172','43686','44759','48274','48348','48952','49643','52210','55580','56230','56407','57930','57995','63830','65413','138646','71351','77608','102025','83878','84727','85039','89242','90596','91378','93895','94043','100388','101217','105518','106584','108694','111679','115046','114720','115805','118622','118763','119139','124080','128823','131551','132161','132761','132835','968','2145','2916','3901','7554','8131','8405','8875','9938','11008','11260','11633','14409','23443','27408','28907','29640','37909','38528','40120','60775','41112','42345','43161','44010','45630','46261','48335','54169','56205','57845','62892','65927','71052','72573','72609','72949','74596','74997','76347','77748','77875','78079','78374','79904','80019','80515','80904','81473','84188','102028','85108','92610','96690','98837','102417','103518','106075','106994','107133','107743','108418','109053','111513','114441','152173','120001','120466','124740','127774','129389','131553','133568','142275','128616','132155','124431','1835','4852','5970','5985','6412','6955','7065','7703','8979','9049','9917','10941','11426','13336','15743','15897','16700','17972','19474','21410','22635','23082','27277','29120','30449','31299','36733','37519','37960','38880','39273','43509','46157','46514','46973','50361','51850','53952','54531','57203','58449','62391','62627','62868','63596','138384','65272','67241','68865','69075','72535','73049','74789','75400','77048','79462','81655','86241','88606','88789','89145','89600','92602','94657','94900','95113','102086','95695','96505','100305','100408','100617','100621','100751','103105','105168','105373','105472','106890','110314','110661','111108','111294','112819','113515','117619','119304','120316','120521','120528','120659','124907','126403','129765','131946','132840','153878','5','803','2639','5453','5594','129144','8608','8891','11318','12098','12783','17960','18400','18679','20839','23247','23479','23920','25659','26382','28634','31791','33691','36559','37647','37686','38127','38824','38946','40172','43126','44441','45829','46984','47544','49109','49486','52170','128455','57399','58303','63100','63763','64448','64981','65895','128047','66289','67269','67319','69236','70023','71428','71681','74427','75660','75870','76389','77814','78152','81308','80554','127991','82858','83539','84011','88645','89138','89758','92226','94088','95964','97567','98652','100307','101113','102703','104239','105170','106108','106842','106907','109530','110458','114806','114884','114941','115031','116830','118122','120000','121285','9024','128624','129618','130084','132992','2029','2594','3371','6931','7325','8446','8837','10917','12757','13544','14020','17641','17956','19344','21647','22075','39354','24708','24967','29565','29572','30608','31214','32653','33914','34278','36147','38435','41529','44877','47239','48848','48908','51292','52433','52552','52699','52792','54130','56588','57681','58385','58941','59934','127472','60452','127483','65780','66892','67721','69590','69747','69880','70898','72508','74337','78317','79008','81699','82051','82348','83068','84196','86674','89038','90018','91299','92325','125673','93518','125382','98274','125485','99009','101785','102137','103741','104396','105700','108474','110143','110357','111635','111934','114266','114681','114932','115534','115558','115652','117848','118484','119292','119814','120456','120690','120792','120862','122837','135325','127676','130746','131123','128759','147482','410','5228','5975','6468','8136','13556','16203','20203','20467','21150','21907','22013','26278','27384','28663','30270','31941','32840','34162','34185','36119','36564','37307','39104','40441','40582','40730','42225','43182','165199','44991','45563','47205','47802','47968','48521','49230','50162','50277','50444','51280','52168','52448','52481','56748','56800','58053','59263','62004','62247','129542','67862','69687','71172','71990','72411','76910','77416','77546','77682','77727','78398','79894','80675','80810','80992','82166','83753','85062','86962','92315','92427','92523','92902','95432','95584','95785','97993','100258','100690','102284','105619','106758','107672','108087','109880','110472','111717','112523','112736','113947','113997','115209','122112','124359','14836','125933','127753','128203','132010','133802','124746','133064','702','993','6457','21267','10924','13381','13702','14265','15358','17782','23246','136398','27031','27425','28252','28150','30523','32050','32794','34635','37771','42823','43177','44655','44946','50684','51410','52005','54919','57085','57408','58220','60140','61380','63650','65512','65768','66317','66554','69854','72617','78633','79523','81468','81491','83427','91756','96136','96855','97081','100090','102016','102598','104110','105600','108651','110916','112024','112880','115349','118644','120519','120620','125661','127864','133420','133679','128793','142913','695','1246','2337','2381','5433','6404','9099','12276','12445','15932','16437','18599','18694','19546','23452','24768','24853','25034','27398','29763','30553','30873','31089','32097','33330','35456','36250','38608','39878','39971','43997','44686','46746','48757','49548','51685','53099','55437','56752','57444','60121','60700','61369','62358','62488','65092','66489','68384','70108','71437','72317','73435','73473','73739','77910','79614','79642','79938','81816','85132','86501','125627','92088','94531','96151','97450','97565','98395','98685','99514','100416','102728','103441','104698','104791','106740','110263','114814','117587','118545','121913','122957','124070','44859','124737','125596','127468','129489','131601','132011','132164','132591','133995','491','1399','2081','2862','3644','8115','8243','10811','11263','11424','11719','11796','13725','15619','16293','16539','17174','17205','18091','20814','22654','22827','24036','24600','25372','25896','26193','31569','31609','34670','35309','36605','37242','38197','39556','41210','43805','45478','46290','49485','137039','52305','53306','55623','61885','62154','66046','68178','68628','138866','72758','73840','73874','76640','76899','76986','79001','82142','82154','84763','87844','88049','90041','96272','96322','96382','97760','151361','103104','104357','107505','109315','140742','111571','113776','118599','121132','122174','122645','124115','125147','130751','130878','131980','133071','19139','7261','14110','21560','22495','26053','30648','33822','56583','60119','66404','70003','152800','6606','8501','9780','10791','18497','31565','31907','33368','34016','152742','128863','3339','4710','33487','33792','46435','133428','13178','26532','32979','15772','16282','51793','57564','6748','16936','3677','41404','5822','33857','49341','2304','19946','24390','24511','25682','27128','29635','30854','39651','40001','60083','17282','6692','16854','57771','58654','31013','66104','34221','12254','1699','205556','228564','307','55322','63500','135226','74906','25543','79455','8943','13840','63758','126538','39978','42682','103425','103524','84214','150486','160656','171007','209726','218420','219742','239709','125991','10377','28083','37582','77648','79389','99671','130006','154107','156027','161958','166132','210035','235727','218240','123749','5478','137832','35344','187863','206624','43631','72385','169785','191531','55395','81857','84341','123836','57050','128123','101599','200268','94207','113663','152212','143036','3114','36257','49550','123115','147724','230563','64794','98026','124601','153827','199381','211130']</t>
-  </si>
-  <si>
-    <t>[0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056,0.00052056]</t>
-  </si>
-  <si>
     <t>standard_report_legacy.total_energy</t>
   </si>
   <si>
@@ -2181,9 +2172,6 @@
     <t>Weather File Name</t>
   </si>
   <si>
-    <t>USA_OR_Portland.726980_TMY2.epw</t>
-  </si>
-  <si>
     <t>../../weather</t>
   </si>
   <si>
@@ -2391,7 +2379,19 @@
     <t>ExportTimeSeriesDatatoCSV</t>
   </si>
   <si>
-    <t>164646'</t>
+    <t>USA_CO_Denver.Intl.AP.725650_TMY3.epw</t>
+  </si>
+  <si>
+    <t>../weather/USA_CO_Denver.Intl.AP.725650_TMY3.epw</t>
+  </si>
+  <si>
+    <t>../weather/USA_CO_Denver.Intl.AP.725650_TMY3.ddy</t>
+  </si>
+  <si>
+    <t>178897'</t>
+  </si>
+  <si>
+    <t>['178897','222412','236646','231874','127676']</t>
   </si>
 </sst>
 </file>
@@ -4172,10 +4172,10 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5979,14 +5979,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" style="1" customWidth="1"/>
     <col min="4" max="5" width="33.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="61.7109375" style="1" customWidth="1"/>
@@ -6029,7 +6029,7 @@
         <v>457</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>458</v>
@@ -6151,7 +6151,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>472</v>
@@ -6162,7 +6162,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>612</v>
@@ -6501,74 +6501,84 @@
       <c r="E39" s="6"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>781</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="44" t="s">
+      <c r="B43" s="44" t="s">
         <v>454</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>613</v>
       </c>
-      <c r="E42" s="6"/>
-      <c r="F42" s="8" t="s">
+      <c r="E43" s="6"/>
+      <c r="F43" s="8" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="17" t="s">
-        <v>706</v>
-      </c>
-      <c r="C43" s="14" t="s">
+      <c r="B44" s="17" t="s">
+        <v>703</v>
+      </c>
+      <c r="C44" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D44" s="23" t="s">
+        <v>698</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="8" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B47" s="18" t="s">
         <v>701</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>614</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="8" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="B46" s="18" t="s">
+      <c r="C47" s="1" t="s">
         <v>704</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>707</v>
       </c>
     </row>
   </sheetData>
@@ -6658,14 +6668,14 @@
       <c r="R1" s="33"/>
       <c r="S1" s="30"/>
       <c r="T1" s="30"/>
-      <c r="U1" s="50" t="s">
+      <c r="U1" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
@@ -6786,13 +6796,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E4" s="39" t="s">
         <v>67</v>
@@ -6826,10 +6836,10 @@
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15" t="s">
@@ -6837,7 +6847,7 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -6864,10 +6874,10 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="42" t="s">
@@ -6875,34 +6885,32 @@
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="45" t="s">
+        <v>782</v>
+      </c>
+      <c r="J6" s="42" t="s">
+        <v>695</v>
+      </c>
+      <c r="K6" s="43">
+        <v>0</v>
+      </c>
+      <c r="L6" s="43">
+        <v>0</v>
+      </c>
+      <c r="M6" s="43">
+        <v>0</v>
+      </c>
+      <c r="N6" s="43">
+        <v>0</v>
+      </c>
+      <c r="O6" s="43">
+        <v>0</v>
+      </c>
+      <c r="P6" s="43" t="s">
         <v>783</v>
       </c>
-      <c r="J6" s="42" t="s">
-        <v>696</v>
-      </c>
-      <c r="K6" s="43">
-        <v>0</v>
-      </c>
-      <c r="L6" s="43">
-        <v>0</v>
-      </c>
-      <c r="M6" s="43">
-        <v>0</v>
-      </c>
-      <c r="N6" s="43">
-        <v>0</v>
-      </c>
-      <c r="O6" s="43">
-        <v>0</v>
-      </c>
-      <c r="P6" s="43" t="s">
-        <v>697</v>
-      </c>
-      <c r="Q6" s="43" t="s">
-        <v>698</v>
-      </c>
+      <c r="Q6" s="43"/>
       <c r="R6" s="42" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="S6" s="42"/>
       <c r="T6" s="42"/>
@@ -6918,13 +6926,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="E7" s="48" t="s">
         <v>67</v>
@@ -6958,10 +6966,10 @@
       </c>
       <c r="C8" s="46"/>
       <c r="D8" s="46" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="F8" s="46"/>
       <c r="G8" s="46" t="s">
@@ -6969,7 +6977,7 @@
       </c>
       <c r="H8" s="46"/>
       <c r="I8" s="46" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="J8" s="46"/>
       <c r="K8" s="47"/>
@@ -6996,10 +7004,10 @@
       </c>
       <c r="C9" s="46"/>
       <c r="D9" s="46" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="F9" s="46"/>
       <c r="G9" s="46" t="s">
@@ -7007,7 +7015,7 @@
       </c>
       <c r="H9" s="46"/>
       <c r="I9" s="46" t="s">
-        <v>713</v>
+        <v>779</v>
       </c>
       <c r="J9" s="46"/>
       <c r="K9" s="47"/>
@@ -7032,13 +7040,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E10" s="39" t="s">
         <v>67</v>
@@ -7066,28 +7074,28 @@
       <c r="Z10" s="39"/>
     </row>
     <row r="11" spans="1:26" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="51" t="b">
+      <c r="A11" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="B11" s="51" t="s">
-        <v>780</v>
-      </c>
-      <c r="C11" s="51" t="s">
-        <v>781</v>
-      </c>
-      <c r="D11" s="51" t="s">
-        <v>780</v>
-      </c>
-      <c r="E11" s="51" t="s">
+      <c r="B11" s="50" t="s">
+        <v>776</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>777</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>776</v>
+      </c>
+      <c r="E11" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
       <c r="M11" s="48"/>
       <c r="N11" s="48"/>
       <c r="O11" s="48"/>
@@ -7104,28 +7112,28 @@
       <c r="Z11" s="48"/>
     </row>
     <row r="12" spans="1:26" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="b">
+      <c r="A12" s="50" t="b">
         <v>1</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>782</v>
-      </c>
-      <c r="E12" s="51" t="s">
+        <v>778</v>
+      </c>
+      <c r="E12" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
       <c r="M12" s="48"/>
       <c r="N12" s="48"/>
       <c r="O12" s="48"/>
@@ -8593,16 +8601,16 @@
     </row>
     <row r="4" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>469</v>
@@ -8626,16 +8634,16 @@
     </row>
     <row r="5" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>469</v>
@@ -8659,16 +8667,16 @@
     </row>
     <row r="6" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="E6" s="46" t="s">
         <v>469</v>
@@ -8692,16 +8700,16 @@
     </row>
     <row r="7" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="E7" s="46" t="s">
         <v>469</v>
@@ -8725,12 +8733,12 @@
     </row>
     <row r="8" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>469</v>
@@ -8754,12 +8762,12 @@
     </row>
     <row r="9" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>469</v>
@@ -8783,12 +8791,12 @@
     </row>
     <row r="10" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>469</v>
@@ -8812,12 +8820,12 @@
     </row>
     <row r="11" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>469</v>
@@ -8841,12 +8849,12 @@
     </row>
     <row r="12" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="B12" s="22"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>469</v>
@@ -8870,11 +8878,11 @@
     </row>
     <row r="13" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>469</v>
@@ -8898,11 +8906,11 @@
     </row>
     <row r="14" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>469</v>
@@ -8926,11 +8934,11 @@
     </row>
     <row r="15" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>469</v>
@@ -8954,11 +8962,11 @@
     </row>
     <row r="16" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>469</v>
@@ -8982,11 +8990,11 @@
     </row>
     <row r="17" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>469</v>
@@ -9010,11 +9018,11 @@
     </row>
     <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>469</v>
@@ -9038,12 +9046,12 @@
     </row>
     <row r="19" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B19" s="22"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>469</v>
@@ -9067,12 +9075,12 @@
     </row>
     <row r="20" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>469</v>
@@ -9096,12 +9104,12 @@
     </row>
     <row r="21" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="B21" s="22"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>469</v>
@@ -9243,15 +9251,15 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>63</v>
@@ -9272,15 +9280,15 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>63</v>
@@ -9297,15 +9305,15 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="F28" s="15" t="s">
         <v>63</v>
@@ -9322,15 +9330,15 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>63</v>
@@ -9347,15 +9355,15 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>63</v>
@@ -9372,15 +9380,15 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>63</v>
@@ -9397,15 +9405,15 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="F32" s="15" t="s">
         <v>63</v>
@@ -9422,15 +9430,15 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="B33" s="22"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>63</v>
@@ -9447,15 +9455,15 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="15" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="F34" s="46" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Metadata and timeseries reports successfully make their way to dencity.
</commit_message>
<xml_diff>
--- a/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
+++ b/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="180" windowWidth="23250" windowHeight="12990" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="240" windowWidth="15360" windowHeight="7755" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -31,16 +31,11 @@
     <definedName name="Workflow">Lookups!$E$14:$E$15</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2254" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="814">
   <si>
     <t>type</t>
   </si>
@@ -2133,9 +2128,6 @@
     <t>standard_report_legacy.total_energy</t>
   </si>
   <si>
-    <t>URBANopt Testing</t>
-  </si>
-  <si>
     <t>../seeds/EmptySeedModel.osm</t>
   </si>
   <si>
@@ -2352,21 +2344,6 @@
     <t>standard_reports.natural_gas_ip</t>
   </si>
   <si>
-    <t>Electric Peak Demand</t>
-  </si>
-  <si>
-    <t>report_out_peak_demand.electric_peak_demand</t>
-  </si>
-  <si>
-    <t>kW</t>
-  </si>
-  <si>
-    <t>Natural Gas Peak Demand</t>
-  </si>
-  <si>
-    <t>report_out_peak_demand.natural_gas_peak_demand</t>
-  </si>
-  <si>
     <t>jrobert1</t>
   </si>
   <si>
@@ -2376,9 +2353,6 @@
     <t>urban_building_type_e_plus</t>
   </si>
   <si>
-    <t>ExportTimeSeriesDatatoCSV</t>
-  </si>
-  <si>
     <t>USA_CO_Denver.Intl.AP.725650_TMY3.epw</t>
   </si>
   <si>
@@ -2392,6 +2366,117 @@
   </si>
   <si>
     <t>['178897','222412','236646','231874','127676']</t>
+  </si>
+  <si>
+    <t>URBANopt Testing 1</t>
+  </si>
+  <si>
+    <t>Add Dencity Meters</t>
+  </si>
+  <si>
+    <t>AddDencityMeters</t>
+  </si>
+  <si>
+    <t>DEnCity Reports</t>
+  </si>
+  <si>
+    <t>DencityReports</t>
+  </si>
+  <si>
+    <t>Output Format</t>
+  </si>
+  <si>
+    <t>output_format</t>
+  </si>
+  <si>
+    <t>CSV</t>
+  </si>
+  <si>
+    <t>DEnCity Datapoint Upload</t>
+  </si>
+  <si>
+    <t>dencity_datapoint_upload</t>
+  </si>
+  <si>
+    <t>DencityDatapointUpload</t>
+  </si>
+  <si>
+    <t>URL of the DEnCity Server</t>
+  </si>
+  <si>
+    <t>hostname</t>
+  </si>
+  <si>
+    <t>http://insight4.hpc.nrel.gov:8080/</t>
+  </si>
+  <si>
+    <t>User ID for DEnCity Server</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>test@nrel.gov</t>
+  </si>
+  <si>
+    <t>Authentication code for User ID on DEnCity server</t>
+  </si>
+  <si>
+    <t>auth_code</t>
+  </si>
+  <si>
+    <t>testing123</t>
+  </si>
+  <si>
+    <t>DEnCity File Upload</t>
+  </si>
+  <si>
+    <t>dencity_file_upload</t>
+  </si>
+  <si>
+    <t>DencityFileUpload</t>
+  </si>
+  <si>
+    <t>../DencityReports/report_metadata.csv</t>
+  </si>
+  <si>
+    <t>Total Life Cycle Cost</t>
+  </si>
+  <si>
+    <t>standard_report.total_life_cycle_cost</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>../DencityReports/report_timeseries.csv</t>
+  </si>
+  <si>
+    <t>Metadata File Path</t>
+  </si>
+  <si>
+    <t>Timeseries File Path</t>
+  </si>
+  <si>
+    <t>file_path_metadata</t>
+  </si>
+  <si>
+    <t>file_path_timeseries</t>
+  </si>
+  <si>
+    <t>urban_building_district_system</t>
+  </si>
+  <si>
+    <t>Type of district system to model</t>
+  </si>
+  <si>
+    <t>district_system_type</t>
+  </si>
+  <si>
+    <t>Conventional</t>
+  </si>
+  <si>
+    <t>UrbanBuildingDistrictSystem</t>
   </si>
 </sst>
 </file>
@@ -4067,7 +4152,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4173,9 +4258,22 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5981,7 +6079,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6029,7 +6129,7 @@
         <v>457</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>458</v>
@@ -6151,7 +6251,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>697</v>
+        <v>777</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>472</v>
@@ -6162,7 +6262,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>612</v>
@@ -6506,7 +6606,7 @@
         <v>28</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>780</v>
+        <v>773</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6514,7 +6614,7 @@
         <v>28</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>781</v>
+        <v>774</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -6542,13 +6642,13 @@
         <v>31</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>449</v>
@@ -6572,13 +6672,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B47" s="18" t="s">
         <v>700</v>
       </c>
-      <c r="B47" s="18" t="s">
-        <v>701</v>
-      </c>
       <c r="C47" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
   </sheetData>
@@ -6612,7 +6712,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z59"/>
+  <dimension ref="A1:Z58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
@@ -6668,14 +6768,14 @@
       <c r="R1" s="33"/>
       <c r="S1" s="30"/>
       <c r="T1" s="30"/>
-      <c r="U1" s="51" t="s">
+      <c r="U1" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
@@ -6847,7 +6947,7 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -6885,7 +6985,7 @@
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="45" t="s">
-        <v>782</v>
+        <v>775</v>
       </c>
       <c r="J6" s="42" t="s">
         <v>695</v>
@@ -6906,7 +7006,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>783</v>
+        <v>776</v>
       </c>
       <c r="Q6" s="43"/>
       <c r="R6" s="42" t="s">
@@ -6926,13 +7026,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E7" s="48" t="s">
         <v>67</v>
@@ -6966,10 +7066,10 @@
       </c>
       <c r="C8" s="46"/>
       <c r="D8" s="46" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="F8" s="46"/>
       <c r="G8" s="46" t="s">
@@ -6977,7 +7077,7 @@
       </c>
       <c r="H8" s="46"/>
       <c r="I8" s="46" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="J8" s="46"/>
       <c r="K8" s="47"/>
@@ -7004,10 +7104,10 @@
       </c>
       <c r="C9" s="46"/>
       <c r="D9" s="46" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F9" s="46"/>
       <c r="G9" s="46" t="s">
@@ -7015,7 +7115,7 @@
       </c>
       <c r="H9" s="46"/>
       <c r="I9" s="46" t="s">
-        <v>779</v>
+        <v>772</v>
       </c>
       <c r="J9" s="46"/>
       <c r="K9" s="47"/>
@@ -7078,13 +7178,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="E11" s="50" t="s">
         <v>159</v>
@@ -7111,370 +7211,490 @@
       <c r="Y11" s="48"/>
       <c r="Z11" s="48"/>
     </row>
-    <row r="12" spans="1:26" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="b">
+    <row r="12" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="51" t="b">
         <v>1</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="52" t="s">
         <v>778</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>778</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>778</v>
-      </c>
-      <c r="E12" s="50" t="s">
+      <c r="C12" s="52" t="s">
+        <v>779</v>
+      </c>
+      <c r="D12" s="52" t="s">
+        <v>779</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="51"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="51"/>
+      <c r="V12" s="51"/>
+      <c r="W12" s="51"/>
+      <c r="X12" s="51"/>
+      <c r="Y12" s="51"/>
+      <c r="Z12" s="51"/>
+    </row>
+    <row r="13" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>780</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>781</v>
+      </c>
+      <c r="D13" s="57" t="s">
+        <v>781</v>
+      </c>
+      <c r="E13" s="57" t="s">
         <v>232</v>
       </c>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="48"/>
-      <c r="S12" s="48"/>
-      <c r="T12" s="48"/>
-      <c r="U12" s="48"/>
-      <c r="V12" s="48"/>
-      <c r="W12" s="48"/>
-      <c r="X12" s="48"/>
-      <c r="Y12" s="48"/>
-      <c r="Z12" s="48"/>
-    </row>
-    <row r="13" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
-    </row>
-    <row r="14" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-    </row>
-    <row r="15" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
-    </row>
-    <row r="16" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-    </row>
-    <row r="17" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-    </row>
-    <row r="18" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="58"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="58"/>
+      <c r="W13" s="58"/>
+      <c r="X13" s="58"/>
+      <c r="Y13" s="58"/>
+      <c r="Z13" s="58"/>
+    </row>
+    <row r="14" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="54"/>
+      <c r="B14" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54" t="s">
+        <v>782</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>783</v>
+      </c>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54" t="s">
+        <v>784</v>
+      </c>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="55"/>
+      <c r="P14" s="55"/>
+      <c r="Q14" s="55"/>
+      <c r="R14" s="55"/>
+      <c r="S14" s="55"/>
+      <c r="T14" s="55"/>
+      <c r="U14" s="55"/>
+      <c r="V14" s="55"/>
+      <c r="W14" s="55"/>
+      <c r="X14" s="55"/>
+      <c r="Y14" s="55"/>
+      <c r="Z14" s="55"/>
+    </row>
+    <row r="15" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>785</v>
+      </c>
+      <c r="C15" s="57" t="s">
+        <v>786</v>
+      </c>
+      <c r="D15" s="57" t="s">
+        <v>787</v>
+      </c>
+      <c r="E15" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="58"/>
+      <c r="R15" s="58"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="58"/>
+      <c r="W15" s="58"/>
+      <c r="X15" s="58"/>
+      <c r="Y15" s="58"/>
+      <c r="Z15" s="58"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="54"/>
+      <c r="B16" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54" t="s">
+        <v>788</v>
+      </c>
+      <c r="E16" s="54" t="s">
+        <v>789</v>
+      </c>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H16" s="54"/>
+      <c r="I16" s="59" t="s">
+        <v>790</v>
+      </c>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="55"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="55"/>
+      <c r="U16" s="55"/>
+      <c r="V16" s="55"/>
+      <c r="W16" s="55"/>
+      <c r="X16" s="55"/>
+      <c r="Y16" s="55"/>
+      <c r="Z16" s="55"/>
+    </row>
+    <row r="17" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="54"/>
+      <c r="B17" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54" t="s">
+        <v>791</v>
+      </c>
+      <c r="E17" s="54" t="s">
+        <v>792</v>
+      </c>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="54"/>
+      <c r="I17" s="53" t="s">
+        <v>793</v>
+      </c>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="55"/>
+      <c r="S17" s="55"/>
+      <c r="T17" s="55"/>
+      <c r="U17" s="55"/>
+      <c r="V17" s="55"/>
+      <c r="W17" s="55"/>
+      <c r="X17" s="55"/>
+      <c r="Y17" s="55"/>
+      <c r="Z17" s="55"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="55"/>
+      <c r="B18" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54" t="s">
+        <v>794</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54" t="s">
+        <v>796</v>
+      </c>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="55"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="55"/>
+      <c r="U18" s="55"/>
+      <c r="V18" s="55"/>
+      <c r="W18" s="55"/>
+      <c r="X18" s="55"/>
+      <c r="Y18" s="55"/>
+      <c r="Z18" s="55"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
-      <c r="V19" s="15"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="15"/>
-      <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
+      <c r="A19" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>797</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>798</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>799</v>
+      </c>
+      <c r="E19" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="58"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="58"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="58"/>
+      <c r="U19" s="58"/>
+      <c r="V19" s="58"/>
+      <c r="W19" s="58"/>
+      <c r="X19" s="58"/>
+      <c r="Y19" s="58"/>
+      <c r="Z19" s="58"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54" t="s">
+        <v>788</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>789</v>
+      </c>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="54"/>
+      <c r="I20" s="59" t="s">
+        <v>790</v>
+      </c>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="56"/>
+      <c r="P20" s="56"/>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="55"/>
+      <c r="T20" s="55"/>
+      <c r="U20" s="55"/>
+      <c r="V20" s="55"/>
+      <c r="W20" s="55"/>
+      <c r="X20" s="55"/>
+      <c r="Y20" s="55"/>
+      <c r="Z20" s="55"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54" t="s">
+        <v>791</v>
+      </c>
+      <c r="E21" s="54" t="s">
+        <v>792</v>
+      </c>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="54"/>
+      <c r="I21" s="53" t="s">
+        <v>793</v>
+      </c>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="55"/>
+      <c r="S21" s="55"/>
+      <c r="T21" s="55"/>
+      <c r="U21" s="55"/>
+      <c r="V21" s="55"/>
+      <c r="W21" s="55"/>
+      <c r="X21" s="55"/>
+      <c r="Y21" s="55"/>
+      <c r="Z21" s="55"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
+      <c r="A22" s="54"/>
+      <c r="B22" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54" t="s">
+        <v>794</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54" t="s">
+        <v>796</v>
+      </c>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="55"/>
+      <c r="R22" s="55"/>
+      <c r="S22" s="55"/>
+      <c r="T22" s="55"/>
+      <c r="U22" s="55"/>
+      <c r="V22" s="55"/>
+      <c r="W22" s="55"/>
+      <c r="X22" s="55"/>
+      <c r="Y22" s="55"/>
+      <c r="Z22" s="55"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="15"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54" t="s">
+        <v>805</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>807</v>
+      </c>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54" t="s">
+        <v>800</v>
+      </c>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="56"/>
+      <c r="R23" s="55"/>
+      <c r="S23" s="55"/>
+      <c r="T23" s="55"/>
+      <c r="U23" s="55"/>
+      <c r="V23" s="55"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="55"/>
+      <c r="Y23" s="55"/>
+      <c r="Z23" s="55"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54" t="s">
+        <v>806</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>808</v>
+      </c>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54" t="s">
+        <v>804</v>
+      </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="41"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -7485,52 +7705,69 @@
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
     </row>
-    <row r="25" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
-      <c r="U25" s="15"/>
-      <c r="V25" s="15"/>
-      <c r="W25" s="15"/>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="15"/>
-      <c r="Z25" s="15"/>
+    <row r="25" spans="1:26" s="51" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="57" t="b">
+        <v>0</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>813</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>809</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>813</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25" s="62"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="58"/>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="58"/>
+      <c r="S25" s="58"/>
+      <c r="T25" s="58"/>
+      <c r="U25" s="58"/>
+      <c r="V25" s="58"/>
+      <c r="W25" s="58"/>
+      <c r="X25" s="58"/>
+      <c r="Y25" s="58"/>
+      <c r="Z25" s="58"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
+      <c r="B26" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="D26" s="10" t="s">
+        <v>810</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>811</v>
+      </c>
       <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
+      <c r="G26" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
+      <c r="I26" s="10" t="s">
+        <v>812</v>
+      </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="41"/>
       <c r="R26" s="15"/>
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
@@ -7542,7 +7779,7 @@
       <c r="Z26" s="15"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -7554,11 +7791,11 @@
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41"/>
-      <c r="P27" s="41"/>
-      <c r="Q27" s="41"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
@@ -7570,7 +7807,7 @@
       <c r="Z27" s="15"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -7582,7 +7819,7 @@
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
-      <c r="M28" s="15"/>
+      <c r="M28" s="10"/>
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
@@ -7610,11 +7847,11 @@
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
       <c r="R29" s="15"/>
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
@@ -7625,24 +7862,24 @@
       <c r="Y29" s="15"/>
       <c r="Z29" s="15"/>
     </row>
-    <row r="30" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="41"/>
-      <c r="P30" s="41"/>
-      <c r="Q30" s="41"/>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
       <c r="S30" s="15"/>
       <c r="T30" s="15"/>
@@ -7724,8 +7961,8 @@
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
       <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="41"/>
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
       <c r="S33" s="15"/>
@@ -7752,8 +7989,8 @@
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
       <c r="N34" s="15"/>
-      <c r="O34" s="41"/>
-      <c r="P34" s="41"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
       <c r="Q34" s="15"/>
       <c r="R34" s="15"/>
       <c r="S34" s="15"/>
@@ -7877,7 +8114,7 @@
       <c r="Y38" s="15"/>
       <c r="Z38" s="15"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -7891,9 +8128,9 @@
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="41"/>
+      <c r="P39" s="41"/>
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
       <c r="S39" s="15"/>
@@ -7905,7 +8142,7 @@
       <c r="Y39" s="15"/>
       <c r="Z39" s="15"/>
     </row>
-    <row r="40" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -7919,9 +8156,9 @@
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="41"/>
-      <c r="P40" s="41"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
       <c r="S40" s="15"/>
@@ -8073,8 +8310,8 @@
       <c r="Y45" s="15"/>
       <c r="Z45" s="15"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
+    <row r="46" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
@@ -8088,8 +8325,8 @@
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
+      <c r="O46" s="41"/>
+      <c r="P46" s="41"/>
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
       <c r="S46" s="15"/>
@@ -8101,8 +8338,8 @@
       <c r="Y46" s="15"/>
       <c r="Z46" s="15"/>
     </row>
-    <row r="47" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
@@ -8116,8 +8353,8 @@
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
       <c r="N47" s="15"/>
-      <c r="O47" s="41"/>
-      <c r="P47" s="41"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
       <c r="S47" s="15"/>
@@ -8144,8 +8381,8 @@
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
+      <c r="O48" s="41"/>
+      <c r="P48" s="41"/>
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
       <c r="S48" s="15"/>
@@ -8200,8 +8437,8 @@
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
-      <c r="O50" s="41"/>
-      <c r="P50" s="41"/>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
       <c r="Q50" s="15"/>
       <c r="R50" s="15"/>
       <c r="S50" s="15"/>
@@ -8228,8 +8465,8 @@
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
-      <c r="O51" s="15"/>
-      <c r="P51" s="15"/>
+      <c r="O51" s="41"/>
+      <c r="P51" s="41"/>
       <c r="Q51" s="15"/>
       <c r="R51" s="15"/>
       <c r="S51" s="15"/>
@@ -8256,8 +8493,8 @@
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
-      <c r="O52" s="41"/>
-      <c r="P52" s="41"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
       <c r="S52" s="15"/>
@@ -8284,8 +8521,8 @@
       <c r="L53" s="15"/>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
+      <c r="O53" s="41"/>
+      <c r="P53" s="41"/>
       <c r="Q53" s="15"/>
       <c r="R53" s="15"/>
       <c r="S53" s="15"/>
@@ -8312,8 +8549,8 @@
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
       <c r="N54" s="15"/>
-      <c r="O54" s="41"/>
-      <c r="P54" s="41"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
       <c r="Q54" s="15"/>
       <c r="R54" s="15"/>
       <c r="S54" s="15"/>
@@ -8340,8 +8577,8 @@
       <c r="L55" s="15"/>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
+      <c r="O55" s="41"/>
+      <c r="P55" s="41"/>
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
       <c r="S55" s="15"/>
@@ -8368,8 +8605,8 @@
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
       <c r="N56" s="15"/>
-      <c r="O56" s="41"/>
-      <c r="P56" s="41"/>
+      <c r="O56" s="15"/>
+      <c r="P56" s="15"/>
       <c r="Q56" s="15"/>
       <c r="R56" s="15"/>
       <c r="S56" s="15"/>
@@ -8396,8 +8633,8 @@
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
       <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
-      <c r="P57" s="15"/>
+      <c r="O57" s="41"/>
+      <c r="P57" s="41"/>
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
       <c r="S57" s="15"/>
@@ -8424,8 +8661,8 @@
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
       <c r="N58" s="15"/>
-      <c r="O58" s="41"/>
-      <c r="P58" s="41"/>
+      <c r="O58" s="15"/>
+      <c r="P58" s="15"/>
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
       <c r="S58" s="15"/>
@@ -8437,34 +8674,6 @@
       <c r="Y58" s="15"/>
       <c r="Z58" s="15"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="15"/>
-      <c r="L59" s="15"/>
-      <c r="M59" s="15"/>
-      <c r="N59" s="15"/>
-      <c r="O59" s="15"/>
-      <c r="P59" s="15"/>
-      <c r="Q59" s="15"/>
-      <c r="R59" s="15"/>
-      <c r="S59" s="15"/>
-      <c r="T59" s="15"/>
-      <c r="U59" s="15"/>
-      <c r="V59" s="15"/>
-      <c r="W59" s="15"/>
-      <c r="X59" s="15"/>
-      <c r="Y59" s="15"/>
-      <c r="Z59" s="15"/>
-    </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
   <mergeCells count="1">
@@ -8472,17 +8681,12 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M92"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -8601,13 +8805,13 @@
     </row>
     <row r="4" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
+        <v>710</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>711</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="C4" s="15" t="s">
         <v>712</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>713</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>696</v>
@@ -8625,7 +8829,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
@@ -8634,16 +8838,16 @@
     </row>
     <row r="5" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
+        <v>713</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>714</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="C5" s="15" t="s">
         <v>715</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>716</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>717</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>469</v>
@@ -8658,7 +8862,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -8667,16 +8871,16 @@
     </row>
     <row r="6" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
+        <v>717</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>718</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="C6" s="46" t="s">
         <v>719</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="D6" s="46" t="s">
         <v>720</v>
-      </c>
-      <c r="D6" s="46" t="s">
-        <v>721</v>
       </c>
       <c r="E6" s="46" t="s">
         <v>469</v>
@@ -8700,16 +8904,16 @@
     </row>
     <row r="7" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
+        <v>721</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>722</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="C7" s="46" t="s">
         <v>723</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="D7" s="46" t="s">
         <v>724</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>725</v>
       </c>
       <c r="E7" s="46" t="s">
         <v>469</v>
@@ -8733,12 +8937,12 @@
     </row>
     <row r="8" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>469</v>
@@ -8762,12 +8966,12 @@
     </row>
     <row r="9" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>469</v>
@@ -8791,12 +8995,12 @@
     </row>
     <row r="10" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>469</v>
@@ -8820,12 +9024,12 @@
     </row>
     <row r="11" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>469</v>
@@ -8849,12 +9053,12 @@
     </row>
     <row r="12" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B12" s="22"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>469</v>
@@ -8878,11 +9082,11 @@
     </row>
     <row r="13" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>469</v>
@@ -8906,11 +9110,11 @@
     </row>
     <row r="14" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>469</v>
@@ -8934,11 +9138,11 @@
     </row>
     <row r="15" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>469</v>
@@ -8962,11 +9166,11 @@
     </row>
     <row r="16" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>469</v>
@@ -8990,11 +9194,11 @@
     </row>
     <row r="17" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>469</v>
@@ -9018,11 +9222,11 @@
     </row>
     <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>469</v>
@@ -9046,12 +9250,12 @@
     </row>
     <row r="19" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B19" s="22"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>469</v>
@@ -9075,12 +9279,12 @@
     </row>
     <row r="20" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>469</v>
@@ -9104,12 +9308,12 @@
     </row>
     <row r="21" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B21" s="22"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>469</v>
@@ -9222,9 +9426,7 @@
       <c r="A25" s="15" t="s">
         <v>650</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>650</v>
-      </c>
+      <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15" t="s">
         <v>655</v>
@@ -9251,15 +9453,15 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15" t="s">
+        <v>754</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>755</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>756</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>63</v>
@@ -9280,15 +9482,15 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>63</v>
@@ -9305,15 +9507,15 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F28" s="15" t="s">
         <v>63</v>
@@ -9330,15 +9532,15 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>63</v>
@@ -9355,15 +9557,15 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>63</v>
@@ -9380,15 +9582,15 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15" t="s">
+        <v>765</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>766</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>767</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>63</v>
@@ -9405,15 +9607,15 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F32" s="15" t="s">
         <v>63</v>
@@ -9428,96 +9630,78 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>770</v>
-      </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15" t="s">
-        <v>771</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>772</v>
-      </c>
-      <c r="F33" s="15" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="60" t="s">
+        <v>801</v>
+      </c>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60" t="s">
+        <v>802</v>
+      </c>
+      <c r="E33" s="60" t="s">
+        <v>803</v>
+      </c>
+      <c r="F33" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="G33" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" s="15" t="b">
+      <c r="G33" s="60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I33" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>773</v>
-      </c>
+      <c r="I33" s="60" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="60"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="15" t="s">
-        <v>774</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>772</v>
-      </c>
-      <c r="F34" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="G34" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="H34" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" s="46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B35" s="22"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36" s="22"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" s="22"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" s="22"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B39" s="22"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B40" s="22"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B41" s="22"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B42" s="22"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" s="22"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" s="22"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" s="22"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B46" s="22"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47" s="22"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B48" s="22"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
@@ -9645,21 +9829,10 @@
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="22"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="22"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
First cut at HVAC configurations for commercial buildings; updating measures list word doc accordingly.
</commit_message>
<xml_diff>
--- a/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
+++ b/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="240" windowWidth="15360" windowHeight="7755" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="240" windowWidth="15360" windowHeight="7755" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="780">
   <si>
     <t>type</t>
   </si>
@@ -1975,33 +1975,12 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>Unmet Cooling Hours</t>
-  </si>
-  <si>
-    <t>hrs</t>
-  </si>
-  <si>
-    <t>Unmet Heating Hours</t>
-  </si>
-  <si>
-    <t>Total Unmet Hours</t>
-  </si>
-  <si>
     <t>Building Area</t>
   </si>
   <si>
     <t>m2</t>
   </si>
   <si>
-    <t>standard_reports.time_setpoint_not_met_during_occupied_cooling</t>
-  </si>
-  <si>
-    <t>standard_reports.time_setpoint_not_met_during_occupied_heating</t>
-  </si>
-  <si>
-    <t>standard_reports.time_setpoint_not_met_during_occupied_hours</t>
-  </si>
-  <si>
     <t>standard_reports.total_building_area</t>
   </si>
   <si>
@@ -2176,18 +2155,6 @@
     <t>total_site_energy_intensity</t>
   </si>
   <si>
-    <t>Total Source Energy Intensity</t>
-  </si>
-  <si>
-    <t>Source EUI</t>
-  </si>
-  <si>
-    <t>total_source_energy_intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.total_source_energy</t>
-  </si>
-  <si>
     <t>Total Natural Gas Intensity</t>
   </si>
   <si>
@@ -2212,90 +2179,6 @@
     <t>standard_report_legacy.total_electricity</t>
   </si>
   <si>
-    <t>Natural Gas Heating Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.heating_natural_gas</t>
-  </si>
-  <si>
-    <t>Cooling Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.cooling_electricity</t>
-  </si>
-  <si>
-    <t>Interior Lighting Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_lighting_electricity</t>
-  </si>
-  <si>
-    <t>Exterior Lighting Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.exterior_lighting_electricity</t>
-  </si>
-  <si>
-    <t>Equipment Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_equipment_electricity</t>
-  </si>
-  <si>
-    <t>Equipment Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_equipment_natural_gas</t>
-  </si>
-  <si>
-    <t>Experior Equipment Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.exterior_equipment_electricity</t>
-  </si>
-  <si>
-    <t>Fans Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.fans_electricity</t>
-  </si>
-  <si>
-    <t>Pumps Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.pumps_electricity</t>
-  </si>
-  <si>
-    <t>Heat Rejection Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.heat_rejection_electricity</t>
-  </si>
-  <si>
-    <t>Humidification Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.humidification_electricity</t>
-  </si>
-  <si>
-    <t>Water Systems Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.water_systems_electricity</t>
-  </si>
-  <si>
-    <t>Water Systems Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.water_systems_natural_gas</t>
-  </si>
-  <si>
-    <t>Refrigeration Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.refrigeration_electricity</t>
-  </si>
-  <si>
     <t>Electricity Cooling</t>
   </si>
   <si>
@@ -2305,12 +2188,6 @@
     <t>kWh</t>
   </si>
   <si>
-    <t>Electricity Fans</t>
-  </si>
-  <si>
-    <t>standard_reports.electricity_fans_ip</t>
-  </si>
-  <si>
     <t>Electricity Heating</t>
   </si>
   <si>
@@ -2323,12 +2200,6 @@
     <t>standard_reports.electricity_ip</t>
   </si>
   <si>
-    <t>Electricity Pumps</t>
-  </si>
-  <si>
-    <t>standard_reports.electricity_pumps_ip</t>
-  </si>
-  <si>
     <t>Natural Gas Heating</t>
   </si>
   <si>
@@ -2362,12 +2233,6 @@
     <t>../weather/USA_CO_Denver.Intl.AP.725650_TMY3.ddy</t>
   </si>
   <si>
-    <t>178897'</t>
-  </si>
-  <si>
-    <t>['178897','222412','236646','231874','127676']</t>
-  </si>
-  <si>
     <t>URBANopt Testing 1</t>
   </si>
   <si>
@@ -2440,15 +2305,6 @@
     <t>../DencityReports/report_metadata.csv</t>
   </si>
   <si>
-    <t>Total Life Cycle Cost</t>
-  </si>
-  <si>
-    <t>standard_report.total_life_cycle_cost</t>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
     <t>../DencityReports/report_timeseries.csv</t>
   </si>
   <si>
@@ -2464,19 +2320,61 @@
     <t>file_path_timeseries</t>
   </si>
   <si>
-    <t>urban_building_district_system</t>
-  </si>
-  <si>
-    <t>Type of district system to model</t>
-  </si>
-  <si>
-    <t>district_system_type</t>
-  </si>
-  <si>
-    <t>Conventional</t>
-  </si>
-  <si>
-    <t>UrbanBuildingDistrictSystem</t>
+    <t>Cooling source to model</t>
+  </si>
+  <si>
+    <t>Heating source to model</t>
+  </si>
+  <si>
+    <t>cooling_source</t>
+  </si>
+  <si>
+    <t>heating_source</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>|'Electric','District Chilled Water','District Ambient Water'|</t>
+  </si>
+  <si>
+    <t>|'Gas','Electric','District Hot Water','District Ambient Water'|</t>
+  </si>
+  <si>
+    <t>['Electric','District Chilled Water','District Ambient Water']</t>
+  </si>
+  <si>
+    <t>['Gas','Electric','District Hot Water','District Ambient Water']</t>
+  </si>
+  <si>
+    <t>District Cooling</t>
+  </si>
+  <si>
+    <t>District Heating</t>
+  </si>
+  <si>
+    <t>142484'</t>
+  </si>
+  <si>
+    <t>standard_reports.district_cooling_ip</t>
+  </si>
+  <si>
+    <t>standard_reports.district_heating_ip</t>
+  </si>
+  <si>
+    <t>['142484','116245','113178']</t>
+  </si>
+  <si>
+    <t>Bldg Use</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>urbangeometrycreation.bldg_use</t>
   </si>
 </sst>
 </file>
@@ -2543,7 +2441,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2628,6 +2526,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -4152,7 +4056,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4273,7 +4177,9 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6080,7 +5986,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6118,7 +6024,7 @@
         <v>435</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>436</v>
@@ -6129,7 +6035,7 @@
         <v>457</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>769</v>
+        <v>726</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>458</v>
@@ -6140,7 +6046,7 @@
         <v>470</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>611</v>
@@ -6151,7 +6057,7 @@
         <v>471</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>473</v>
@@ -6219,21 +6125,21 @@
         <v>$1.96/hour</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="23" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="2" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -6251,7 +6157,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>777</v>
+        <v>732</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>472</v>
@@ -6262,7 +6168,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>612</v>
@@ -6298,7 +6204,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
@@ -6373,9 +6279,8 @@
         <f>IF(LEN(INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)-2))=0,"",INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)-2))</f>
         <v>Sample Method</v>
       </c>
-      <c r="B25" s="18" t="str">
-        <f>IF(D25&lt;&gt;"",D25,IF(LEN(INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)-1))=0,"",INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)-1)))</f>
-        <v>individual_variables</v>
+      <c r="B25" s="18" t="s">
+        <v>453</v>
       </c>
       <c r="C25" s="25" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)))=0,"",INDEX(Lookups!$C$19:$AF$28,1,3*MATCH(Setup!$B22,Lookups!$A$19:$A$28,0)))</f>
@@ -6606,7 +6511,7 @@
         <v>28</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>773</v>
+        <v>730</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6614,7 +6519,7 @@
         <v>28</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>774</v>
+        <v>731</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -6642,13 +6547,13 @@
         <v>31</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>449</v>
@@ -6672,13 +6577,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -6714,7 +6619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6896,13 +6801,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
       <c r="E4" s="39" t="s">
         <v>67</v>
@@ -6936,10 +6841,10 @@
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>687</v>
+        <v>680</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15" t="s">
@@ -6947,7 +6852,7 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -6974,10 +6879,10 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="42" t="s">
@@ -6985,10 +6890,10 @@
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="45" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="J6" s="42" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="K6" s="43">
         <v>0</v>
@@ -7005,12 +6910,12 @@
       <c r="O6" s="43">
         <v>0</v>
       </c>
-      <c r="P6" s="43" t="s">
+      <c r="P6" s="64" t="s">
         <v>776</v>
       </c>
       <c r="Q6" s="43"/>
       <c r="R6" s="42" t="s">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="S6" s="42"/>
       <c r="T6" s="42"/>
@@ -7026,13 +6931,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="D7" s="48" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="E7" s="48" t="s">
         <v>67</v>
@@ -7066,10 +6971,10 @@
       </c>
       <c r="C8" s="46"/>
       <c r="D8" s="46" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="F8" s="46"/>
       <c r="G8" s="46" t="s">
@@ -7077,7 +6982,7 @@
       </c>
       <c r="H8" s="46"/>
       <c r="I8" s="46" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="J8" s="46"/>
       <c r="K8" s="47"/>
@@ -7104,10 +7009,10 @@
       </c>
       <c r="C9" s="46"/>
       <c r="D9" s="46" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="F9" s="46"/>
       <c r="G9" s="46" t="s">
@@ -7115,7 +7020,7 @@
       </c>
       <c r="H9" s="46"/>
       <c r="I9" s="46" t="s">
-        <v>772</v>
+        <v>729</v>
       </c>
       <c r="J9" s="46"/>
       <c r="K9" s="47"/>
@@ -7140,13 +7045,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>693</v>
+        <v>686</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
       <c r="E10" s="39" t="s">
         <v>67</v>
@@ -7173,170 +7078,202 @@
       <c r="Y10" s="39"/>
       <c r="Z10" s="39"/>
     </row>
-    <row r="11" spans="1:26" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50" t="b">
+    <row r="11" spans="1:26" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="62"/>
+      <c r="B11" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62" t="s">
+        <v>761</v>
+      </c>
+      <c r="E11" s="62" t="s">
+        <v>763</v>
+      </c>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62" t="s">
+        <v>765</v>
+      </c>
+      <c r="J11" s="62" t="s">
+        <v>767</v>
+      </c>
+      <c r="K11" s="62">
+        <v>0</v>
+      </c>
+      <c r="L11" s="62">
+        <v>0</v>
+      </c>
+      <c r="M11" s="62">
+        <v>0</v>
+      </c>
+      <c r="N11" s="62">
+        <v>0</v>
+      </c>
+      <c r="O11" s="62">
+        <v>0</v>
+      </c>
+      <c r="P11" s="62" t="s">
+        <v>769</v>
+      </c>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="62" t="s">
+        <v>687</v>
+      </c>
+      <c r="S11" s="62"/>
+      <c r="T11" s="62"/>
+      <c r="U11" s="62"/>
+      <c r="V11" s="62"/>
+      <c r="W11" s="62"/>
+      <c r="X11" s="62"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="62"/>
+    </row>
+    <row r="12" spans="1:26" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="62"/>
+      <c r="B12" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62" t="s">
+        <v>762</v>
+      </c>
+      <c r="E12" s="62" t="s">
+        <v>764</v>
+      </c>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62" t="s">
+        <v>766</v>
+      </c>
+      <c r="J12" s="62" t="s">
+        <v>768</v>
+      </c>
+      <c r="K12" s="62">
+        <v>0</v>
+      </c>
+      <c r="L12" s="62">
+        <v>0</v>
+      </c>
+      <c r="M12" s="62">
+        <v>0</v>
+      </c>
+      <c r="N12" s="62">
+        <v>0</v>
+      </c>
+      <c r="O12" s="62">
+        <v>0</v>
+      </c>
+      <c r="P12" s="62" t="s">
+        <v>770</v>
+      </c>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="62" t="s">
+        <v>687</v>
+      </c>
+      <c r="S12" s="62"/>
+      <c r="T12" s="62"/>
+      <c r="U12" s="62"/>
+      <c r="V12" s="62"/>
+      <c r="W12" s="62"/>
+      <c r="X12" s="62"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="62"/>
+    </row>
+    <row r="13" spans="1:26" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="B11" s="50" t="s">
-        <v>770</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>771</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>770</v>
-      </c>
-      <c r="E11" s="50" t="s">
+      <c r="B13" s="50" t="s">
+        <v>727</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>728</v>
+      </c>
+      <c r="D13" s="50" t="s">
+        <v>727</v>
+      </c>
+      <c r="E13" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="48"/>
-      <c r="Z11" s="48"/>
-    </row>
-    <row r="12" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="b">
-        <v>1</v>
-      </c>
-      <c r="B12" s="52" t="s">
-        <v>778</v>
-      </c>
-      <c r="C12" s="52" t="s">
-        <v>779</v>
-      </c>
-      <c r="D12" s="52" t="s">
-        <v>779</v>
-      </c>
-      <c r="E12" s="52" t="s">
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
+      <c r="U13" s="48"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="48"/>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="48"/>
+    </row>
+    <row r="14" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="51" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>733</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>734</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>734</v>
+      </c>
+      <c r="E14" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="51"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="51"/>
-      <c r="T12" s="51"/>
-      <c r="U12" s="51"/>
-      <c r="V12" s="51"/>
-      <c r="W12" s="51"/>
-      <c r="X12" s="51"/>
-      <c r="Y12" s="51"/>
-      <c r="Z12" s="51"/>
-    </row>
-    <row r="13" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="B13" s="57" t="s">
-        <v>780</v>
-      </c>
-      <c r="C13" s="57" t="s">
-        <v>781</v>
-      </c>
-      <c r="D13" s="57" t="s">
-        <v>781</v>
-      </c>
-      <c r="E13" s="57" t="s">
-        <v>232</v>
-      </c>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="58"/>
-      <c r="R13" s="58"/>
-      <c r="S13" s="58"/>
-      <c r="T13" s="58"/>
-      <c r="U13" s="58"/>
-      <c r="V13" s="58"/>
-      <c r="W13" s="58"/>
-      <c r="X13" s="58"/>
-      <c r="Y13" s="58"/>
-      <c r="Z13" s="58"/>
-    </row>
-    <row r="14" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54" t="s">
-        <v>782</v>
-      </c>
-      <c r="E14" s="54" t="s">
-        <v>783</v>
-      </c>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54" t="s">
-        <v>784</v>
-      </c>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="55"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="55"/>
-      <c r="P14" s="55"/>
-      <c r="Q14" s="55"/>
-      <c r="R14" s="55"/>
-      <c r="S14" s="55"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="55"/>
-      <c r="V14" s="55"/>
-      <c r="W14" s="55"/>
-      <c r="X14" s="55"/>
-      <c r="Y14" s="55"/>
-      <c r="Z14" s="55"/>
-    </row>
-    <row r="15" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="51"/>
+    </row>
+    <row r="15" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>785</v>
+        <v>735</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>786</v>
+        <v>736</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>787</v>
+        <v>736</v>
       </c>
       <c r="E15" s="57" t="s">
         <v>232</v>
@@ -7363,25 +7300,25 @@
       <c r="Y15" s="58"/>
       <c r="Z15" s="58"/>
     </row>
-    <row r="16" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="54"/>
       <c r="B16" s="54" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="54"/>
       <c r="D16" s="54" t="s">
-        <v>788</v>
+        <v>737</v>
       </c>
       <c r="E16" s="54" t="s">
-        <v>789</v>
+        <v>738</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="H16" s="54"/>
-      <c r="I16" s="59" t="s">
-        <v>790</v>
+      <c r="I16" s="54" t="s">
+        <v>739</v>
       </c>
       <c r="J16" s="54"/>
       <c r="K16" s="54"/>
@@ -7401,63 +7338,63 @@
       <c r="Y16" s="55"/>
       <c r="Z16" s="55"/>
     </row>
-    <row r="17" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
-      <c r="B17" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54" t="s">
-        <v>791</v>
-      </c>
-      <c r="E17" s="54" t="s">
-        <v>792</v>
-      </c>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H17" s="54"/>
-      <c r="I17" s="53" t="s">
-        <v>793</v>
-      </c>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="55"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="55"/>
-      <c r="P17" s="55"/>
-      <c r="Q17" s="55"/>
-      <c r="R17" s="55"/>
-      <c r="S17" s="55"/>
-      <c r="T17" s="55"/>
-      <c r="U17" s="55"/>
-      <c r="V17" s="55"/>
-      <c r="W17" s="55"/>
-      <c r="X17" s="55"/>
-      <c r="Y17" s="55"/>
-      <c r="Z17" s="55"/>
-    </row>
-    <row r="18" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="55"/>
+    <row r="17" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="57" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>740</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>741</v>
+      </c>
+      <c r="D17" s="57" t="s">
+        <v>742</v>
+      </c>
+      <c r="E17" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="58"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="58"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="58"/>
+      <c r="U17" s="58"/>
+      <c r="V17" s="58"/>
+      <c r="W17" s="58"/>
+      <c r="X17" s="58"/>
+      <c r="Y17" s="58"/>
+      <c r="Z17" s="58"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="54"/>
       <c r="B18" s="54" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="54"/>
       <c r="D18" s="54" t="s">
-        <v>794</v>
+        <v>743</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>795</v>
+        <v>744</v>
       </c>
       <c r="F18" s="54"/>
       <c r="G18" s="54" t="s">
         <v>103</v>
       </c>
       <c r="H18" s="54"/>
-      <c r="I18" s="54" t="s">
-        <v>796</v>
+      <c r="I18" s="59" t="s">
+        <v>745</v>
       </c>
       <c r="J18" s="54"/>
       <c r="K18" s="54"/>
@@ -7477,72 +7414,72 @@
       <c r="Y18" s="55"/>
       <c r="Z18" s="55"/>
     </row>
-    <row r="19" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="b">
-        <v>1</v>
-      </c>
-      <c r="B19" s="57" t="s">
-        <v>797</v>
-      </c>
-      <c r="C19" s="57" t="s">
-        <v>798</v>
-      </c>
-      <c r="D19" s="57" t="s">
-        <v>799</v>
-      </c>
-      <c r="E19" s="57" t="s">
-        <v>232</v>
-      </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="58"/>
-      <c r="O19" s="58"/>
-      <c r="P19" s="58"/>
-      <c r="Q19" s="58"/>
-      <c r="R19" s="58"/>
-      <c r="S19" s="58"/>
-      <c r="T19" s="58"/>
-      <c r="U19" s="58"/>
-      <c r="V19" s="58"/>
-      <c r="W19" s="58"/>
-      <c r="X19" s="58"/>
-      <c r="Y19" s="58"/>
-      <c r="Z19" s="58"/>
+    <row r="19" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="54"/>
+      <c r="B19" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54" t="s">
+        <v>746</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>747</v>
+      </c>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="54"/>
+      <c r="I19" s="53" t="s">
+        <v>748</v>
+      </c>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="55"/>
+      <c r="T19" s="55"/>
+      <c r="U19" s="55"/>
+      <c r="V19" s="55"/>
+      <c r="W19" s="55"/>
+      <c r="X19" s="55"/>
+      <c r="Y19" s="55"/>
+      <c r="Z19" s="55"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
+      <c r="A20" s="55"/>
       <c r="B20" s="54" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="54"/>
       <c r="D20" s="54" t="s">
-        <v>788</v>
+        <v>749</v>
       </c>
       <c r="E20" s="54" t="s">
-        <v>789</v>
+        <v>750</v>
       </c>
       <c r="F20" s="54"/>
       <c r="G20" s="54" t="s">
         <v>103</v>
       </c>
       <c r="H20" s="54"/>
-      <c r="I20" s="59" t="s">
-        <v>790</v>
+      <c r="I20" s="54" t="s">
+        <v>751</v>
       </c>
       <c r="J20" s="54"/>
       <c r="K20" s="54"/>
       <c r="L20" s="54"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="56"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="55"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="55"/>
       <c r="R20" s="55"/>
       <c r="S20" s="55"/>
       <c r="T20" s="55"/>
@@ -7554,42 +7491,42 @@
       <c r="Z20" s="55"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="55"/>
-      <c r="B21" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54" t="s">
-        <v>791</v>
-      </c>
-      <c r="E21" s="54" t="s">
-        <v>792</v>
-      </c>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21" s="54"/>
-      <c r="I21" s="53" t="s">
-        <v>793</v>
-      </c>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="55"/>
-      <c r="S21" s="55"/>
-      <c r="T21" s="55"/>
-      <c r="U21" s="55"/>
-      <c r="V21" s="55"/>
-      <c r="W21" s="55"/>
-      <c r="X21" s="55"/>
-      <c r="Y21" s="55"/>
-      <c r="Z21" s="55"/>
+      <c r="A21" s="57" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>752</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>753</v>
+      </c>
+      <c r="D21" s="57" t="s">
+        <v>754</v>
+      </c>
+      <c r="E21" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="58"/>
+      <c r="Q21" s="58"/>
+      <c r="R21" s="58"/>
+      <c r="S21" s="58"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="V21" s="58"/>
+      <c r="W21" s="58"/>
+      <c r="X21" s="58"/>
+      <c r="Y21" s="58"/>
+      <c r="Z21" s="58"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="54"/>
@@ -7598,27 +7535,27 @@
       </c>
       <c r="C22" s="54"/>
       <c r="D22" s="54" t="s">
-        <v>794</v>
+        <v>743</v>
       </c>
       <c r="E22" s="54" t="s">
-        <v>795</v>
+        <v>744</v>
       </c>
       <c r="F22" s="54"/>
       <c r="G22" s="54" t="s">
         <v>103</v>
       </c>
       <c r="H22" s="54"/>
-      <c r="I22" s="54" t="s">
-        <v>796</v>
+      <c r="I22" s="59" t="s">
+        <v>745</v>
       </c>
       <c r="J22" s="54"/>
       <c r="K22" s="54"/>
       <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="55"/>
-      <c r="O22" s="55"/>
-      <c r="P22" s="55"/>
-      <c r="Q22" s="55"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="56"/>
       <c r="R22" s="55"/>
       <c r="S22" s="55"/>
       <c r="T22" s="55"/>
@@ -7630,33 +7567,33 @@
       <c r="Z22" s="55"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
+      <c r="A23" s="55"/>
       <c r="B23" s="54" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="54"/>
       <c r="D23" s="54" t="s">
-        <v>805</v>
+        <v>746</v>
       </c>
       <c r="E23" s="54" t="s">
-        <v>807</v>
+        <v>747</v>
       </c>
       <c r="F23" s="54"/>
       <c r="G23" s="54" t="s">
         <v>103</v>
       </c>
       <c r="H23" s="54"/>
-      <c r="I23" s="54" t="s">
-        <v>800</v>
+      <c r="I23" s="53" t="s">
+        <v>748</v>
       </c>
       <c r="J23" s="54"/>
       <c r="K23" s="54"/>
       <c r="L23" s="54"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="56"/>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="56"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
       <c r="R23" s="55"/>
       <c r="S23" s="55"/>
       <c r="T23" s="55"/>
@@ -7668,16 +7605,16 @@
       <c r="Z23" s="55"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="54" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="54"/>
       <c r="D24" s="54" t="s">
-        <v>806</v>
+        <v>749</v>
       </c>
       <c r="E24" s="54" t="s">
-        <v>808</v>
+        <v>750</v>
       </c>
       <c r="F24" s="54"/>
       <c r="G24" s="54" t="s">
@@ -7685,89 +7622,92 @@
       </c>
       <c r="H24" s="54"/>
       <c r="I24" s="54" t="s">
-        <v>804</v>
-      </c>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="15"/>
-      <c r="W24" s="15"/>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="15"/>
-      <c r="Z24" s="15"/>
-    </row>
-    <row r="25" spans="1:26" s="51" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="b">
-        <v>0</v>
-      </c>
-      <c r="B25" s="57" t="s">
-        <v>813</v>
-      </c>
-      <c r="C25" s="57" t="s">
-        <v>809</v>
-      </c>
-      <c r="D25" s="57" t="s">
-        <v>813</v>
-      </c>
-      <c r="E25" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="I25" s="62"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
-      <c r="T25" s="58"/>
-      <c r="U25" s="58"/>
-      <c r="V25" s="58"/>
-      <c r="W25" s="58"/>
-      <c r="X25" s="58"/>
-      <c r="Y25" s="58"/>
-      <c r="Z25" s="58"/>
+        <v>751</v>
+      </c>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="55"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="55"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="55"/>
+      <c r="T24" s="55"/>
+      <c r="U24" s="55"/>
+      <c r="V24" s="55"/>
+      <c r="W24" s="55"/>
+      <c r="X24" s="55"/>
+      <c r="Y24" s="55"/>
+      <c r="Z24" s="55"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="54"/>
+      <c r="B25" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54" t="s">
+        <v>757</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>759</v>
+      </c>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54" t="s">
+        <v>755</v>
+      </c>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="56"/>
+      <c r="Q25" s="56"/>
+      <c r="R25" s="55"/>
+      <c r="S25" s="55"/>
+      <c r="T25" s="55"/>
+      <c r="U25" s="55"/>
+      <c r="V25" s="55"/>
+      <c r="W25" s="55"/>
+      <c r="X25" s="55"/>
+      <c r="Y25" s="55"/>
+      <c r="Z25" s="55"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10" t="s">
-        <v>810</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>811</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10" t="s">
-        <v>812</v>
+      <c r="A26" s="15"/>
+      <c r="B26" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54" t="s">
+        <v>758</v>
+      </c>
+      <c r="E26" s="54" t="s">
+        <v>760</v>
+      </c>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54" t="s">
+        <v>756</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="41"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
@@ -8686,19 +8626,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M90"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="23" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
@@ -8805,16 +8745,16 @@
     </row>
     <row r="4" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>469</v>
@@ -8837,32 +8777,32 @@
       <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>713</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>714</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>715</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>716</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="A5" s="46" t="s">
+        <v>706</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>707</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>708</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>709</v>
+      </c>
+      <c r="E5" s="46" t="s">
         <v>469</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="15" t="b">
+      <c r="G5" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="I5" s="15" t="b">
-        <v>1</v>
+      <c r="I5" s="46" t="b">
+        <v>0</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
@@ -8871,16 +8811,16 @@
     </row>
     <row r="6" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>717</v>
+        <v>710</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>719</v>
+        <v>712</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>720</v>
+        <v>713</v>
       </c>
       <c r="E6" s="46" t="s">
         <v>469</v>
@@ -8902,32 +8842,28 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
-        <v>721</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>722</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>723</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>724</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>469</v>
-      </c>
-      <c r="F7" s="46" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>646</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>647</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="46" t="b">
+      <c r="G7" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="I7" s="46" t="b">
+      <c r="I7" s="15" t="b">
         <v>0</v>
       </c>
       <c r="J7" s="15"/>
@@ -8935,17 +8871,17 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>725</v>
-      </c>
-      <c r="B8" s="22"/>
+        <v>714</v>
+      </c>
+      <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>469</v>
+        <v>716</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>63</v>
@@ -8964,17 +8900,17 @@
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>727</v>
-      </c>
-      <c r="B9" s="22"/>
+        <v>717</v>
+      </c>
+      <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>728</v>
+        <v>718</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>469</v>
+        <v>716</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>63</v>
@@ -8988,22 +8924,18 @@
       <c r="I9" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-    </row>
-    <row r="10" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>729</v>
-      </c>
-      <c r="B10" s="22"/>
+        <v>719</v>
+      </c>
+      <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>469</v>
+        <v>716</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>63</v>
@@ -9017,22 +8949,18 @@
       <c r="I10" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-    </row>
-    <row r="11" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>731</v>
-      </c>
-      <c r="B11" s="22"/>
+        <v>721</v>
+      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>469</v>
+        <v>723</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>63</v>
@@ -9046,22 +8974,18 @@
       <c r="I11" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-    </row>
-    <row r="12" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>733</v>
-      </c>
-      <c r="B12" s="22"/>
+        <v>724</v>
+      </c>
+      <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>734</v>
+        <v>725</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>469</v>
+        <v>723</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>63</v>
@@ -9075,633 +8999,177 @@
       <c r="I12" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-    </row>
-    <row r="13" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>735</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
-        <v>736</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F13" s="15" t="s">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
+        <v>771</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="D13" s="46" t="s">
+        <v>774</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>723</v>
+      </c>
+      <c r="F13" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="15" t="b">
+      <c r="G13" s="60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-    </row>
-    <row r="14" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>737</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
-        <v>738</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F14" s="15" t="s">
+      <c r="I13" s="60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
+        <v>772</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="D14" s="46" t="s">
+        <v>775</v>
+      </c>
+      <c r="E14" s="46" t="s">
+        <v>723</v>
+      </c>
+      <c r="F14" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="15" t="b">
+      <c r="G14" s="60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="I14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-    </row>
-    <row r="15" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>739</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
-        <v>740</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="15" t="b">
+      <c r="I14" s="60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="46" t="s">
+        <v>777</v>
+      </c>
+      <c r="B15" s="53"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="46" t="s">
+        <v>779</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>778</v>
+      </c>
+      <c r="F15" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="I15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-    </row>
-    <row r="16" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>741</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15" t="s">
-        <v>742</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-    </row>
-    <row r="17" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>743</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-    </row>
-    <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>745</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15" t="s">
-        <v>746</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-    </row>
-    <row r="19" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>747</v>
-      </c>
+      <c r="I15" s="46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="22"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="22"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15" t="s">
-        <v>748</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-    </row>
-    <row r="20" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>749</v>
-      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="22"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
-        <v>750</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-    </row>
-    <row r="21" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>751</v>
-      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="22"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15" t="s">
-        <v>752</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-    </row>
-    <row r="22" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>646</v>
-      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="22"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15" t="s">
-        <v>652</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>648</v>
-      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="22"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15" t="s">
-        <v>653</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>649</v>
-      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="22"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15" t="s">
-        <v>654</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>650</v>
-      </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15" t="s">
-        <v>655</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>651</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>753</v>
-      </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15" t="s">
-        <v>754</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>755</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>756</v>
-      </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15" t="s">
-        <v>757</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>755</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>758</v>
-      </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15" t="s">
-        <v>759</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>755</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H28" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>760</v>
-      </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15" t="s">
-        <v>761</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>755</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H29" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>762</v>
-      </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15" t="s">
-        <v>763</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>755</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I30" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>764</v>
-      </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15" t="s">
-        <v>765</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>766</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H31" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I31" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>767</v>
-      </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15" t="s">
-        <v>768</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>766</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G32" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="60" t="s">
-        <v>801</v>
-      </c>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60" t="s">
-        <v>802</v>
-      </c>
-      <c r="E33" s="60" t="s">
-        <v>803</v>
-      </c>
-      <c r="F33" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="G33" s="60" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" s="60" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33" s="60" t="b">
-        <v>0</v>
-      </c>
-      <c r="J33" s="60"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="60"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="22"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="22"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="22"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="22"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="22"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="22"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="22"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="22"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="22"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="22"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="22"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="22"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="22"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="22"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="22"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="22"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="22"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="22"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="22"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="22"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="22"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="22"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="22"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
@@ -9754,81 +9222,6 @@
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="22"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="22"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="22"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="22"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="22"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="22"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="22"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="22"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="22"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="22"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="22"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="22"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="22"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="22"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="22"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="22"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="22"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="22"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="22"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="22"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="22"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="22"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="22"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="22"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="22"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -18123,7 +17516,7 @@
         <v>638</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -18140,7 +17533,7 @@
         <v>636</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -18157,7 +17550,7 @@
         <v>637</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -18174,7 +17567,7 @@
         <v>639</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -18191,7 +17584,7 @@
         <v>641</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
@@ -18259,18 +17652,18 @@
         <v>553</v>
       </c>
       <c r="U18" s="22" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="V18" s="22"/>
       <c r="W18" s="22"/>
       <c r="X18" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="AA18" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="AD18" s="22" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="AE18" s="22"/>
       <c r="AF18" s="22"/>
@@ -18316,16 +17709,16 @@
         <v>580</v>
       </c>
       <c r="U19" s="22" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="V19" s="22" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="W19" s="22" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="AA19" s="22" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="AB19" s="22">
         <v>30</v>
@@ -18334,13 +17727,13 @@
         <v>589</v>
       </c>
       <c r="AD19" s="22" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="AE19" s="22" t="b">
         <v>1</v>
       </c>
       <c r="AF19" s="22" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
@@ -18390,16 +17783,16 @@
         <v>2</v>
       </c>
       <c r="W20" s="22" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="AD20" s="22" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
       <c r="AE20" s="22" t="b">
         <v>1</v>
       </c>
       <c r="AF20" s="22" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
@@ -18477,13 +17870,13 @@
         <v>541</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="M23" s="22">
         <v>1</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="O23" s="23" t="s">
         <v>568</v>
@@ -18529,16 +17922,16 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="J25" s="23">
         <v>0</v>
       </c>
       <c r="K25" s="23" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>539</v>
@@ -18550,18 +17943,18 @@
         <v>578</v>
       </c>
       <c r="O25" s="23" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="P25" s="22">
         <v>2</v>
       </c>
       <c r="Q25" s="22" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>544</v>
@@ -18581,7 +17974,7 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>558</v>
@@ -18604,7 +17997,7 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>559</v>
@@ -18616,13 +18009,13 @@
         <v>575</v>
       </c>
       <c r="O28" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="P28" s="23">
         <v>0</v>
       </c>
       <c r="Q28" s="23" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
@@ -18646,24 +18039,24 @@
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="L31" s="22" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="M31" s="23">
         <v>0</v>
       </c>
       <c r="N31" s="23" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="L32" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="M32" s="23">
         <v>1</v>
       </c>
       <c r="N32" s="23" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating spreadsheet to handle city db and updating urban building type measure to better accommodate residential multifamily.
</commit_message>
<xml_diff>
--- a/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
+++ b/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="240" windowWidth="15360" windowHeight="7755" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="300" windowWidth="15360" windowHeight="7695" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="797">
   <si>
     <t>type</t>
   </si>
@@ -2077,18 +2077,6 @@
     <t>UrbanGeometryCreation</t>
   </si>
   <si>
-    <t>city_json_path</t>
-  </si>
-  <si>
-    <t>City JSON Path</t>
-  </si>
-  <si>
-    <t>building_id</t>
-  </si>
-  <si>
-    <t>Building ID</t>
-  </si>
-  <si>
     <t>UrbanBuildingType</t>
   </si>
   <si>
@@ -2101,9 +2089,6 @@
     <t>discrete</t>
   </si>
   <si>
-    <t>|'142484','116245','142872','43254','1459','134032','143122','15204','155513','181948','142238','191582','185054','208359','113178','192702','236371','190013','6434','231850','128469','172662','222162','122347','158690','202694','56659','85635','3571','83186','227340','41962','217309','52660','161648','184642','3847','2373','62625','65373','58283','58911','237783','79514','110389','144568','5955','78754','96419','83574','223270','148046','191859','33879','52936','106804','221612','61663','207542','213989','49369','116055','151927','8514','100535','187338','207180','50936','11886','20763','230376','134949','151680','152016','164646','206572','178897','181797','183160','206869','187675','200594','222412','223723','233024','234608','235990','240241','203425','186746','215740','227893','230795','147716','150821','151683','155087','173389','208781','221871','236646','134575','138298','141692','146223','147538','148715','154723','155770','159371','166226','166447','185614','190700','200435','203431','209303','211686','225506','226857','231874','236181','134829','153445','188330','195998','215567','236722','240378','136118','144038','145786','156369','160789','166893','177498','184217','197688','212943','223606','224837','225080','228898','229908','234747','236146','236944','139179','140483','141333','141742','149927','150157','153100','157664','160763','164828','165203','166177','167379','169768','170121','170176','171097','172136','172760','174951','176543','188603','188635','192839','194021','194266','196939','199268','207526','207791','209874','210350','216983','219655','221577','225998','231823','233786','139210','139560','140971','148938','153385','156024','156566','157189','161540','162805','165776','181190','183554','184555','185691','187767','192580','196291','200692','203271','205426','209161','212361','212521','214551','220751','221103','222785','226178','234948','236366','238464','140303','155940','171027','184033','193357','206646','228561','240057','158140','159829','168276','181627','181985','194704','199802','200515','214462','220549','224670','231114','231559','238379','239180','139056','146495','160004','163839','170485','174902','176024','181799','188941','190575','192751','195570','212682','215390','222246','227246','232402','233696','238260','238366','138674','140217','149213','151733','155395','156878','157846','182991','197481','200860','204224','212394','215129','151466','157857','205201','208419','222958','224064','238013','142841','145861','145877','146423','165161','166962','171677','197554','199848','218849','219161','221310','234670','235539','239758','136089','138309','139280','139552','139972','140112','141291','145092','146832','147765','148030','149426','151459','151615','153585','154644','155425','156031','162031','158373','161939','163262','164664','168617','169885','169922','171070','173586','177972','178711','179427','179543','181848','183383','186074','186323','186484','186645','188930','189510','194658','197850','198151','204452','208462','210041','210801','211161','213948','214599','217006','220057','222119','229206','229762','236497','237377','240264','139906','142689','144492','161710','171251','173347','182732','199171','199748','218496','157559','161139','162145','175894','177668','179093','191030','211557','217141','218850','140479','152927','154431','154464','159986','179970','179999','184576','180201','187575','189920','190567','192647','207120','208849','212153','214562','218163','229721','229883','230166','233318','235390','135669','136042','146188','146794','150655','155019','159866','160735','164404','165424','172541','186414','176530','178186','181487','185242','190676','193814','196736','206032','212641','224220','224416','225635','233901','234701','237931','138231','141323','144648','145555','150780','150899','152839','156034','156206','157204','163155','164382','164577','166037','167180','171781','172656','175940','176083','176527','177893','179370','179380','180506','180928','181312','186261','186821','188752','188829','192028','192253','195430','196757','197324','204858','202564','203048','209777','209943','211983','215123','215882','217903','219176','227481','232103','234356','239047','144314','152718','161890','173232','184010','185603','189087','192262','195632','202699','223098','223836','224922','229421','140000','140062','168535','175315','179702','193716','211405','226429','212193','229689','156794','159799','163819','179634','181429','190947','205996','211049','224660','134586','140179','140897','148743','148792','153916','155447','161638','161681','163049','163218','186378','169820','177857','178398','182872','183800','188456','191281','191863','194747','199020','201060','205442','210315','214715','217037','218199','228236','229366','230278','230745','238378','238645','141358','141807','146429','151549','163349','159431','163012','176825','178193','189427','189930','191574','194472','196651','199478','205863','225950','231182','146349','161436','187104','191021','191734','194086','197836','203209','230430','136919','147914','150225','151174','151776','166433','170224','177521','185308','192052','200711','206227','210308','222863','222913','231145','236127','137197','140158','146957','148680','158508','167413','181146','188059','195832','215406','219282','221742','228771','230227','233235','137687','139905','148683','153540','154931','160185','161507','168943','175576','190299','194794','211649','213228','218327','227520','137733','143531','145229','152035','156082','162358','162560','166563','167482','174906','177785','179581','181727','184831','187591','188181','192875','197918','203955','205171','206049','211102','211511','140460','182042','185846','186059','194978','202325','207738','210823','213539','224910','143750','146664','157155','171037','185610','214994','222640','236462','135958','145554','152220','154793','155394','157781','173632','179192','190668','186750','191225','206920','218691','219325','221114','135888','137520','140523','142060','144519','145787','146424','147199','147684','154270','160406','161101','161838','163303','163875','164094','164561','166429','168479','168736','169732','172313','172383','175207','176225','178036','182775','186511','187648','188736','190841','194156','195367','195774','204083','210774','212113','214198','216378','218821','220433','232024','232440','235333','236582','239376','200511','200703','216368','216854','220985','221684','221834','221849','222135','223137','223721','224158','224504','226166','226297','226695','229251','230716','230761','234635','234895','235308','236196','237124','237960','238930','239976','240032','122105','168573','96922','144185','151931','156986','190213','217362','164013','104780','121861','167901','184630','124937','185146','193248','195079','77300','80971','86658','131929','204467','143637','203758','81361','106807','80313','131985','159184','212516','219061','143680','199109','200379','210667','213357','88336','90589','160050','187722','190416','196196','216274','108357','158067','191814','209748','218028','168409','88808','91652','107419','120394','130934','176535','186299','215284','72338','150378','155290','156516','157947','216010','219839','96387','103082','120734','122770','146527','147644','184966','107876','175298','184668','149130','150004','156304','174164','189171','84614','88533','90706','156563','179208','199464','80947','84283','85985','96257','101054','108605','122529','133615','137288','152785','169737','172060','218831','219358','83489','92916','108429','117211','119645','150610','149445','170454','184703','189645','190838','191674','214057','92414','115798','119426','128986','140277','154095','155957','160911','181632','126037','142972','305','557','784','3098','3672','4208','6537','7626','8122','9776','13779','16415','17391','17442','17741','18019','18138','20033','22734','23111','25358','26767','27364','27864','29168','30409','34851','35629','40383','37821','37934','38939','41644','42197','42305','42734','43507','43919','44444','44863','47006','47204','48052','59307','50573','53776','57248','58083','58533','62498','64663','65211','65916','66016','66723','67740','70467','73642','77256','78947','78958','79333','80104','80443','80717','81835','82425','82968','84578','87717','91015','91765','93806','96354','99101','99674','99978','103749','103853','104550','104801','105053','105736','105868','110303','110562','111378','111785','114642','117175','118705','123784','127336','127500','128766','129848','132134','132751','132950','133166','133776','131234','3671','4081','135435','12530','14875','25798','27308','30244','36571','41743','43437','44422','50607','55895','60525','66798','68600','68660','80402','82849','84693','92321','96066','107805','113252','116607','124001','130014','133034','132020','133819','1614','9787','15251','16859','18125','18253','21029','22044','24430','25821','30558','35912','39172','43686','44759','48274','48348','48952','49643','52210','55580','56230','56407','57930','57995','63830','65413','138646','71351','77608','102025','83878','84727','85039','89242','90596','91378','93895','94043','100388','101217','105518','106584','108694','111679','115046','114720','115805','118622','118763','119139','124080','128823','131551','132161','132761','132835','968','2145','2916','3901','7554','8131','8405','8875','9938','11008','11260','11633','14409','23443','27408','28907','29640','37909','38528','40120','60775','41112','42345','43161','44010','45630','46261','48335','54169','56205','57845','62892','65927','71052','72573','72609','72949','74596','74997','76347','77748','77875','78079','78374','79904','80019','80515','80904','81473','84188','102028','85108','92610','96690','98837','102417','103518','106075','106994','107133','107743','108418','109053','111513','114441','152173','120001','120466','124740','127774','129389','131553','133568','142275','128616','132155','124431','1835','4852','5970','5985','6412','6955','7065','7703','8979','9049','9917','10941','11426','13336','15743','15897','16700','17972','19474','21410','22635','23082','27277','29120','30449','31299','36733','37519','37960','38880','39273','43509','46157','46514','46973','50361','51850','53952','54531','57203','58449','62391','62627','62868','63596','138384','65272','67241','68865','69075','72535','73049','74789','75400','77048','79462','81655','86241','88606','88789','89145','89600','92602','94657','94900','95113','102086','95695','96505','100305','100408','100617','100621','100751','103105','105168','105373','105472','106890','110314','110661','111108','111294','112819','113515','117619','119304','120316','120521','120528','120659','124907','126403','129765','131946','132840','153878','5','803','2639','5453','5594','129144','8608','8891','11318','12098','12783','17960','18400','18679','20839','23247','23479','23920','25659','26382','28634','31791','33691','36559','37647','37686','38127','38824','38946','40172','43126','44441','45829','46984','47544','49109','49486','52170','128455','57399','58303','63100','63763','64448','64981','65895','128047','66289','67269','67319','69236','70023','71428','71681','74427','75660','75870','76389','77814','78152','81308','80554','127991','82858','83539','84011','88645','89138','89758','92226','94088','95964','97567','98652','100307','101113','102703','104239','105170','106108','106842','106907','109530','110458','114806','114884','114941','115031','116830','118122','120000','121285','9024','128624','129618','130084','132992','2029','2594','3371','6931','7325','8446','8837','10917','12757','13544','14020','17641','17956','19344','21647','22075','39354','24708','24967','29565','29572','30608','31214','32653','33914','34278','36147','38435','41529','44877','47239','48848','48908','51292','52433','52552','52699','52792','54130','56588','57681','58385','58941','59934','127472','60452','127483','65780','66892','67721','69590','69747','69880','70898','72508','74337','78317','79008','81699','82051','82348','83068','84196','86674','89038','90018','91299','92325','125673','93518','125382','98274','125485','99009','101785','102137','103741','104396','105700','108474','110143','110357','111635','111934','114266','114681','114932','115534','115558','115652','117848','118484','119292','119814','120456','120690','120792','120862','122837','135325','127676','130746','131123','128759','147482','410','5228','5975','6468','8136','13556','16203','20203','20467','21150','21907','22013','26278','27384','28663','30270','31941','32840','34162','34185','36119','36564','37307','39104','40441','40582','40730','42225','43182','165199','44991','45563','47205','47802','47968','48521','49230','50162','50277','50444','51280','52168','52448','52481','56748','56800','58053','59263','62004','62247','129542','67862','69687','71172','71990','72411','76910','77416','77546','77682','77727','78398','79894','80675','80810','80992','82166','83753','85062','86962','92315','92427','92523','92902','95432','95584','95785','97993','100258','100690','102284','105619','106758','107672','108087','109880','110472','111717','112523','112736','113947','113997','115209','122112','124359','14836','125933','127753','128203','132010','133802','124746','133064','702','993','6457','21267','10924','13381','13702','14265','15358','17782','23246','136398','27031','27425','28252','28150','30523','32050','32794','34635','37771','42823','43177','44655','44946','50684','51410','52005','54919','57085','57408','58220','60140','61380','63650','65512','65768','66317','66554','69854','72617','78633','79523','81468','81491','83427','91756','96136','96855','97081','100090','102016','102598','104110','105600','108651','110916','112024','112880','115349','118644','120519','120620','125661','127864','133420','133679','128793','142913','695','1246','2337','2381','5433','6404','9099','12276','12445','15932','16437','18599','18694','19546','23452','24768','24853','25034','27398','29763','30553','30873','31089','32097','33330','35456','36250','38608','39878','39971','43997','44686','46746','48757','49548','51685','53099','55437','56752','57444','60121','60700','61369','62358','62488','65092','66489','68384','70108','71437','72317','73435','73473','73739','77910','79614','79642','79938','81816','85132','86501','125627','92088','94531','96151','97450','97565','98395','98685','99514','100416','102728','103441','104698','104791','106740','110263','114814','117587','118545','121913','122957','124070','44859','124737','125596','127468','129489','131601','132011','132164','132591','133995','491','1399','2081','2862','3644','8115','8243','10811','11263','11424','11719','11796','13725','15619','16293','16539','17174','17205','18091','20814','22654','22827','24036','24600','25372','25896','26193','31569','31609','34670','35309','36605','37242','38197','39556','41210','43805','45478','46290','49485','137039','52305','53306','55623','61885','62154','66046','68178','68628','138866','72758','73840','73874','76640','76899','76986','79001','82142','82154','84763','87844','88049','90041','96272','96322','96382','97760','151361','103104','104357','107505','109315','140742','111571','113776','118599','121132','122174','122645','124115','125147','130751','130878','131980','133071','19139','7261','14110','21560','22495','26053','30648','33822','56583','60119','66404','70003','152800','6606','8501','9780','10791','18497','31565','31907','33368','34016','152742','128863','3339','4710','33487','33792','46435','133428','13178','26532','32979','15772','16282','51793','57564','6748','16936','3677','41404','5822','33857','49341','2304','19946','24390','24511','25682','27128','29635','30854','39651','40001','60083','17282','6692','16854','57771','58654','31013','66104','34221','12254','1699','205556','228564','307','55322','63500','135226','74906','25543','79455','8943','13840','63758','126538','39978','42682','103425','103524','84214','150486','160656','171007','209726','218420','219742','239709','125991','10377','28083','37582','77648','79389','99671','130006','154107','156027','161958','166132','210035','235727','218240','123749','5478','137832','35344','187863','206624','43631','72385','169785','191531','55395','81857','84341','123836','57050','128123','101599','200268','94207','113663','152212','143036','3114','36257','49550','123115','147724','230563','64794','98026','124601','153827','199381','211130'|</t>
-  </si>
-  <si>
     <t>standard_report_legacy.total_energy</t>
   </si>
   <si>
@@ -2113,21 +2098,9 @@
     <t>../../../openstudio-urban-measures</t>
   </si>
   <si>
-    <t>Directory</t>
-  </si>
-  <si>
-    <t>city_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ../../../lib/city_data/city.json</t>
-  </si>
-  <si>
     <t>empty</t>
   </si>
   <si>
-    <t>../../urban_geometry_creation/tests</t>
-  </si>
-  <si>
     <t>SetResidentialEPWFile</t>
   </si>
   <si>
@@ -2230,9 +2203,6 @@
     <t>../weather/USA_CO_Denver.Intl.AP.725650_TMY3.epw</t>
   </si>
   <si>
-    <t>../weather/USA_CO_Denver.Intl.AP.725650_TMY3.ddy</t>
-  </si>
-  <si>
     <t>URBANopt Testing 1</t>
   </si>
   <si>
@@ -2332,18 +2302,6 @@
     <t>heating_source</t>
   </si>
   <si>
-    <t>Electric</t>
-  </si>
-  <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>|'Electric','District Chilled Water','District Ambient Water'|</t>
-  </si>
-  <si>
-    <t>|'Gas','Electric','District Hot Water','District Ambient Water'|</t>
-  </si>
-  <si>
     <t>['Electric','District Chilled Water','District Ambient Water']</t>
   </si>
   <si>
@@ -2356,25 +2314,118 @@
     <t>District Heating</t>
   </si>
   <si>
-    <t>142484'</t>
-  </si>
-  <si>
     <t>standard_reports.district_cooling_ip</t>
   </si>
   <si>
     <t>standard_reports.district_heating_ip</t>
   </si>
   <si>
-    <t>['142484','116245','113178']</t>
-  </si>
-  <si>
     <t>Bldg Use</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>urbangeometrycreation.bldg_use</t>
+    <t>City Database Url</t>
+  </si>
+  <si>
+    <t>city_db_url</t>
+  </si>
+  <si>
+    <t>http://insight4.hpc.nrel.gov:8081/</t>
+  </si>
+  <si>
+    <t>Building Source ID</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
+  <si>
+    <t>Building Source Name</t>
+  </si>
+  <si>
+    <t>source_name</t>
+  </si>
+  <si>
+    <t>NREL_GDS</t>
+  </si>
+  <si>
+    <t>Surrounding Buildings</t>
+  </si>
+  <si>
+    <t>surrounding_buildings</t>
+  </si>
+  <si>
+    <t>ShadingOnly</t>
+  </si>
+  <si>
+    <t>urbanbuildingtype.bldg_use</t>
+  </si>
+  <si>
+    <t>Res Units</t>
+  </si>
+  <si>
+    <t>urbanbuildingtype.res_units</t>
+  </si>
+  <si>
+    <t>225950'</t>
+  </si>
+  <si>
+    <t>|'102472', '102905', '108457', '114115', '114593', '119747', '119764', '119928', '12349', '12442', '13365', '133769', '133781', '134009', '13466', '135497', '149555', '150017', '150020', '150541', '150543', '157313', '157798', '158279', '159300', '15988', '165544', '165761', '165781', '166541', '166560', '166737', '166767', '17337', '173534', '174739', '175015', '181740', '181756', '182026', '183490', '184411', '190972', '190985', '191878', '192072', '192075', '200149', '200333', '200348', '201831', '20584', '207895', '21002', '2101', '214904', '215387', '21569', '215879', '216067', '225234', '234485', '235095', '238995', '239535', '239556', '239990', '239991', '249839', '2541', '2567', '259114', '273275', '277313', '277515', '281665', '283782', '30020', '30133', '31582', '38811', '39344', '43911', '46468', '48527', '49478', '49479', '49520', '58111', '58121', '59570', '61651', '62712', '63102', '71281', '71285', '74835', '76846', '79584', '81044', '81046', '83538', '85007', '85057', '89025', '8907', '9315', '9319', '97840'|</t>
+  </si>
+  <si>
+    <t>['102472', '102905', '108457', '114115', '114593', '119747', '119764', '119928', '12349', '12442', '13365', '133769', '133781', '134009', '13466', '135497', '149555', '150017', '150020', '150541', '150543', '157313', '157798', '158279', '159300', '15988', '165544', '165761', '165781', '166541', '166560', '166737', '166767', '17337', '173534', '174739', '175015', '181740', '181756', '182026', '183490', '184411', '190972', '190985', '191878', '192072', '192075', '200149', '200333', '200348', '201831', '20584', '207895', '21002', '2101', '214904', '215387', '21569', '215879', '216067', '225234', '234485', '235095', '238995', '239535', '239556', '239990', '239991', '249839', '2541', '2567', '259114', '273275', '277313', '277515', '281665', '283782', '30020', '30133', '31582', '38811', '39344', '43911', '46468', '48527', '49478', '49479', '49520', '58111', '58121', '59570', '61651', '62712', '63102', '71281', '71285', '74835', '76846', '79584', '81044', '81046', '83538', '85007', '85057', '89025', '8907', '9315', '9319', '97840']</t>
+  </si>
+  <si>
+    <t>|'NA','Electric','District Chilled Water','District Ambient Water'|</t>
+  </si>
+  <si>
+    <t>|'NA','Gas','Electric','District Hot Water','District Ambient Water'|</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Has Basement</t>
+  </si>
+  <si>
+    <t>urbanbuildingtype.has_basement</t>
+  </si>
+  <si>
+    <t>Num Spaces</t>
+  </si>
+  <si>
+    <t>urbanbuildingtype.num_spaces</t>
+  </si>
+  <si>
+    <t>Units Per Space</t>
+  </si>
+  <si>
+    <t>urbanbuildingtype.units_per_space</t>
+  </si>
+  <si>
+    <t>|'11886','5594','993','8446','13702','18400','23920','27364','28634','38939','80717','42197','46984','80443','65895','67721','69590','78152','78633','79523','84214','99009','100307','104110','115652','120456','127864','129618','129848','135226','138231','147538','156024','162805','168535','171097','183800','209726','228898','43631','8979','30608','23111','5453','64981','23247','28150','31791','33691','52792','38946','40172','44863','49486','50684','55395','103105','93806','59934','66016','66317','74427','80554','87717','239709','98274','97081','103425','114806','117848','118122','120862','126037','127336','127483','131123','139210','140483','140897','141291','141742','150899','153445','164828','170121','172760','177857','192028','205426','3901','229908','234356','305','2639','6537','8131','8875','9776','9938','10941','11633','13336','46514','17741','17972','18019','18679','20033','23443','60775','118622','27277','29640','28907','29120','29572','37582','42345','43161','43919','44877','46157','46261','46973','100617','57930','67269','48952','54130','82051','71681','54169','56588','59307','120001','72385','62868','62892','62627','74596','82858','75400','75660','77648','89600','77748','77875','78374','79389','81655','218420','105736','89138','92602','93518','93895','94900','100388','102028','120316','102086','104396','106994','110562','110916','111785','113515','117619','115031','210801','120000','204083','120466','121285','126538','223137','127991','128624','132020','148938','211161','129765','130006','132161','156034','133568','134829','156027','172656','139179','139552','142060','146349','146832','147199','151615','154107','155770','159431','181190','161101','161838','163012','163262','182775','240378','163303','164561','165203','168617','178398','179543','183383','186511','187104','191531','191734','231823','197836','200692','202564','209303','210041','212113','235727','217141','218850','219742','237124','237377','154931','35344','1614','491','15251','16539','22654','22044','31609','34670','35912','57995','97760','104357','106584','124080','139905','148683','225950','238930','177785','190299','194472','196651','203955','212394','218327','240032','237960','191582','222162','83186','58911','79514','192702'|</t>
+  </si>
+  <si>
+    <t>['11886','5594','993','8446','13702','18400','23920','27364','28634','38939','80717','42197','46984','80443','65895','67721','69590','78152','78633','79523','84214','99009','100307','104110','115652','120456','127864','129618','129848','135226','138231','147538','156024','162805','168535','171097','183800','209726','228898','43631','8979','30608','23111','5453','64981','23247','28150','31791','33691','52792','38946','40172','44863','49486','50684','55395','103105','93806','59934','66016','66317','74427','80554','87717','239709','98274','97081','103425','114806','117848','118122','120862','126037','127336','127483','131123','139210','140483','140897','141291','141742','150899','153445','164828','170121','172760','177857','192028','205426','3901','229908','234356','305','2639','6537','8131','8875','9776','9938','10941','11633','13336','46514','17741','17972','18019','18679','20033','23443','60775','118622','27277','29640','28907','29120','29572','37582','42345','43161','43919','44877','46157','46261','46973','100617','57930','67269','48952','54130','82051','71681','54169','56588','59307','120001','72385','62868','62892','62627','74596','82858','75400','75660','77648','89600','77748','77875','78374','79389','81655','218420','105736','89138','92602','93518','93895','94900','100388','102028','120316','102086','104396','106994','110562','110916','111785','113515','117619','115031','210801','120000','204083','120466','121285','126538','223137','127991','128624','132020','148938','211161','129765','130006','132161','156034','133568','134829','156027','172656','139179','139552','142060','146349','146832','147199','151615','154107','155770','159431','181190','161101','161838','163012','163262','182775','240378','163303','164561','165203','168617','178398','179543','183383','186511','187104','191531','191734','231823','197836','200692','202564','209303','210041','212113','235727','217141','218850','219742','237124','237377','154931','35344','1614','491','15251','16539','22654','22044','31609','34670','35912','57995','97760','104357','106584','124080','139905','148683','225950','238930','177785','190299','194472','196651','203955','212394','218327','240032','237960','191582','222162','83186','58911','79514','192702']</t>
+  </si>
+  <si>
+    <t>spaces</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>bldgtype</t>
+  </si>
+  <si>
+    <t>unitsperspace</t>
+  </si>
+  <si>
+    <t>Below Ground Stories</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>urbangeometrycreation.below_ground_stories</t>
   </si>
 </sst>
 </file>
@@ -4056,7 +4107,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4174,12 +4225,14 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5983,10 +6036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6035,7 +6088,7 @@
         <v>457</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>726</v>
+        <v>717</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>458</v>
@@ -6157,7 +6210,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>472</v>
@@ -6168,7 +6221,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>612</v>
@@ -6511,79 +6564,58 @@
         <v>28</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>731</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="44" t="s">
+      <c r="B42" s="44" t="s">
         <v>454</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>613</v>
       </c>
-      <c r="E43" s="6"/>
-      <c r="F43" s="8" t="s">
+      <c r="E42" s="6"/>
+      <c r="F42" s="8" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="17" t="s">
-        <v>695</v>
-      </c>
-      <c r="C44" s="14" t="s">
+      <c r="B43" s="17" t="s">
+        <v>687</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D44" s="23" t="s">
-        <v>690</v>
-      </c>
-      <c r="F44" s="2" t="s">
+      <c r="D43" s="23" t="s">
+        <v>685</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+    <row r="45" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B45" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>614</v>
       </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="8" t="s">
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="8" t="s">
         <v>610</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="B47" s="18" t="s">
-        <v>693</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -6617,9 +6649,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z58"/>
+  <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6673,14 +6707,14 @@
       <c r="R1" s="33"/>
       <c r="S1" s="30"/>
       <c r="T1" s="30"/>
-      <c r="U1" s="61" t="s">
+      <c r="U1" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
@@ -6796,7 +6830,7 @@
       </c>
       <c r="Z3" s="35"/>
     </row>
-    <row r="4" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="b">
         <v>1</v>
       </c>
@@ -6804,7 +6838,7 @@
         <v>679</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="D4" s="39" t="s">
         <v>679</v>
@@ -6834,43 +6868,43 @@
       <c r="Y4" s="39"/>
       <c r="Z4" s="39"/>
     </row>
-    <row r="5" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15" t="s">
-        <v>681</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>680</v>
-      </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15" t="s">
+    <row r="5" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="46"/>
+      <c r="B5" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46" t="s">
+        <v>762</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>763</v>
+      </c>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15" t="s">
-        <v>694</v>
-      </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="59" t="s">
+        <v>764</v>
+      </c>
+      <c r="J5" s="46"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="46"/>
     </row>
     <row r="6" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="42"/>
@@ -6879,10 +6913,10 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
-        <v>683</v>
+        <v>765</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>682</v>
+        <v>766</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="42" t="s">
@@ -6890,10 +6924,10 @@
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="45" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
       <c r="J6" s="42" t="s">
-        <v>688</v>
+        <v>777</v>
       </c>
       <c r="K6" s="43">
         <v>0</v>
@@ -6910,12 +6944,12 @@
       <c r="O6" s="43">
         <v>0</v>
       </c>
-      <c r="P6" s="64" t="s">
-        <v>776</v>
+      <c r="P6" s="42" t="s">
+        <v>778</v>
       </c>
       <c r="Q6" s="43"/>
       <c r="R6" s="42" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="S6" s="42"/>
       <c r="T6" s="42"/>
@@ -6926,665 +6960,599 @@
       <c r="Y6" s="42"/>
       <c r="Z6" s="42"/>
     </row>
-    <row r="7" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="b">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>679</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>681</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>679</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="39"/>
+      <c r="X9" s="39"/>
+      <c r="Y9" s="39"/>
+      <c r="Z9" s="39"/>
+    </row>
+    <row r="10" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="46"/>
+      <c r="B10" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46" t="s">
+        <v>762</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>763</v>
+      </c>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="46"/>
+      <c r="I10" s="59" t="s">
+        <v>764</v>
+      </c>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="46"/>
+      <c r="U10" s="46"/>
+      <c r="V10" s="46"/>
+      <c r="W10" s="46"/>
+      <c r="X10" s="46"/>
+      <c r="Y10" s="46"/>
+      <c r="Z10" s="46"/>
+    </row>
+    <row r="11" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="42"/>
+      <c r="B11" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42" t="s">
+        <v>765</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>766</v>
+      </c>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="42"/>
+      <c r="I11" s="45" t="s">
+        <v>776</v>
+      </c>
+      <c r="J11" s="42" t="s">
+        <v>788</v>
+      </c>
+      <c r="K11" s="43">
+        <v>0</v>
+      </c>
+      <c r="L11" s="43">
+        <v>0</v>
+      </c>
+      <c r="M11" s="43">
+        <v>0</v>
+      </c>
+      <c r="N11" s="43">
+        <v>0</v>
+      </c>
+      <c r="O11" s="43">
+        <v>0</v>
+      </c>
+      <c r="P11" s="42" t="s">
+        <v>789</v>
+      </c>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="42" t="s">
+        <v>683</v>
+      </c>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="42"/>
+      <c r="V11" s="42"/>
+      <c r="W11" s="42"/>
+      <c r="X11" s="42"/>
+      <c r="Y11" s="42"/>
+      <c r="Z11" s="42"/>
+    </row>
+    <row r="12" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>767</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>768</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>769</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>770</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>771</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>772</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>688</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>688</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>688</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="48"/>
+      <c r="U14" s="48"/>
+      <c r="V14" s="48"/>
+      <c r="W14" s="48"/>
+      <c r="X14" s="48"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="48"/>
+    </row>
+    <row r="15" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="46"/>
+      <c r="B15" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46" t="s">
+        <v>691</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>689</v>
+      </c>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46" t="s">
+        <v>693</v>
+      </c>
+      <c r="J15" s="46"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="46"/>
+      <c r="S15" s="46"/>
+      <c r="T15" s="46"/>
+      <c r="U15" s="46"/>
+      <c r="V15" s="46"/>
+      <c r="W15" s="46"/>
+      <c r="X15" s="46"/>
+      <c r="Y15" s="46"/>
+      <c r="Z15" s="46"/>
+    </row>
+    <row r="16" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="46"/>
+      <c r="B16" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46" t="s">
+        <v>692</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>690</v>
+      </c>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46" t="s">
+        <v>720</v>
+      </c>
+      <c r="J16" s="46"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="46"/>
+      <c r="S16" s="46"/>
+      <c r="T16" s="46"/>
+      <c r="U16" s="46"/>
+      <c r="V16" s="46"/>
+      <c r="W16" s="46"/>
+      <c r="X16" s="46"/>
+      <c r="Y16" s="46"/>
+      <c r="Z16" s="46"/>
+    </row>
+    <row r="17" spans="1:26" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>680</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>682</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>680</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="39"/>
+      <c r="T17" s="39"/>
+      <c r="U17" s="39"/>
+      <c r="V17" s="39"/>
+      <c r="W17" s="39"/>
+      <c r="X17" s="39"/>
+      <c r="Y17" s="39"/>
+      <c r="Z17" s="39"/>
+    </row>
+    <row r="18" spans="1:26" s="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="61"/>
+      <c r="B18" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61" t="s">
+        <v>751</v>
+      </c>
+      <c r="E18" s="61" t="s">
+        <v>753</v>
+      </c>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="61"/>
+      <c r="I18" s="64" t="s">
+        <v>781</v>
+      </c>
+      <c r="J18" s="61" t="s">
+        <v>779</v>
+      </c>
+      <c r="K18" s="61">
+        <v>0</v>
+      </c>
+      <c r="L18" s="61">
+        <v>0</v>
+      </c>
+      <c r="M18" s="61">
+        <v>0</v>
+      </c>
+      <c r="N18" s="61">
+        <v>0</v>
+      </c>
+      <c r="O18" s="61">
+        <v>0</v>
+      </c>
+      <c r="P18" s="61" t="s">
+        <v>755</v>
+      </c>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61" t="s">
+        <v>683</v>
+      </c>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="61"/>
+      <c r="V18" s="61"/>
+      <c r="W18" s="61"/>
+      <c r="X18" s="61"/>
+      <c r="Y18" s="61"/>
+      <c r="Z18" s="61"/>
+    </row>
+    <row r="19" spans="1:26" s="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="61"/>
+      <c r="B19" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61" t="s">
+        <v>752</v>
+      </c>
+      <c r="E19" s="61" t="s">
+        <v>754</v>
+      </c>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="61"/>
+      <c r="I19" s="64" t="s">
+        <v>781</v>
+      </c>
+      <c r="J19" s="61" t="s">
+        <v>780</v>
+      </c>
+      <c r="K19" s="61">
+        <v>0</v>
+      </c>
+      <c r="L19" s="61">
+        <v>0</v>
+      </c>
+      <c r="M19" s="61">
+        <v>0</v>
+      </c>
+      <c r="N19" s="61">
+        <v>0</v>
+      </c>
+      <c r="O19" s="61">
+        <v>0</v>
+      </c>
+      <c r="P19" s="61" t="s">
+        <v>756</v>
+      </c>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="61" t="s">
+        <v>683</v>
+      </c>
+      <c r="S19" s="61"/>
+      <c r="T19" s="61"/>
+      <c r="U19" s="61"/>
+      <c r="V19" s="61"/>
+      <c r="W19" s="61"/>
+      <c r="X19" s="61"/>
+      <c r="Y19" s="61"/>
+      <c r="Z19" s="61"/>
+    </row>
+    <row r="20" spans="1:26" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="B7" s="48" t="s">
-        <v>697</v>
-      </c>
-      <c r="C7" s="48" t="s">
-        <v>697</v>
-      </c>
-      <c r="D7" s="48" t="s">
-        <v>697</v>
-      </c>
-      <c r="E7" s="48" t="s">
+      <c r="B20" s="50" t="s">
+        <v>718</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>719</v>
+      </c>
+      <c r="D20" s="50" t="s">
+        <v>718</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48"/>
+      <c r="W20" s="48"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+    </row>
+    <row r="21" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="51" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21" s="52" t="s">
+        <v>723</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>724</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>724</v>
+      </c>
+      <c r="E21" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="49"/>
-      <c r="R7" s="48"/>
-      <c r="S7" s="48"/>
-      <c r="T7" s="48"/>
-      <c r="U7" s="48"/>
-      <c r="V7" s="48"/>
-      <c r="W7" s="48"/>
-      <c r="X7" s="48"/>
-      <c r="Y7" s="48"/>
-      <c r="Z7" s="48"/>
-    </row>
-    <row r="8" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46" t="s">
-        <v>700</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>698</v>
-      </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46" t="s">
-        <v>702</v>
-      </c>
-      <c r="J8" s="46"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="46"/>
-      <c r="W8" s="46"/>
-      <c r="X8" s="46"/>
-      <c r="Y8" s="46"/>
-      <c r="Z8" s="46"/>
-    </row>
-    <row r="9" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46" t="s">
-        <v>701</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>699</v>
-      </c>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46" t="s">
-        <v>729</v>
-      </c>
-      <c r="J9" s="46"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="46"/>
-      <c r="U9" s="46"/>
-      <c r="V9" s="46"/>
-      <c r="W9" s="46"/>
-      <c r="X9" s="46"/>
-      <c r="Y9" s="46"/>
-      <c r="Z9" s="46"/>
-    </row>
-    <row r="10" spans="1:26" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>684</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>686</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>684</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="39"/>
-      <c r="T10" s="39"/>
-      <c r="U10" s="39"/>
-      <c r="V10" s="39"/>
-      <c r="W10" s="39"/>
-      <c r="X10" s="39"/>
-      <c r="Y10" s="39"/>
-      <c r="Z10" s="39"/>
-    </row>
-    <row r="11" spans="1:26" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
-      <c r="B11" s="62" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62" t="s">
-        <v>761</v>
-      </c>
-      <c r="E11" s="62" t="s">
-        <v>763</v>
-      </c>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62" t="s">
-        <v>765</v>
-      </c>
-      <c r="J11" s="62" t="s">
-        <v>767</v>
-      </c>
-      <c r="K11" s="62">
-        <v>0</v>
-      </c>
-      <c r="L11" s="62">
-        <v>0</v>
-      </c>
-      <c r="M11" s="62">
-        <v>0</v>
-      </c>
-      <c r="N11" s="62">
-        <v>0</v>
-      </c>
-      <c r="O11" s="62">
-        <v>0</v>
-      </c>
-      <c r="P11" s="62" t="s">
-        <v>769</v>
-      </c>
-      <c r="Q11" s="62"/>
-      <c r="R11" s="62" t="s">
-        <v>687</v>
-      </c>
-      <c r="S11" s="62"/>
-      <c r="T11" s="62"/>
-      <c r="U11" s="62"/>
-      <c r="V11" s="62"/>
-      <c r="W11" s="62"/>
-      <c r="X11" s="62"/>
-      <c r="Y11" s="62"/>
-      <c r="Z11" s="62"/>
-    </row>
-    <row r="12" spans="1:26" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
-      <c r="B12" s="62" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62" t="s">
-        <v>762</v>
-      </c>
-      <c r="E12" s="62" t="s">
-        <v>764</v>
-      </c>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62" t="s">
-        <v>766</v>
-      </c>
-      <c r="J12" s="62" t="s">
-        <v>768</v>
-      </c>
-      <c r="K12" s="62">
-        <v>0</v>
-      </c>
-      <c r="L12" s="62">
-        <v>0</v>
-      </c>
-      <c r="M12" s="62">
-        <v>0</v>
-      </c>
-      <c r="N12" s="62">
-        <v>0</v>
-      </c>
-      <c r="O12" s="62">
-        <v>0</v>
-      </c>
-      <c r="P12" s="62" t="s">
-        <v>770</v>
-      </c>
-      <c r="Q12" s="62"/>
-      <c r="R12" s="62" t="s">
-        <v>687</v>
-      </c>
-      <c r="S12" s="62"/>
-      <c r="T12" s="62"/>
-      <c r="U12" s="62"/>
-      <c r="V12" s="62"/>
-      <c r="W12" s="62"/>
-      <c r="X12" s="62"/>
-      <c r="Y12" s="62"/>
-      <c r="Z12" s="62"/>
-    </row>
-    <row r="13" spans="1:26" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="B13" s="50" t="s">
-        <v>727</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>728</v>
-      </c>
-      <c r="D13" s="50" t="s">
-        <v>727</v>
-      </c>
-      <c r="E13" s="50" t="s">
-        <v>159</v>
-      </c>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
-      <c r="U13" s="48"/>
-      <c r="V13" s="48"/>
-      <c r="W13" s="48"/>
-      <c r="X13" s="48"/>
-      <c r="Y13" s="48"/>
-      <c r="Z13" s="48"/>
-    </row>
-    <row r="14" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="B14" s="52" t="s">
-        <v>733</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>734</v>
-      </c>
-      <c r="D14" s="52" t="s">
-        <v>734</v>
-      </c>
-      <c r="E14" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="51"/>
-      <c r="T14" s="51"/>
-      <c r="U14" s="51"/>
-      <c r="V14" s="51"/>
-      <c r="W14" s="51"/>
-      <c r="X14" s="51"/>
-      <c r="Y14" s="51"/>
-      <c r="Z14" s="51"/>
-    </row>
-    <row r="15" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="b">
-        <v>0</v>
-      </c>
-      <c r="B15" s="57" t="s">
-        <v>735</v>
-      </c>
-      <c r="C15" s="57" t="s">
-        <v>736</v>
-      </c>
-      <c r="D15" s="57" t="s">
-        <v>736</v>
-      </c>
-      <c r="E15" s="57" t="s">
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="51"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="51"/>
+      <c r="V21" s="51"/>
+      <c r="W21" s="51"/>
+      <c r="X21" s="51"/>
+      <c r="Y21" s="51"/>
+      <c r="Z21" s="51"/>
+    </row>
+    <row r="22" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="57" t="b">
+        <v>0</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>725</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>726</v>
+      </c>
+      <c r="D22" s="57" t="s">
+        <v>726</v>
+      </c>
+      <c r="E22" s="57" t="s">
         <v>232</v>
       </c>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="58"/>
-      <c r="O15" s="58"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="58"/>
-      <c r="S15" s="58"/>
-      <c r="T15" s="58"/>
-      <c r="U15" s="58"/>
-      <c r="V15" s="58"/>
-      <c r="W15" s="58"/>
-      <c r="X15" s="58"/>
-      <c r="Y15" s="58"/>
-      <c r="Z15" s="58"/>
-    </row>
-    <row r="16" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54" t="s">
-        <v>737</v>
-      </c>
-      <c r="E16" s="54" t="s">
-        <v>738</v>
-      </c>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54" t="s">
-        <v>739</v>
-      </c>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="55"/>
-      <c r="R16" s="55"/>
-      <c r="S16" s="55"/>
-      <c r="T16" s="55"/>
-      <c r="U16" s="55"/>
-      <c r="V16" s="55"/>
-      <c r="W16" s="55"/>
-      <c r="X16" s="55"/>
-      <c r="Y16" s="55"/>
-      <c r="Z16" s="55"/>
-    </row>
-    <row r="17" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="57" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17" s="57" t="s">
-        <v>740</v>
-      </c>
-      <c r="C17" s="57" t="s">
-        <v>741</v>
-      </c>
-      <c r="D17" s="57" t="s">
-        <v>742</v>
-      </c>
-      <c r="E17" s="57" t="s">
-        <v>232</v>
-      </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58"/>
-      <c r="O17" s="58"/>
-      <c r="P17" s="58"/>
-      <c r="Q17" s="58"/>
-      <c r="R17" s="58"/>
-      <c r="S17" s="58"/>
-      <c r="T17" s="58"/>
-      <c r="U17" s="58"/>
-      <c r="V17" s="58"/>
-      <c r="W17" s="58"/>
-      <c r="X17" s="58"/>
-      <c r="Y17" s="58"/>
-      <c r="Z17" s="58"/>
-    </row>
-    <row r="18" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
-      <c r="B18" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54" t="s">
-        <v>743</v>
-      </c>
-      <c r="E18" s="54" t="s">
-        <v>744</v>
-      </c>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="59" t="s">
-        <v>745</v>
-      </c>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="55"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="55"/>
-      <c r="P18" s="55"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="55"/>
-      <c r="S18" s="55"/>
-      <c r="T18" s="55"/>
-      <c r="U18" s="55"/>
-      <c r="V18" s="55"/>
-      <c r="W18" s="55"/>
-      <c r="X18" s="55"/>
-      <c r="Y18" s="55"/>
-      <c r="Z18" s="55"/>
-    </row>
-    <row r="19" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
-      <c r="B19" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54" t="s">
-        <v>746</v>
-      </c>
-      <c r="E19" s="54" t="s">
-        <v>747</v>
-      </c>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H19" s="54"/>
-      <c r="I19" s="53" t="s">
-        <v>748</v>
-      </c>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="55"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="55"/>
-      <c r="R19" s="55"/>
-      <c r="S19" s="55"/>
-      <c r="T19" s="55"/>
-      <c r="U19" s="55"/>
-      <c r="V19" s="55"/>
-      <c r="W19" s="55"/>
-      <c r="X19" s="55"/>
-      <c r="Y19" s="55"/>
-      <c r="Z19" s="55"/>
-    </row>
-    <row r="20" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="55"/>
-      <c r="B20" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54" t="s">
-        <v>749</v>
-      </c>
-      <c r="E20" s="54" t="s">
-        <v>750</v>
-      </c>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54" t="s">
-        <v>751</v>
-      </c>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="55"/>
-      <c r="P20" s="55"/>
-      <c r="Q20" s="55"/>
-      <c r="R20" s="55"/>
-      <c r="S20" s="55"/>
-      <c r="T20" s="55"/>
-      <c r="U20" s="55"/>
-      <c r="V20" s="55"/>
-      <c r="W20" s="55"/>
-      <c r="X20" s="55"/>
-      <c r="Y20" s="55"/>
-      <c r="Z20" s="55"/>
-    </row>
-    <row r="21" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="57" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21" s="57" t="s">
-        <v>752</v>
-      </c>
-      <c r="C21" s="57" t="s">
-        <v>753</v>
-      </c>
-      <c r="D21" s="57" t="s">
-        <v>754</v>
-      </c>
-      <c r="E21" s="57" t="s">
-        <v>232</v>
-      </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="58"/>
-      <c r="P21" s="58"/>
-      <c r="Q21" s="58"/>
-      <c r="R21" s="58"/>
-      <c r="S21" s="58"/>
-      <c r="T21" s="58"/>
-      <c r="U21" s="58"/>
-      <c r="V21" s="58"/>
-      <c r="W21" s="58"/>
-      <c r="X21" s="58"/>
-      <c r="Y21" s="58"/>
-      <c r="Z21" s="58"/>
-    </row>
-    <row r="22" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
-      <c r="B22" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54" t="s">
-        <v>743</v>
-      </c>
-      <c r="E22" s="54" t="s">
-        <v>744</v>
-      </c>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H22" s="54"/>
-      <c r="I22" s="59" t="s">
-        <v>745</v>
-      </c>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
-      <c r="O22" s="56"/>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="55"/>
-      <c r="S22" s="55"/>
-      <c r="T22" s="55"/>
-      <c r="U22" s="55"/>
-      <c r="V22" s="55"/>
-      <c r="W22" s="55"/>
-      <c r="X22" s="55"/>
-      <c r="Y22" s="55"/>
-      <c r="Z22" s="55"/>
-    </row>
-    <row r="23" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="58"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="58"/>
+      <c r="Q22" s="58"/>
+      <c r="R22" s="58"/>
+      <c r="S22" s="58"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="58"/>
+      <c r="W22" s="58"/>
+      <c r="X22" s="58"/>
+      <c r="Y22" s="58"/>
+      <c r="Z22" s="58"/>
+    </row>
+    <row r="23" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="54"/>
       <c r="B23" s="54" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="54"/>
       <c r="D23" s="54" t="s">
-        <v>746</v>
+        <v>727</v>
       </c>
       <c r="E23" s="54" t="s">
-        <v>747</v>
+        <v>728</v>
       </c>
       <c r="F23" s="54"/>
       <c r="G23" s="54" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="H23" s="54"/>
-      <c r="I23" s="53" t="s">
-        <v>748</v>
+      <c r="I23" s="54" t="s">
+        <v>729</v>
       </c>
       <c r="J23" s="54"/>
       <c r="K23" s="54"/>
@@ -7604,72 +7572,72 @@
       <c r="Y23" s="55"/>
       <c r="Z23" s="55"/>
     </row>
-    <row r="24" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
-      <c r="B24" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54" t="s">
-        <v>749</v>
-      </c>
-      <c r="E24" s="54" t="s">
-        <v>750</v>
-      </c>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54" t="s">
-        <v>751</v>
-      </c>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="55"/>
-      <c r="O24" s="55"/>
-      <c r="P24" s="55"/>
-      <c r="Q24" s="55"/>
-      <c r="R24" s="55"/>
-      <c r="S24" s="55"/>
-      <c r="T24" s="55"/>
-      <c r="U24" s="55"/>
-      <c r="V24" s="55"/>
-      <c r="W24" s="55"/>
-      <c r="X24" s="55"/>
-      <c r="Y24" s="55"/>
-      <c r="Z24" s="55"/>
-    </row>
-    <row r="25" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="57" t="b">
+        <v>0</v>
+      </c>
+      <c r="B24" s="57" t="s">
+        <v>730</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>731</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>732</v>
+      </c>
+      <c r="E24" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="58"/>
+      <c r="Q24" s="58"/>
+      <c r="R24" s="58"/>
+      <c r="S24" s="58"/>
+      <c r="T24" s="58"/>
+      <c r="U24" s="58"/>
+      <c r="V24" s="58"/>
+      <c r="W24" s="58"/>
+      <c r="X24" s="58"/>
+      <c r="Y24" s="58"/>
+      <c r="Z24" s="58"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="54"/>
       <c r="B25" s="54" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="54"/>
       <c r="D25" s="54" t="s">
-        <v>757</v>
+        <v>733</v>
       </c>
       <c r="E25" s="54" t="s">
-        <v>759</v>
+        <v>734</v>
       </c>
       <c r="F25" s="54"/>
       <c r="G25" s="54" t="s">
         <v>103</v>
       </c>
       <c r="H25" s="54"/>
-      <c r="I25" s="54" t="s">
-        <v>755</v>
+      <c r="I25" s="59" t="s">
+        <v>735</v>
       </c>
       <c r="J25" s="54"/>
       <c r="K25" s="54"/>
       <c r="L25" s="54"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="56"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="56"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="55"/>
       <c r="R25" s="55"/>
       <c r="S25" s="55"/>
       <c r="T25" s="55"/>
@@ -7680,229 +7648,299 @@
       <c r="Y25" s="55"/>
       <c r="Z25" s="55"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
+    <row r="26" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="54"/>
       <c r="B26" s="54" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="54"/>
       <c r="D26" s="54" t="s">
-        <v>758</v>
+        <v>736</v>
       </c>
       <c r="E26" s="54" t="s">
-        <v>760</v>
+        <v>737</v>
       </c>
       <c r="F26" s="54"/>
       <c r="G26" s="54" t="s">
         <v>103</v>
       </c>
       <c r="H26" s="54"/>
-      <c r="I26" s="54" t="s">
-        <v>756</v>
-      </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
-      <c r="V26" s="15"/>
-      <c r="W26" s="15"/>
-      <c r="X26" s="15"/>
-      <c r="Y26" s="15"/>
-      <c r="Z26" s="15"/>
+      <c r="I26" s="53" t="s">
+        <v>738</v>
+      </c>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="55"/>
+      <c r="U26" s="55"/>
+      <c r="V26" s="55"/>
+      <c r="W26" s="55"/>
+      <c r="X26" s="55"/>
+      <c r="Y26" s="55"/>
+      <c r="Z26" s="55"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="15"/>
-      <c r="W27" s="15"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="15"/>
+      <c r="A27" s="55"/>
+      <c r="B27" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54" t="s">
+        <v>739</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>740</v>
+      </c>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54" t="s">
+        <v>741</v>
+      </c>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="55"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="55"/>
+      <c r="Q27" s="55"/>
+      <c r="R27" s="55"/>
+      <c r="S27" s="55"/>
+      <c r="T27" s="55"/>
+      <c r="U27" s="55"/>
+      <c r="V27" s="55"/>
+      <c r="W27" s="55"/>
+      <c r="X27" s="55"/>
+      <c r="Y27" s="55"/>
+      <c r="Z27" s="55"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
-      <c r="U28" s="15"/>
-      <c r="V28" s="15"/>
-      <c r="W28" s="15"/>
-      <c r="X28" s="15"/>
-      <c r="Y28" s="15"/>
-      <c r="Z28" s="15"/>
+      <c r="A28" s="57" t="b">
+        <v>0</v>
+      </c>
+      <c r="B28" s="57" t="s">
+        <v>742</v>
+      </c>
+      <c r="C28" s="57" t="s">
+        <v>743</v>
+      </c>
+      <c r="D28" s="57" t="s">
+        <v>744</v>
+      </c>
+      <c r="E28" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="57"/>
+      <c r="M28" s="58"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="58"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="58"/>
+      <c r="R28" s="58"/>
+      <c r="S28" s="58"/>
+      <c r="T28" s="58"/>
+      <c r="U28" s="58"/>
+      <c r="V28" s="58"/>
+      <c r="W28" s="58"/>
+      <c r="X28" s="58"/>
+      <c r="Y28" s="58"/>
+      <c r="Z28" s="58"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
-      <c r="V29" s="15"/>
-      <c r="W29" s="15"/>
-      <c r="X29" s="15"/>
-      <c r="Y29" s="15"/>
-      <c r="Z29" s="15"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
-      <c r="V30" s="15"/>
-      <c r="W30" s="15"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="15"/>
-      <c r="Z30" s="15"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
-      <c r="T31" s="15"/>
-      <c r="U31" s="15"/>
-      <c r="V31" s="15"/>
-      <c r="W31" s="15"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="15"/>
-      <c r="Z31" s="15"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
-      <c r="T32" s="15"/>
-      <c r="U32" s="15"/>
-      <c r="V32" s="15"/>
-      <c r="W32" s="15"/>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="15"/>
-      <c r="Z32" s="15"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="54"/>
+      <c r="B29" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54" t="s">
+        <v>733</v>
+      </c>
+      <c r="E29" s="54" t="s">
+        <v>734</v>
+      </c>
+      <c r="F29" s="54"/>
+      <c r="G29" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="54"/>
+      <c r="I29" s="59" t="s">
+        <v>735</v>
+      </c>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="55"/>
+      <c r="S29" s="55"/>
+      <c r="T29" s="55"/>
+      <c r="U29" s="55"/>
+      <c r="V29" s="55"/>
+      <c r="W29" s="55"/>
+      <c r="X29" s="55"/>
+      <c r="Y29" s="55"/>
+      <c r="Z29" s="55"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="55"/>
+      <c r="B30" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54" t="s">
+        <v>736</v>
+      </c>
+      <c r="E30" s="54" t="s">
+        <v>737</v>
+      </c>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="54"/>
+      <c r="I30" s="53" t="s">
+        <v>738</v>
+      </c>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="55"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="55"/>
+      <c r="P30" s="55"/>
+      <c r="Q30" s="55"/>
+      <c r="R30" s="55"/>
+      <c r="S30" s="55"/>
+      <c r="T30" s="55"/>
+      <c r="U30" s="55"/>
+      <c r="V30" s="55"/>
+      <c r="W30" s="55"/>
+      <c r="X30" s="55"/>
+      <c r="Y30" s="55"/>
+      <c r="Z30" s="55"/>
+    </row>
+    <row r="31" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="54"/>
+      <c r="B31" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54" t="s">
+        <v>739</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>740</v>
+      </c>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54" t="s">
+        <v>741</v>
+      </c>
+      <c r="J31" s="54"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="55"/>
+      <c r="O31" s="55"/>
+      <c r="P31" s="55"/>
+      <c r="Q31" s="55"/>
+      <c r="R31" s="55"/>
+      <c r="S31" s="55"/>
+      <c r="T31" s="55"/>
+      <c r="U31" s="55"/>
+      <c r="V31" s="55"/>
+      <c r="W31" s="55"/>
+      <c r="X31" s="55"/>
+      <c r="Y31" s="55"/>
+      <c r="Z31" s="55"/>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="54"/>
+      <c r="B32" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54" t="s">
+        <v>747</v>
+      </c>
+      <c r="E32" s="54" t="s">
+        <v>749</v>
+      </c>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54" t="s">
+        <v>745</v>
+      </c>
+      <c r="J32" s="54"/>
+      <c r="K32" s="54"/>
+      <c r="L32" s="54"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="55"/>
+      <c r="S32" s="55"/>
+      <c r="T32" s="55"/>
+      <c r="U32" s="55"/>
+      <c r="V32" s="55"/>
+      <c r="W32" s="55"/>
+      <c r="X32" s="55"/>
+      <c r="Y32" s="55"/>
+      <c r="Z32" s="55"/>
+    </row>
+    <row r="33" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
+      <c r="B33" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54" t="s">
+        <v>748</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>750</v>
+      </c>
+      <c r="F33" s="54"/>
+      <c r="G33" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54" t="s">
+        <v>746</v>
+      </c>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
       <c r="M33" s="15"/>
       <c r="N33" s="15"/>
-      <c r="O33" s="41"/>
-      <c r="P33" s="41"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
       <c r="S33" s="15"/>
@@ -7914,89 +7952,119 @@
       <c r="Y33" s="15"/>
       <c r="Z33" s="15"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
-      <c r="T34" s="15"/>
-      <c r="U34" s="15"/>
-      <c r="V34" s="15"/>
-      <c r="W34" s="15"/>
-      <c r="X34" s="15"/>
-      <c r="Y34" s="15"/>
-      <c r="Z34" s="15"/>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
-      <c r="T35" s="15"/>
-      <c r="U35" s="15"/>
-      <c r="V35" s="15"/>
-      <c r="W35" s="15"/>
-      <c r="X35" s="15"/>
-      <c r="Y35" s="15"/>
-      <c r="Z35" s="15"/>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
-      <c r="U36" s="15"/>
-      <c r="V36" s="15"/>
-      <c r="W36" s="15"/>
-      <c r="X36" s="15"/>
-      <c r="Y36" s="15"/>
-      <c r="Z36" s="15"/>
+    <row r="34" spans="1:26" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>680</v>
+      </c>
+      <c r="C34" s="39" t="s">
+        <v>682</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>680</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="39"/>
+      <c r="P34" s="39"/>
+      <c r="Q34" s="39"/>
+      <c r="R34" s="39"/>
+      <c r="S34" s="39"/>
+      <c r="T34" s="39"/>
+      <c r="U34" s="39"/>
+      <c r="V34" s="39"/>
+      <c r="W34" s="39"/>
+      <c r="X34" s="39"/>
+      <c r="Y34" s="39"/>
+      <c r="Z34" s="39"/>
+    </row>
+    <row r="35" spans="1:26" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="46"/>
+      <c r="B35" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46" t="s">
+        <v>751</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>753</v>
+      </c>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" s="46"/>
+      <c r="I35" s="66" t="s">
+        <v>781</v>
+      </c>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
+      <c r="N35" s="46"/>
+      <c r="O35" s="46"/>
+      <c r="P35" s="46"/>
+      <c r="Q35" s="46"/>
+      <c r="R35" s="46"/>
+      <c r="S35" s="46"/>
+      <c r="T35" s="46"/>
+      <c r="U35" s="46"/>
+      <c r="V35" s="46"/>
+      <c r="W35" s="46"/>
+      <c r="X35" s="46"/>
+      <c r="Y35" s="46"/>
+      <c r="Z35" s="46"/>
+    </row>
+    <row r="36" spans="1:26" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="46"/>
+      <c r="B36" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46" t="s">
+        <v>752</v>
+      </c>
+      <c r="E36" s="46" t="s">
+        <v>754</v>
+      </c>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="H36" s="46"/>
+      <c r="I36" s="66" t="s">
+        <v>781</v>
+      </c>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="46"/>
+      <c r="O36" s="46"/>
+      <c r="P36" s="46"/>
+      <c r="Q36" s="46"/>
+      <c r="R36" s="46"/>
+      <c r="S36" s="46"/>
+      <c r="T36" s="46"/>
+      <c r="U36" s="46"/>
+      <c r="V36" s="46"/>
+      <c r="W36" s="46"/>
+      <c r="X36" s="46"/>
+      <c r="Y36" s="46"/>
+      <c r="Z36" s="46"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
@@ -8054,7 +8122,7 @@
       <c r="Y38" s="15"/>
       <c r="Z38" s="15"/>
     </row>
-    <row r="39" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -8068,9 +8136,9 @@
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="41"/>
-      <c r="P39" s="41"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
       <c r="S39" s="15"/>
@@ -8097,8 +8165,8 @@
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
+      <c r="O40" s="41"/>
+      <c r="P40" s="41"/>
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
       <c r="S40" s="15"/>
@@ -8251,7 +8319,7 @@
       <c r="Z45" s="15"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
@@ -8264,7 +8332,7 @@
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
+      <c r="N46" s="10"/>
       <c r="O46" s="41"/>
       <c r="P46" s="41"/>
       <c r="Q46" s="15"/>
@@ -8321,8 +8389,8 @@
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
-      <c r="O48" s="41"/>
-      <c r="P48" s="41"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
       <c r="S48" s="15"/>
@@ -8349,8 +8417,8 @@
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
       <c r="N49" s="15"/>
-      <c r="O49" s="41"/>
-      <c r="P49" s="41"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
       <c r="Q49" s="15"/>
       <c r="R49" s="15"/>
       <c r="S49" s="15"/>
@@ -8405,8 +8473,8 @@
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
-      <c r="O51" s="41"/>
-      <c r="P51" s="41"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
       <c r="Q51" s="15"/>
       <c r="R51" s="15"/>
       <c r="S51" s="15"/>
@@ -8446,8 +8514,8 @@
       <c r="Y52" s="15"/>
       <c r="Z52" s="15"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
+    <row r="53" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
@@ -8545,8 +8613,8 @@
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
       <c r="N56" s="15"/>
-      <c r="O56" s="15"/>
-      <c r="P56" s="15"/>
+      <c r="O56" s="41"/>
+      <c r="P56" s="41"/>
       <c r="Q56" s="15"/>
       <c r="R56" s="15"/>
       <c r="S56" s="15"/>
@@ -8573,8 +8641,8 @@
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
       <c r="N57" s="15"/>
-      <c r="O57" s="41"/>
-      <c r="P57" s="41"/>
+      <c r="O57" s="15"/>
+      <c r="P57" s="15"/>
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
       <c r="S57" s="15"/>
@@ -8601,8 +8669,8 @@
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
       <c r="N58" s="15"/>
-      <c r="O58" s="15"/>
-      <c r="P58" s="15"/>
+      <c r="O58" s="41"/>
+      <c r="P58" s="41"/>
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
       <c r="S58" s="15"/>
@@ -8613,6 +8681,202 @@
       <c r="X58" s="15"/>
       <c r="Y58" s="15"/>
       <c r="Z58" s="15"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A59" s="15"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="15"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15"/>
+      <c r="O59" s="15"/>
+      <c r="P59" s="15"/>
+      <c r="Q59" s="15"/>
+      <c r="R59" s="15"/>
+      <c r="S59" s="15"/>
+      <c r="T59" s="15"/>
+      <c r="U59" s="15"/>
+      <c r="V59" s="15"/>
+      <c r="W59" s="15"/>
+      <c r="X59" s="15"/>
+      <c r="Y59" s="15"/>
+      <c r="Z59" s="15"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A60" s="15"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15"/>
+      <c r="O60" s="41"/>
+      <c r="P60" s="41"/>
+      <c r="Q60" s="15"/>
+      <c r="R60" s="15"/>
+      <c r="S60" s="15"/>
+      <c r="T60" s="15"/>
+      <c r="U60" s="15"/>
+      <c r="V60" s="15"/>
+      <c r="W60" s="15"/>
+      <c r="X60" s="15"/>
+      <c r="Y60" s="15"/>
+      <c r="Z60" s="15"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A61" s="15"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
+      <c r="Q61" s="15"/>
+      <c r="R61" s="15"/>
+      <c r="S61" s="15"/>
+      <c r="T61" s="15"/>
+      <c r="U61" s="15"/>
+      <c r="V61" s="15"/>
+      <c r="W61" s="15"/>
+      <c r="X61" s="15"/>
+      <c r="Y61" s="15"/>
+      <c r="Z61" s="15"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A62" s="15"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="15"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15"/>
+      <c r="O62" s="41"/>
+      <c r="P62" s="41"/>
+      <c r="Q62" s="15"/>
+      <c r="R62" s="15"/>
+      <c r="S62" s="15"/>
+      <c r="T62" s="15"/>
+      <c r="U62" s="15"/>
+      <c r="V62" s="15"/>
+      <c r="W62" s="15"/>
+      <c r="X62" s="15"/>
+      <c r="Y62" s="15"/>
+      <c r="Z62" s="15"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A63" s="15"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="15"/>
+      <c r="Q63" s="15"/>
+      <c r="R63" s="15"/>
+      <c r="S63" s="15"/>
+      <c r="T63" s="15"/>
+      <c r="U63" s="15"/>
+      <c r="V63" s="15"/>
+      <c r="W63" s="15"/>
+      <c r="X63" s="15"/>
+      <c r="Y63" s="15"/>
+      <c r="Z63" s="15"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
+      <c r="O64" s="41"/>
+      <c r="P64" s="41"/>
+      <c r="Q64" s="15"/>
+      <c r="R64" s="15"/>
+      <c r="S64" s="15"/>
+      <c r="T64" s="15"/>
+      <c r="U64" s="15"/>
+      <c r="V64" s="15"/>
+      <c r="W64" s="15"/>
+      <c r="X64" s="15"/>
+      <c r="Y64" s="15"/>
+      <c r="Z64" s="15"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A65" s="15"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15"/>
+      <c r="O65" s="15"/>
+      <c r="P65" s="15"/>
+      <c r="Q65" s="15"/>
+      <c r="R65" s="15"/>
+      <c r="S65" s="15"/>
+      <c r="T65" s="15"/>
+      <c r="U65" s="15"/>
+      <c r="V65" s="15"/>
+      <c r="W65" s="15"/>
+      <c r="X65" s="15"/>
+      <c r="Y65" s="15"/>
+      <c r="Z65" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -8626,20 +8890,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="23" customWidth="1"/>
     <col min="3" max="3" width="28.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="67.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -8745,16 +9009,16 @@
     </row>
     <row r="4" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>703</v>
+        <v>694</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>704</v>
+        <v>695</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>705</v>
+        <v>696</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>469</v>
@@ -8778,16 +9042,16 @@
     </row>
     <row r="5" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>706</v>
+        <v>697</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>707</v>
+        <v>698</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>708</v>
+        <v>699</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>709</v>
+        <v>700</v>
       </c>
       <c r="E5" s="46" t="s">
         <v>469</v>
@@ -8811,16 +9075,16 @@
     </row>
     <row r="6" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>711</v>
+        <v>702</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="E6" s="46" t="s">
         <v>469</v>
@@ -8873,15 +9137,15 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>63</v>
@@ -8902,15 +9166,15 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>63</v>
@@ -8927,15 +9191,15 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>63</v>
@@ -8952,15 +9216,15 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>63</v>
@@ -8977,15 +9241,15 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>725</v>
+        <v>716</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>63</v>
@@ -9002,14 +9266,14 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
-        <v>771</v>
+        <v>757</v>
       </c>
       <c r="B13" s="22"/>
       <c r="D13" s="46" t="s">
-        <v>774</v>
+        <v>759</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="F13" s="46" t="s">
         <v>63</v>
@@ -9026,14 +9290,14 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>772</v>
+        <v>758</v>
       </c>
       <c r="B14" s="22"/>
       <c r="D14" s="46" t="s">
-        <v>775</v>
+        <v>760</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="F14" s="46" t="s">
         <v>63</v>
@@ -9050,15 +9314,15 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>777</v>
+        <v>761</v>
       </c>
       <c r="B15" s="53"/>
       <c r="C15" s="23"/>
       <c r="D15" s="46" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>778</v>
+        <v>792</v>
       </c>
       <c r="F15" s="46" t="s">
         <v>103</v>
@@ -9070,58 +9334,163 @@
         <v>1</v>
       </c>
       <c r="I15" s="46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="46" t="s">
+        <v>774</v>
+      </c>
       <c r="B16" s="22"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D16" s="46" t="s">
+        <v>775</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>795</v>
+      </c>
+      <c r="F16" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
+        <v>784</v>
+      </c>
+      <c r="B17" s="53"/>
+      <c r="D17" s="46" t="s">
+        <v>785</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>790</v>
+      </c>
+      <c r="F17" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="46" t="s">
+        <v>786</v>
+      </c>
+      <c r="B18" s="53"/>
+      <c r="D18" s="46" t="s">
+        <v>787</v>
+      </c>
+      <c r="E18" s="46" t="s">
+        <v>793</v>
+      </c>
+      <c r="F18" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="46" t="s">
+        <v>782</v>
+      </c>
       <c r="B19" s="22"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D19" s="46" t="s">
+        <v>783</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>791</v>
+      </c>
+      <c r="F19" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="46" t="s">
+        <v>794</v>
+      </c>
       <c r="B20" s="22"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D20" s="46" t="s">
+        <v>796</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>795</v>
+      </c>
+      <c r="F20" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="22"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" s="22"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="22"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="22"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" s="22"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="22"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" s="22"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="22"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="22"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="22"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="22"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" s="22"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
@@ -9222,6 +9591,12 @@
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="22"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="22"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updating logic in urban building type measure to work with residential measures related to zones, thermostats, HVAC equip, etc.
</commit_message>
<xml_diff>
--- a/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
+++ b/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="793">
   <si>
     <t>type</t>
   </si>
@@ -2203,9 +2203,6 @@
     <t>../weather/USA_CO_Denver.Intl.AP.725650_TMY3.epw</t>
   </si>
   <si>
-    <t>URBANopt Testing 1</t>
-  </si>
-  <si>
     <t>Add Dencity Meters</t>
   </si>
   <si>
@@ -2383,12 +2380,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Has Basement</t>
-  </si>
-  <si>
-    <t>urbanbuildingtype.has_basement</t>
-  </si>
-  <si>
     <t>Num Spaces</t>
   </si>
   <si>
@@ -2410,12 +2401,6 @@
     <t>spaces</t>
   </si>
   <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>bldgtype</t>
-  </si>
-  <si>
     <t>unitsperspace</t>
   </si>
   <si>
@@ -2426,6 +2411,9 @@
   </si>
   <si>
     <t>urbangeometrycreation.below_ground_stories</t>
+  </si>
+  <si>
+    <t>URBANopt Testing 2</t>
   </si>
 </sst>
 </file>
@@ -4229,10 +4217,10 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6039,7 +6027,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6210,7 +6198,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>722</v>
+        <v>792</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>472</v>
@@ -6652,7 +6640,7 @@
   <dimension ref="A1:Z65"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6707,14 +6695,14 @@
       <c r="R1" s="33"/>
       <c r="S1" s="30"/>
       <c r="T1" s="30"/>
-      <c r="U1" s="65" t="s">
+      <c r="U1" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
@@ -6832,7 +6820,7 @@
     </row>
     <row r="4" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="39" t="s">
         <v>679</v>
@@ -6875,10 +6863,10 @@
       </c>
       <c r="C5" s="46"/>
       <c r="D5" s="46" t="s">
+        <v>761</v>
+      </c>
+      <c r="E5" s="46" t="s">
         <v>762</v>
-      </c>
-      <c r="E5" s="46" t="s">
-        <v>763</v>
       </c>
       <c r="F5" s="46"/>
       <c r="G5" s="46" t="s">
@@ -6886,7 +6874,7 @@
       </c>
       <c r="H5" s="46"/>
       <c r="I5" s="59" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="J5" s="46"/>
       <c r="K5" s="47"/>
@@ -6913,10 +6901,10 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
+        <v>764</v>
+      </c>
+      <c r="E6" s="42" t="s">
         <v>765</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>766</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="42" t="s">
@@ -6924,28 +6912,28 @@
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="45" t="s">
+        <v>775</v>
+      </c>
+      <c r="J6" s="42" t="s">
         <v>776</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="K6" s="43">
+        <v>0</v>
+      </c>
+      <c r="L6" s="43">
+        <v>0</v>
+      </c>
+      <c r="M6" s="43">
+        <v>0</v>
+      </c>
+      <c r="N6" s="43">
+        <v>0</v>
+      </c>
+      <c r="O6" s="43">
+        <v>0</v>
+      </c>
+      <c r="P6" s="42" t="s">
         <v>777</v>
-      </c>
-      <c r="K6" s="43">
-        <v>0</v>
-      </c>
-      <c r="L6" s="43">
-        <v>0</v>
-      </c>
-      <c r="M6" s="43">
-        <v>0</v>
-      </c>
-      <c r="N6" s="43">
-        <v>0</v>
-      </c>
-      <c r="O6" s="43">
-        <v>0</v>
-      </c>
-      <c r="P6" s="42" t="s">
-        <v>778</v>
       </c>
       <c r="Q6" s="43"/>
       <c r="R6" s="42" t="s">
@@ -6965,16 +6953,16 @@
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>767</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>768</v>
       </c>
       <c r="G7" s="23" t="s">
         <v>103</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -6982,21 +6970,21 @@
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>770</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>771</v>
       </c>
       <c r="G8" s="23" t="s">
         <v>61</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="39" t="s">
         <v>679</v>
@@ -7039,10 +7027,10 @@
       </c>
       <c r="C10" s="46"/>
       <c r="D10" s="46" t="s">
+        <v>761</v>
+      </c>
+      <c r="E10" s="46" t="s">
         <v>762</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>763</v>
       </c>
       <c r="F10" s="46"/>
       <c r="G10" s="46" t="s">
@@ -7050,7 +7038,7 @@
       </c>
       <c r="H10" s="46"/>
       <c r="I10" s="59" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="J10" s="46"/>
       <c r="K10" s="47"/>
@@ -7077,10 +7065,10 @@
       </c>
       <c r="C11" s="42"/>
       <c r="D11" s="42" t="s">
+        <v>764</v>
+      </c>
+      <c r="E11" s="42" t="s">
         <v>765</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>766</v>
       </c>
       <c r="F11" s="42"/>
       <c r="G11" s="42" t="s">
@@ -7088,10 +7076,10 @@
       </c>
       <c r="H11" s="42"/>
       <c r="I11" s="45" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J11" s="42" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="K11" s="43">
         <v>0</v>
@@ -7109,7 +7097,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="42" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="Q11" s="43"/>
       <c r="R11" s="42" t="s">
@@ -7129,16 +7117,16 @@
         <v>21</v>
       </c>
       <c r="D12" s="23" t="s">
+        <v>766</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>767</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>768</v>
       </c>
       <c r="G12" s="23" t="s">
         <v>103</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="J12" s="4"/>
     </row>
@@ -7147,16 +7135,16 @@
         <v>21</v>
       </c>
       <c r="D13" s="23" t="s">
+        <v>769</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>770</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>771</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="J13" s="4"/>
     </row>
@@ -7319,10 +7307,10 @@
       </c>
       <c r="C18" s="61"/>
       <c r="D18" s="61" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E18" s="61" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F18" s="61"/>
       <c r="G18" s="61" t="s">
@@ -7330,10 +7318,10 @@
       </c>
       <c r="H18" s="61"/>
       <c r="I18" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="J18" s="61" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="K18" s="61">
         <v>0</v>
@@ -7351,7 +7339,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="61" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="Q18" s="61"/>
       <c r="R18" s="61" t="s">
@@ -7373,10 +7361,10 @@
       </c>
       <c r="C19" s="61"/>
       <c r="D19" s="61" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E19" s="61" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F19" s="61"/>
       <c r="G19" s="61" t="s">
@@ -7384,10 +7372,10 @@
       </c>
       <c r="H19" s="61"/>
       <c r="I19" s="64" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="J19" s="61" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="K19" s="61">
         <v>0</v>
@@ -7405,7 +7393,7 @@
         <v>0</v>
       </c>
       <c r="P19" s="61" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="Q19" s="61"/>
       <c r="R19" s="61" t="s">
@@ -7463,13 +7451,13 @@
         <v>0</v>
       </c>
       <c r="B21" s="52" t="s">
+        <v>722</v>
+      </c>
+      <c r="C21" s="52" t="s">
         <v>723</v>
       </c>
-      <c r="C21" s="52" t="s">
-        <v>724</v>
-      </c>
       <c r="D21" s="52" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E21" s="52" t="s">
         <v>67</v>
@@ -7501,13 +7489,13 @@
         <v>0</v>
       </c>
       <c r="B22" s="57" t="s">
+        <v>724</v>
+      </c>
+      <c r="C22" s="57" t="s">
         <v>725</v>
       </c>
-      <c r="C22" s="57" t="s">
-        <v>726</v>
-      </c>
       <c r="D22" s="57" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E22" s="57" t="s">
         <v>232</v>
@@ -7541,10 +7529,10 @@
       </c>
       <c r="C23" s="54"/>
       <c r="D23" s="54" t="s">
+        <v>726</v>
+      </c>
+      <c r="E23" s="54" t="s">
         <v>727</v>
-      </c>
-      <c r="E23" s="54" t="s">
-        <v>728</v>
       </c>
       <c r="F23" s="54"/>
       <c r="G23" s="54" t="s">
@@ -7552,7 +7540,7 @@
       </c>
       <c r="H23" s="54"/>
       <c r="I23" s="54" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="J23" s="54"/>
       <c r="K23" s="54"/>
@@ -7577,13 +7565,13 @@
         <v>0</v>
       </c>
       <c r="B24" s="57" t="s">
+        <v>729</v>
+      </c>
+      <c r="C24" s="57" t="s">
         <v>730</v>
       </c>
-      <c r="C24" s="57" t="s">
+      <c r="D24" s="57" t="s">
         <v>731</v>
-      </c>
-      <c r="D24" s="57" t="s">
-        <v>732</v>
       </c>
       <c r="E24" s="57" t="s">
         <v>232</v>
@@ -7617,10 +7605,10 @@
       </c>
       <c r="C25" s="54"/>
       <c r="D25" s="54" t="s">
+        <v>732</v>
+      </c>
+      <c r="E25" s="54" t="s">
         <v>733</v>
-      </c>
-      <c r="E25" s="54" t="s">
-        <v>734</v>
       </c>
       <c r="F25" s="54"/>
       <c r="G25" s="54" t="s">
@@ -7628,7 +7616,7 @@
       </c>
       <c r="H25" s="54"/>
       <c r="I25" s="59" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="J25" s="54"/>
       <c r="K25" s="54"/>
@@ -7655,10 +7643,10 @@
       </c>
       <c r="C26" s="54"/>
       <c r="D26" s="54" t="s">
+        <v>735</v>
+      </c>
+      <c r="E26" s="54" t="s">
         <v>736</v>
-      </c>
-      <c r="E26" s="54" t="s">
-        <v>737</v>
       </c>
       <c r="F26" s="54"/>
       <c r="G26" s="54" t="s">
@@ -7666,7 +7654,7 @@
       </c>
       <c r="H26" s="54"/>
       <c r="I26" s="53" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J26" s="54"/>
       <c r="K26" s="54"/>
@@ -7693,10 +7681,10 @@
       </c>
       <c r="C27" s="54"/>
       <c r="D27" s="54" t="s">
+        <v>738</v>
+      </c>
+      <c r="E27" s="54" t="s">
         <v>739</v>
-      </c>
-      <c r="E27" s="54" t="s">
-        <v>740</v>
       </c>
       <c r="F27" s="54"/>
       <c r="G27" s="54" t="s">
@@ -7704,7 +7692,7 @@
       </c>
       <c r="H27" s="54"/>
       <c r="I27" s="54" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J27" s="54"/>
       <c r="K27" s="54"/>
@@ -7729,13 +7717,13 @@
         <v>0</v>
       </c>
       <c r="B28" s="57" t="s">
+        <v>741</v>
+      </c>
+      <c r="C28" s="57" t="s">
         <v>742</v>
       </c>
-      <c r="C28" s="57" t="s">
+      <c r="D28" s="57" t="s">
         <v>743</v>
-      </c>
-      <c r="D28" s="57" t="s">
-        <v>744</v>
       </c>
       <c r="E28" s="57" t="s">
         <v>232</v>
@@ -7769,10 +7757,10 @@
       </c>
       <c r="C29" s="54"/>
       <c r="D29" s="54" t="s">
+        <v>732</v>
+      </c>
+      <c r="E29" s="54" t="s">
         <v>733</v>
-      </c>
-      <c r="E29" s="54" t="s">
-        <v>734</v>
       </c>
       <c r="F29" s="54"/>
       <c r="G29" s="54" t="s">
@@ -7780,7 +7768,7 @@
       </c>
       <c r="H29" s="54"/>
       <c r="I29" s="59" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="J29" s="54"/>
       <c r="K29" s="54"/>
@@ -7807,10 +7795,10 @@
       </c>
       <c r="C30" s="54"/>
       <c r="D30" s="54" t="s">
+        <v>735</v>
+      </c>
+      <c r="E30" s="54" t="s">
         <v>736</v>
-      </c>
-      <c r="E30" s="54" t="s">
-        <v>737</v>
       </c>
       <c r="F30" s="54"/>
       <c r="G30" s="54" t="s">
@@ -7818,7 +7806,7 @@
       </c>
       <c r="H30" s="54"/>
       <c r="I30" s="53" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J30" s="54"/>
       <c r="K30" s="54"/>
@@ -7845,10 +7833,10 @@
       </c>
       <c r="C31" s="54"/>
       <c r="D31" s="54" t="s">
+        <v>738</v>
+      </c>
+      <c r="E31" s="54" t="s">
         <v>739</v>
-      </c>
-      <c r="E31" s="54" t="s">
-        <v>740</v>
       </c>
       <c r="F31" s="54"/>
       <c r="G31" s="54" t="s">
@@ -7856,7 +7844,7 @@
       </c>
       <c r="H31" s="54"/>
       <c r="I31" s="54" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J31" s="54"/>
       <c r="K31" s="54"/>
@@ -7883,10 +7871,10 @@
       </c>
       <c r="C32" s="54"/>
       <c r="D32" s="54" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E32" s="54" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F32" s="54"/>
       <c r="G32" s="54" t="s">
@@ -7894,7 +7882,7 @@
       </c>
       <c r="H32" s="54"/>
       <c r="I32" s="54" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="J32" s="54"/>
       <c r="K32" s="54"/>
@@ -7921,10 +7909,10 @@
       </c>
       <c r="C33" s="54"/>
       <c r="D33" s="54" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F33" s="54"/>
       <c r="G33" s="54" t="s">
@@ -7932,7 +7920,7 @@
       </c>
       <c r="H33" s="54"/>
       <c r="I33" s="54" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
@@ -7997,18 +7985,18 @@
       </c>
       <c r="C35" s="46"/>
       <c r="D35" s="46" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F35" s="46"/>
       <c r="G35" s="46" t="s">
         <v>61</v>
       </c>
       <c r="H35" s="46"/>
-      <c r="I35" s="66" t="s">
-        <v>781</v>
+      <c r="I35" s="65" t="s">
+        <v>780</v>
       </c>
       <c r="J35" s="46"/>
       <c r="K35" s="46"/>
@@ -8035,18 +8023,18 @@
       </c>
       <c r="C36" s="46"/>
       <c r="D36" s="46" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E36" s="46" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F36" s="46"/>
       <c r="G36" s="46" t="s">
         <v>61</v>
       </c>
       <c r="H36" s="46"/>
-      <c r="I36" s="66" t="s">
-        <v>781</v>
+      <c r="I36" s="65" t="s">
+        <v>780</v>
       </c>
       <c r="J36" s="46"/>
       <c r="K36" s="46"/>
@@ -8890,11 +8878,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M67"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20:I20"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9266,11 +9254,11 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B13" s="22"/>
       <c r="D13" s="46" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E13" s="46" t="s">
         <v>714</v>
@@ -9290,11 +9278,11 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B14" s="22"/>
       <c r="D14" s="46" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E14" s="46" t="s">
         <v>714</v>
@@ -9314,16 +9302,14 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B15" s="53"/>
       <c r="C15" s="23"/>
       <c r="D15" s="46" t="s">
-        <v>773</v>
-      </c>
-      <c r="E15" s="46" t="s">
-        <v>792</v>
-      </c>
+        <v>772</v>
+      </c>
+      <c r="E15" s="46"/>
       <c r="F15" s="46" t="s">
         <v>103</v>
       </c>
@@ -9339,14 +9325,14 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B16" s="22"/>
       <c r="D16" s="46" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="F16" s="46" t="s">
         <v>64</v>
@@ -9363,14 +9349,14 @@
     </row>
     <row r="17" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="B17" s="53"/>
       <c r="D17" s="46" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="F17" s="46" t="s">
         <v>64</v>
@@ -9387,14 +9373,14 @@
     </row>
     <row r="18" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="B18" s="53"/>
       <c r="D18" s="46" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="F18" s="46" t="s">
         <v>63</v>
@@ -9411,14 +9397,14 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
-        <v>782</v>
+        <v>789</v>
       </c>
       <c r="B19" s="22"/>
       <c r="D19" s="46" t="s">
-        <v>783</v>
+        <v>791</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F19" s="46" t="s">
         <v>64</v>
@@ -9434,28 +9420,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
-        <v>794</v>
-      </c>
       <c r="B20" s="22"/>
-      <c r="D20" s="46" t="s">
-        <v>796</v>
-      </c>
-      <c r="E20" s="46" t="s">
-        <v>795</v>
-      </c>
-      <c r="F20" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="46" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="22"/>
@@ -9594,9 +9559,6 @@
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="22"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Adding LODO example districts.
</commit_message>
<xml_diff>
--- a/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
+++ b/OpenStudio-analysis-spreadsheet/projects/urban-spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="300" windowWidth="15360" windowHeight="7695" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="300" windowWidth="15360" windowHeight="7695" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2328" uniqueCount="792">
   <si>
     <t>type</t>
   </si>
@@ -2101,24 +2101,6 @@
     <t>empty</t>
   </si>
   <si>
-    <t>SetResidentialEPWFile</t>
-  </si>
-  <si>
-    <t>weather_directory</t>
-  </si>
-  <si>
-    <t>weather_file_name</t>
-  </si>
-  <si>
-    <t>Weather Directory</t>
-  </si>
-  <si>
-    <t>Weather File Name</t>
-  </si>
-  <si>
-    <t>../../weather</t>
-  </si>
-  <si>
     <t>Total Site Energy Intensity</t>
   </si>
   <si>
@@ -2197,9 +2179,6 @@
     <t>urban_building_type_e_plus</t>
   </si>
   <si>
-    <t>USA_CO_Denver.Intl.AP.725650_TMY3.epw</t>
-  </si>
-  <si>
     <t>../weather/USA_CO_Denver.Intl.AP.725650_TMY3.epw</t>
   </si>
   <si>
@@ -2414,6 +2393,24 @@
   </si>
   <si>
     <t>URBANopt Testing 2</t>
+  </si>
+  <si>
+    <t>177160'</t>
+  </si>
+  <si>
+    <t>|'177160','178322','176443','176438','176439','178310','178209','176440'|</t>
+  </si>
+  <si>
+    <t>['177160','178322','176443','176438','176439','178310','178209','176440']</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>project_name</t>
+  </si>
+  <si>
+    <t>Denver LODO 1</t>
   </si>
 </sst>
 </file>
@@ -4095,7 +4092,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4197,9 +4194,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -6076,7 +6070,7 @@
         <v>457</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>458</v>
@@ -6198,7 +6192,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>792</v>
+        <v>785</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>472</v>
@@ -6552,7 +6546,7 @@
         <v>28</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>721</v>
+        <v>714</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6637,11 +6631,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z65"/>
+  <dimension ref="A1:Z68"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6695,14 +6687,14 @@
       <c r="R1" s="33"/>
       <c r="S1" s="30"/>
       <c r="T1" s="30"/>
-      <c r="U1" s="66" t="s">
+      <c r="U1" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
@@ -6818,7 +6810,7 @@
       </c>
       <c r="Z3" s="35"/>
     </row>
-    <row r="4" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="b">
         <v>0</v>
       </c>
@@ -6863,18 +6855,18 @@
       </c>
       <c r="C5" s="46"/>
       <c r="D5" s="46" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="F5" s="46"/>
       <c r="G5" s="46" t="s">
         <v>103</v>
       </c>
       <c r="H5" s="46"/>
-      <c r="I5" s="59" t="s">
-        <v>763</v>
+      <c r="I5" s="58" t="s">
+        <v>756</v>
       </c>
       <c r="J5" s="46"/>
       <c r="K5" s="47"/>
@@ -6882,7 +6874,7 @@
       <c r="M5" s="47"/>
       <c r="N5" s="47"/>
       <c r="O5" s="47"/>
-      <c r="P5" s="63"/>
+      <c r="P5" s="62"/>
       <c r="Q5" s="47"/>
       <c r="R5" s="46"/>
       <c r="S5" s="46"/>
@@ -6901,10 +6893,10 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>765</v>
+        <v>758</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="42" t="s">
@@ -6912,10 +6904,10 @@
       </c>
       <c r="H6" s="42"/>
       <c r="I6" s="45" t="s">
-        <v>775</v>
+        <v>768</v>
       </c>
       <c r="J6" s="42" t="s">
-        <v>776</v>
+        <v>769</v>
       </c>
       <c r="K6" s="43">
         <v>0</v>
@@ -6933,7 +6925,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="42" t="s">
-        <v>777</v>
+        <v>770</v>
       </c>
       <c r="Q6" s="43"/>
       <c r="R6" s="42" t="s">
@@ -6953,16 +6945,16 @@
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>767</v>
+        <v>760</v>
       </c>
       <c r="G7" s="23" t="s">
         <v>103</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>768</v>
+        <v>761</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -6970,21 +6962,21 @@
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>769</v>
+        <v>762</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>770</v>
+        <v>763</v>
       </c>
       <c r="G8" s="23" t="s">
         <v>61</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" s="39" t="s">
         <v>679</v>
@@ -7027,18 +7019,18 @@
       </c>
       <c r="C10" s="46"/>
       <c r="D10" s="46" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
       <c r="F10" s="46"/>
       <c r="G10" s="46" t="s">
         <v>103</v>
       </c>
       <c r="H10" s="46"/>
-      <c r="I10" s="59" t="s">
-        <v>763</v>
+      <c r="I10" s="58" t="s">
+        <v>756</v>
       </c>
       <c r="J10" s="46"/>
       <c r="K10" s="47"/>
@@ -7046,7 +7038,7 @@
       <c r="M10" s="47"/>
       <c r="N10" s="47"/>
       <c r="O10" s="47"/>
-      <c r="P10" s="63"/>
+      <c r="P10" s="62"/>
       <c r="Q10" s="47"/>
       <c r="R10" s="46"/>
       <c r="S10" s="46"/>
@@ -7065,10 +7057,10 @@
       </c>
       <c r="C11" s="42"/>
       <c r="D11" s="42" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>765</v>
+        <v>758</v>
       </c>
       <c r="F11" s="42"/>
       <c r="G11" s="42" t="s">
@@ -7076,10 +7068,10 @@
       </c>
       <c r="H11" s="42"/>
       <c r="I11" s="45" t="s">
-        <v>775</v>
+        <v>768</v>
       </c>
       <c r="J11" s="42" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
       <c r="K11" s="43">
         <v>0</v>
@@ -7097,7 +7089,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="42" t="s">
-        <v>786</v>
+        <v>779</v>
       </c>
       <c r="Q11" s="43"/>
       <c r="R11" s="42" t="s">
@@ -7117,16 +7109,16 @@
         <v>21</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>767</v>
+        <v>760</v>
       </c>
       <c r="G12" s="23" t="s">
         <v>103</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>768</v>
+        <v>761</v>
       </c>
       <c r="J12" s="4"/>
     </row>
@@ -7135,56 +7127,56 @@
         <v>21</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>769</v>
+        <v>762</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>770</v>
+        <v>763</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>61</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>771</v>
+        <v>764</v>
       </c>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>688</v>
-      </c>
-      <c r="C14" s="48" t="s">
-        <v>688</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>688</v>
-      </c>
-      <c r="E14" s="48" t="s">
+    <row r="14" spans="1:26" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>679</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>681</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>679</v>
+      </c>
+      <c r="E14" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="48"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="48"/>
-      <c r="X14" s="48"/>
-      <c r="Y14" s="48"/>
-      <c r="Z14" s="48"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="39"/>
+      <c r="U14" s="39"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
     </row>
     <row r="15" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="46"/>
@@ -7193,18 +7185,18 @@
       </c>
       <c r="C15" s="46"/>
       <c r="D15" s="46" t="s">
-        <v>691</v>
+        <v>754</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>689</v>
+        <v>755</v>
       </c>
       <c r="F15" s="46"/>
       <c r="G15" s="46" t="s">
         <v>103</v>
       </c>
       <c r="H15" s="46"/>
-      <c r="I15" s="46" t="s">
-        <v>693</v>
+      <c r="I15" s="58" t="s">
+        <v>756</v>
       </c>
       <c r="J15" s="46"/>
       <c r="K15" s="47"/>
@@ -7212,7 +7204,7 @@
       <c r="M15" s="47"/>
       <c r="N15" s="47"/>
       <c r="O15" s="47"/>
-      <c r="P15" s="47"/>
+      <c r="P15" s="62"/>
       <c r="Q15" s="47"/>
       <c r="R15" s="46"/>
       <c r="S15" s="46"/>
@@ -7231,18 +7223,18 @@
       </c>
       <c r="C16" s="46"/>
       <c r="D16" s="46" t="s">
-        <v>692</v>
+        <v>789</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>690</v>
+        <v>790</v>
       </c>
       <c r="F16" s="46"/>
       <c r="G16" s="46" t="s">
         <v>103</v>
       </c>
       <c r="H16" s="46"/>
-      <c r="I16" s="46" t="s">
-        <v>720</v>
+      <c r="I16" s="64" t="s">
+        <v>791</v>
       </c>
       <c r="J16" s="46"/>
       <c r="K16" s="47"/>
@@ -7250,7 +7242,7 @@
       <c r="M16" s="47"/>
       <c r="N16" s="47"/>
       <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
+      <c r="P16" s="62"/>
       <c r="Q16" s="47"/>
       <c r="R16" s="46"/>
       <c r="S16" s="46"/>
@@ -7262,881 +7254,887 @@
       <c r="Y16" s="46"/>
       <c r="Z16" s="46"/>
     </row>
-    <row r="17" spans="1:26" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17" s="39" t="s">
+    <row r="17" spans="1:26" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="42"/>
+      <c r="B17" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42" t="s">
+        <v>757</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>758</v>
+      </c>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="42"/>
+      <c r="I17" s="45" t="s">
+        <v>786</v>
+      </c>
+      <c r="J17" s="42" t="s">
+        <v>787</v>
+      </c>
+      <c r="K17" s="43">
+        <v>0</v>
+      </c>
+      <c r="L17" s="43">
+        <v>0</v>
+      </c>
+      <c r="M17" s="43">
+        <v>0</v>
+      </c>
+      <c r="N17" s="43">
+        <v>0</v>
+      </c>
+      <c r="O17" s="43">
+        <v>0</v>
+      </c>
+      <c r="P17" s="42" t="s">
+        <v>788</v>
+      </c>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="42" t="s">
+        <v>683</v>
+      </c>
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="42"/>
+      <c r="V17" s="42"/>
+      <c r="W17" s="42"/>
+      <c r="X17" s="42"/>
+      <c r="Y17" s="42"/>
+      <c r="Z17" s="42"/>
+    </row>
+    <row r="18" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>759</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>760</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:26" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>762</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>763</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>764</v>
+      </c>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:26" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B20" s="39" t="s">
         <v>680</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C20" s="39" t="s">
         <v>682</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D20" s="39" t="s">
         <v>680</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E20" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
-      <c r="T17" s="39"/>
-      <c r="U17" s="39"/>
-      <c r="V17" s="39"/>
-      <c r="W17" s="39"/>
-      <c r="X17" s="39"/>
-      <c r="Y17" s="39"/>
-      <c r="Z17" s="39"/>
-    </row>
-    <row r="18" spans="1:26" s="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
-      <c r="B18" s="61" t="s">
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="39"/>
+      <c r="S20" s="39"/>
+      <c r="T20" s="39"/>
+      <c r="U20" s="39"/>
+      <c r="V20" s="39"/>
+      <c r="W20" s="39"/>
+      <c r="X20" s="39"/>
+      <c r="Y20" s="39"/>
+      <c r="Z20" s="39"/>
+    </row>
+    <row r="21" spans="1:26" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="60"/>
+      <c r="B21" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61" t="s">
-        <v>750</v>
-      </c>
-      <c r="E18" s="61" t="s">
-        <v>752</v>
-      </c>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61" t="s">
+      <c r="C21" s="60"/>
+      <c r="D21" s="60" t="s">
+        <v>743</v>
+      </c>
+      <c r="E21" s="60" t="s">
+        <v>745</v>
+      </c>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="61"/>
-      <c r="I18" s="64" t="s">
-        <v>780</v>
-      </c>
-      <c r="J18" s="61" t="s">
-        <v>778</v>
-      </c>
-      <c r="K18" s="61">
-        <v>0</v>
-      </c>
-      <c r="L18" s="61">
-        <v>0</v>
-      </c>
-      <c r="M18" s="61">
-        <v>0</v>
-      </c>
-      <c r="N18" s="61">
-        <v>0</v>
-      </c>
-      <c r="O18" s="61">
-        <v>0</v>
-      </c>
-      <c r="P18" s="61" t="s">
-        <v>754</v>
-      </c>
-      <c r="Q18" s="61"/>
-      <c r="R18" s="61" t="s">
+      <c r="H21" s="60"/>
+      <c r="I21" s="63" t="s">
+        <v>773</v>
+      </c>
+      <c r="J21" s="60" t="s">
+        <v>771</v>
+      </c>
+      <c r="K21" s="60">
+        <v>0</v>
+      </c>
+      <c r="L21" s="60">
+        <v>0</v>
+      </c>
+      <c r="M21" s="60">
+        <v>0</v>
+      </c>
+      <c r="N21" s="60">
+        <v>0</v>
+      </c>
+      <c r="O21" s="60">
+        <v>0</v>
+      </c>
+      <c r="P21" s="60" t="s">
+        <v>747</v>
+      </c>
+      <c r="Q21" s="60"/>
+      <c r="R21" s="60" t="s">
         <v>683</v>
       </c>
-      <c r="S18" s="61"/>
-      <c r="T18" s="61"/>
-      <c r="U18" s="61"/>
-      <c r="V18" s="61"/>
-      <c r="W18" s="61"/>
-      <c r="X18" s="61"/>
-      <c r="Y18" s="61"/>
-      <c r="Z18" s="61"/>
-    </row>
-    <row r="19" spans="1:26" s="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
-      <c r="B19" s="61" t="s">
+      <c r="S21" s="60"/>
+      <c r="T21" s="60"/>
+      <c r="U21" s="60"/>
+      <c r="V21" s="60"/>
+      <c r="W21" s="60"/>
+      <c r="X21" s="60"/>
+      <c r="Y21" s="60"/>
+      <c r="Z21" s="60"/>
+    </row>
+    <row r="22" spans="1:26" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="60"/>
+      <c r="B22" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61" t="s">
-        <v>751</v>
-      </c>
-      <c r="E19" s="61" t="s">
-        <v>753</v>
-      </c>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61" t="s">
+      <c r="C22" s="60"/>
+      <c r="D22" s="60" t="s">
+        <v>744</v>
+      </c>
+      <c r="E22" s="60" t="s">
+        <v>746</v>
+      </c>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="61"/>
-      <c r="I19" s="64" t="s">
-        <v>780</v>
-      </c>
-      <c r="J19" s="61" t="s">
-        <v>779</v>
-      </c>
-      <c r="K19" s="61">
-        <v>0</v>
-      </c>
-      <c r="L19" s="61">
-        <v>0</v>
-      </c>
-      <c r="M19" s="61">
-        <v>0</v>
-      </c>
-      <c r="N19" s="61">
-        <v>0</v>
-      </c>
-      <c r="O19" s="61">
-        <v>0</v>
-      </c>
-      <c r="P19" s="61" t="s">
-        <v>755</v>
-      </c>
-      <c r="Q19" s="61"/>
-      <c r="R19" s="61" t="s">
+      <c r="H22" s="60"/>
+      <c r="I22" s="63" t="s">
+        <v>773</v>
+      </c>
+      <c r="J22" s="60" t="s">
+        <v>772</v>
+      </c>
+      <c r="K22" s="60">
+        <v>0</v>
+      </c>
+      <c r="L22" s="60">
+        <v>0</v>
+      </c>
+      <c r="M22" s="60">
+        <v>0</v>
+      </c>
+      <c r="N22" s="60">
+        <v>0</v>
+      </c>
+      <c r="O22" s="60">
+        <v>0</v>
+      </c>
+      <c r="P22" s="60" t="s">
+        <v>748</v>
+      </c>
+      <c r="Q22" s="60"/>
+      <c r="R22" s="60" t="s">
         <v>683</v>
       </c>
-      <c r="S19" s="61"/>
-      <c r="T19" s="61"/>
-      <c r="U19" s="61"/>
-      <c r="V19" s="61"/>
-      <c r="W19" s="61"/>
-      <c r="X19" s="61"/>
-      <c r="Y19" s="61"/>
-      <c r="Z19" s="61"/>
-    </row>
-    <row r="20" spans="1:26" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50" t="b">
+      <c r="S22" s="60"/>
+      <c r="T22" s="60"/>
+      <c r="U22" s="60"/>
+      <c r="V22" s="60"/>
+      <c r="W22" s="60"/>
+      <c r="X22" s="60"/>
+      <c r="Y22" s="60"/>
+      <c r="Z22" s="60"/>
+    </row>
+    <row r="23" spans="1:26" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B23" s="49" t="s">
+        <v>712</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>713</v>
+      </c>
+      <c r="D23" s="49" t="s">
+        <v>712</v>
+      </c>
+      <c r="E23" s="49" t="s">
+        <v>159</v>
+      </c>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48"/>
+      <c r="S23" s="48"/>
+      <c r="T23" s="48"/>
+      <c r="U23" s="48"/>
+      <c r="V23" s="48"/>
+      <c r="W23" s="48"/>
+      <c r="X23" s="48"/>
+      <c r="Y23" s="48"/>
+      <c r="Z23" s="48"/>
+    </row>
+    <row r="24" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>715</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>716</v>
+      </c>
+      <c r="D24" s="51" t="s">
+        <v>716</v>
+      </c>
+      <c r="E24" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="50"/>
+      <c r="R24" s="50"/>
+      <c r="S24" s="50"/>
+      <c r="T24" s="50"/>
+      <c r="U24" s="50"/>
+      <c r="V24" s="50"/>
+      <c r="W24" s="50"/>
+      <c r="X24" s="50"/>
+      <c r="Y24" s="50"/>
+      <c r="Z24" s="50"/>
+    </row>
+    <row r="25" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="B25" s="56" t="s">
+        <v>717</v>
+      </c>
+      <c r="C25" s="56" t="s">
         <v>718</v>
       </c>
-      <c r="C20" s="50" t="s">
+      <c r="D25" s="56" t="s">
+        <v>718</v>
+      </c>
+      <c r="E25" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="57"/>
+      <c r="R25" s="57"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
+      <c r="Y25" s="57"/>
+      <c r="Z25" s="57"/>
+    </row>
+    <row r="26" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="53"/>
+      <c r="B26" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53" t="s">
         <v>719</v>
       </c>
-      <c r="D20" s="50" t="s">
-        <v>718</v>
-      </c>
-      <c r="E20" s="50" t="s">
-        <v>159</v>
-      </c>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="48"/>
-      <c r="S20" s="48"/>
-      <c r="T20" s="48"/>
-      <c r="U20" s="48"/>
-      <c r="V20" s="48"/>
-      <c r="W20" s="48"/>
-      <c r="X20" s="48"/>
-      <c r="Y20" s="48"/>
-      <c r="Z20" s="48"/>
-    </row>
-    <row r="21" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21" s="52" t="s">
+      <c r="E26" s="53" t="s">
+        <v>720</v>
+      </c>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53" t="s">
+        <v>721</v>
+      </c>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="54"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="54"/>
+      <c r="S26" s="54"/>
+      <c r="T26" s="54"/>
+      <c r="U26" s="54"/>
+      <c r="V26" s="54"/>
+      <c r="W26" s="54"/>
+      <c r="X26" s="54"/>
+      <c r="Y26" s="54"/>
+      <c r="Z26" s="54"/>
+    </row>
+    <row r="27" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="B27" s="56" t="s">
         <v>722</v>
       </c>
-      <c r="C21" s="52" t="s">
+      <c r="C27" s="56" t="s">
         <v>723</v>
       </c>
-      <c r="D21" s="52" t="s">
-        <v>723</v>
-      </c>
-      <c r="E21" s="52" t="s">
+      <c r="D27" s="56" t="s">
+        <v>724</v>
+      </c>
+      <c r="E27" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="57"/>
+      <c r="N27" s="57"/>
+      <c r="O27" s="57"/>
+      <c r="P27" s="57"/>
+      <c r="Q27" s="57"/>
+      <c r="R27" s="57"/>
+      <c r="S27" s="57"/>
+      <c r="T27" s="57"/>
+      <c r="U27" s="57"/>
+      <c r="V27" s="57"/>
+      <c r="W27" s="57"/>
+      <c r="X27" s="57"/>
+      <c r="Y27" s="57"/>
+      <c r="Z27" s="57"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="53"/>
+      <c r="B28" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53" t="s">
+        <v>725</v>
+      </c>
+      <c r="E28" s="53" t="s">
+        <v>726</v>
+      </c>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="53"/>
+      <c r="I28" s="58" t="s">
+        <v>727</v>
+      </c>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="54"/>
+      <c r="N28" s="54"/>
+      <c r="O28" s="54"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="54"/>
+      <c r="T28" s="54"/>
+      <c r="U28" s="54"/>
+      <c r="V28" s="54"/>
+      <c r="W28" s="54"/>
+      <c r="X28" s="54"/>
+      <c r="Y28" s="54"/>
+      <c r="Z28" s="54"/>
+    </row>
+    <row r="29" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="53"/>
+      <c r="B29" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53" t="s">
+        <v>728</v>
+      </c>
+      <c r="E29" s="53" t="s">
+        <v>729</v>
+      </c>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="53"/>
+      <c r="I29" s="52" t="s">
+        <v>730</v>
+      </c>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
+      <c r="O29" s="54"/>
+      <c r="P29" s="54"/>
+      <c r="Q29" s="54"/>
+      <c r="R29" s="54"/>
+      <c r="S29" s="54"/>
+      <c r="T29" s="54"/>
+      <c r="U29" s="54"/>
+      <c r="V29" s="54"/>
+      <c r="W29" s="54"/>
+      <c r="X29" s="54"/>
+      <c r="Y29" s="54"/>
+      <c r="Z29" s="54"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="54"/>
+      <c r="B30" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53" t="s">
+        <v>731</v>
+      </c>
+      <c r="E30" s="53" t="s">
+        <v>732</v>
+      </c>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53" t="s">
+        <v>733</v>
+      </c>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="54"/>
+      <c r="O30" s="54"/>
+      <c r="P30" s="54"/>
+      <c r="Q30" s="54"/>
+      <c r="R30" s="54"/>
+      <c r="S30" s="54"/>
+      <c r="T30" s="54"/>
+      <c r="U30" s="54"/>
+      <c r="V30" s="54"/>
+      <c r="W30" s="54"/>
+      <c r="X30" s="54"/>
+      <c r="Y30" s="54"/>
+      <c r="Z30" s="54"/>
+    </row>
+    <row r="31" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="56" t="b">
+        <v>0</v>
+      </c>
+      <c r="B31" s="56" t="s">
+        <v>734</v>
+      </c>
+      <c r="C31" s="56" t="s">
+        <v>735</v>
+      </c>
+      <c r="D31" s="56" t="s">
+        <v>736</v>
+      </c>
+      <c r="E31" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="57"/>
+      <c r="P31" s="57"/>
+      <c r="Q31" s="57"/>
+      <c r="R31" s="57"/>
+      <c r="S31" s="57"/>
+      <c r="T31" s="57"/>
+      <c r="U31" s="57"/>
+      <c r="V31" s="57"/>
+      <c r="W31" s="57"/>
+      <c r="X31" s="57"/>
+      <c r="Y31" s="57"/>
+      <c r="Z31" s="57"/>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="53"/>
+      <c r="B32" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53" t="s">
+        <v>725</v>
+      </c>
+      <c r="E32" s="53" t="s">
+        <v>726</v>
+      </c>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="53"/>
+      <c r="I32" s="58" t="s">
+        <v>727</v>
+      </c>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="53"/>
+      <c r="M32" s="55"/>
+      <c r="N32" s="55"/>
+      <c r="O32" s="55"/>
+      <c r="P32" s="55"/>
+      <c r="Q32" s="55"/>
+      <c r="R32" s="54"/>
+      <c r="S32" s="54"/>
+      <c r="T32" s="54"/>
+      <c r="U32" s="54"/>
+      <c r="V32" s="54"/>
+      <c r="W32" s="54"/>
+      <c r="X32" s="54"/>
+      <c r="Y32" s="54"/>
+      <c r="Z32" s="54"/>
+    </row>
+    <row r="33" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="54"/>
+      <c r="B33" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53" t="s">
+        <v>728</v>
+      </c>
+      <c r="E33" s="53" t="s">
+        <v>729</v>
+      </c>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="53"/>
+      <c r="I33" s="52" t="s">
+        <v>730</v>
+      </c>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="54"/>
+      <c r="N33" s="54"/>
+      <c r="O33" s="54"/>
+      <c r="P33" s="54"/>
+      <c r="Q33" s="54"/>
+      <c r="R33" s="54"/>
+      <c r="S33" s="54"/>
+      <c r="T33" s="54"/>
+      <c r="U33" s="54"/>
+      <c r="V33" s="54"/>
+      <c r="W33" s="54"/>
+      <c r="X33" s="54"/>
+      <c r="Y33" s="54"/>
+      <c r="Z33" s="54"/>
+    </row>
+    <row r="34" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="53"/>
+      <c r="B34" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53" t="s">
+        <v>731</v>
+      </c>
+      <c r="E34" s="53" t="s">
+        <v>732</v>
+      </c>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53" t="s">
+        <v>733</v>
+      </c>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="53"/>
+      <c r="N34" s="54"/>
+      <c r="O34" s="54"/>
+      <c r="P34" s="54"/>
+      <c r="Q34" s="54"/>
+      <c r="R34" s="54"/>
+      <c r="S34" s="54"/>
+      <c r="T34" s="54"/>
+      <c r="U34" s="54"/>
+      <c r="V34" s="54"/>
+      <c r="W34" s="54"/>
+      <c r="X34" s="54"/>
+      <c r="Y34" s="54"/>
+      <c r="Z34" s="54"/>
+    </row>
+    <row r="35" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="53"/>
+      <c r="B35" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53" t="s">
+        <v>739</v>
+      </c>
+      <c r="E35" s="53" t="s">
+        <v>741</v>
+      </c>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53" t="s">
+        <v>737</v>
+      </c>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="55"/>
+      <c r="O35" s="55"/>
+      <c r="P35" s="55"/>
+      <c r="Q35" s="55"/>
+      <c r="R35" s="54"/>
+      <c r="S35" s="54"/>
+      <c r="T35" s="54"/>
+      <c r="U35" s="54"/>
+      <c r="V35" s="54"/>
+      <c r="W35" s="54"/>
+      <c r="X35" s="54"/>
+      <c r="Y35" s="54"/>
+      <c r="Z35" s="54"/>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53" t="s">
+        <v>740</v>
+      </c>
+      <c r="E36" s="53" t="s">
+        <v>742</v>
+      </c>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53" t="s">
+        <v>738</v>
+      </c>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="15"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="15"/>
+      <c r="X36" s="15"/>
+      <c r="Y36" s="15"/>
+      <c r="Z36" s="15"/>
+    </row>
+    <row r="37" spans="1:26" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B37" s="39" t="s">
+        <v>680</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>682</v>
+      </c>
+      <c r="D37" s="39" t="s">
+        <v>680</v>
+      </c>
+      <c r="E37" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="51"/>
-      <c r="R21" s="51"/>
-      <c r="S21" s="51"/>
-      <c r="T21" s="51"/>
-      <c r="U21" s="51"/>
-      <c r="V21" s="51"/>
-      <c r="W21" s="51"/>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="51"/>
-      <c r="Z21" s="51"/>
-    </row>
-    <row r="22" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="57" t="b">
-        <v>0</v>
-      </c>
-      <c r="B22" s="57" t="s">
-        <v>724</v>
-      </c>
-      <c r="C22" s="57" t="s">
-        <v>725</v>
-      </c>
-      <c r="D22" s="57" t="s">
-        <v>725</v>
-      </c>
-      <c r="E22" s="57" t="s">
-        <v>232</v>
-      </c>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="58"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="58"/>
-      <c r="P22" s="58"/>
-      <c r="Q22" s="58"/>
-      <c r="R22" s="58"/>
-      <c r="S22" s="58"/>
-      <c r="T22" s="58"/>
-      <c r="U22" s="58"/>
-      <c r="V22" s="58"/>
-      <c r="W22" s="58"/>
-      <c r="X22" s="58"/>
-      <c r="Y22" s="58"/>
-      <c r="Z22" s="58"/>
-    </row>
-    <row r="23" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
-      <c r="B23" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54" t="s">
-        <v>726</v>
-      </c>
-      <c r="E23" s="54" t="s">
-        <v>727</v>
-      </c>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54" t="s">
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="39"/>
+      <c r="P37" s="39"/>
+      <c r="Q37" s="39"/>
+      <c r="R37" s="39"/>
+      <c r="S37" s="39"/>
+      <c r="T37" s="39"/>
+      <c r="U37" s="39"/>
+      <c r="V37" s="39"/>
+      <c r="W37" s="39"/>
+      <c r="X37" s="39"/>
+      <c r="Y37" s="39"/>
+      <c r="Z37" s="39"/>
+    </row>
+    <row r="38" spans="1:26" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="46"/>
+      <c r="B38" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46" t="s">
+        <v>743</v>
+      </c>
+      <c r="E38" s="46" t="s">
+        <v>745</v>
+      </c>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54" t="s">
-        <v>728</v>
-      </c>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="55"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="55"/>
-      <c r="R23" s="55"/>
-      <c r="S23" s="55"/>
-      <c r="T23" s="55"/>
-      <c r="U23" s="55"/>
-      <c r="V23" s="55"/>
-      <c r="W23" s="55"/>
-      <c r="X23" s="55"/>
-      <c r="Y23" s="55"/>
-      <c r="Z23" s="55"/>
-    </row>
-    <row r="24" spans="1:26" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="57" t="b">
-        <v>0</v>
-      </c>
-      <c r="B24" s="57" t="s">
-        <v>729</v>
-      </c>
-      <c r="C24" s="57" t="s">
-        <v>730</v>
-      </c>
-      <c r="D24" s="57" t="s">
-        <v>731</v>
-      </c>
-      <c r="E24" s="57" t="s">
-        <v>232</v>
-      </c>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="58"/>
-      <c r="O24" s="58"/>
-      <c r="P24" s="58"/>
-      <c r="Q24" s="58"/>
-      <c r="R24" s="58"/>
-      <c r="S24" s="58"/>
-      <c r="T24" s="58"/>
-      <c r="U24" s="58"/>
-      <c r="V24" s="58"/>
-      <c r="W24" s="58"/>
-      <c r="X24" s="58"/>
-      <c r="Y24" s="58"/>
-      <c r="Z24" s="58"/>
-    </row>
-    <row r="25" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
-      <c r="B25" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54" t="s">
-        <v>732</v>
-      </c>
-      <c r="E25" s="54" t="s">
-        <v>733</v>
-      </c>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H25" s="54"/>
-      <c r="I25" s="59" t="s">
-        <v>734</v>
-      </c>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="55"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="55"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="55"/>
-      <c r="R25" s="55"/>
-      <c r="S25" s="55"/>
-      <c r="T25" s="55"/>
-      <c r="U25" s="55"/>
-      <c r="V25" s="55"/>
-      <c r="W25" s="55"/>
-      <c r="X25" s="55"/>
-      <c r="Y25" s="55"/>
-      <c r="Z25" s="55"/>
-    </row>
-    <row r="26" spans="1:26" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
-      <c r="B26" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54" t="s">
-        <v>735</v>
-      </c>
-      <c r="E26" s="54" t="s">
-        <v>736</v>
-      </c>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H26" s="54"/>
-      <c r="I26" s="53" t="s">
-        <v>737</v>
-      </c>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="55"/>
-      <c r="R26" s="55"/>
-      <c r="S26" s="55"/>
-      <c r="T26" s="55"/>
-      <c r="U26" s="55"/>
-      <c r="V26" s="55"/>
-      <c r="W26" s="55"/>
-      <c r="X26" s="55"/>
-      <c r="Y26" s="55"/>
-      <c r="Z26" s="55"/>
-    </row>
-    <row r="27" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="55"/>
-      <c r="B27" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54" t="s">
-        <v>738</v>
-      </c>
-      <c r="E27" s="54" t="s">
-        <v>739</v>
-      </c>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54" t="s">
-        <v>740</v>
-      </c>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="55"/>
-      <c r="N27" s="55"/>
-      <c r="O27" s="55"/>
-      <c r="P27" s="55"/>
-      <c r="Q27" s="55"/>
-      <c r="R27" s="55"/>
-      <c r="S27" s="55"/>
-      <c r="T27" s="55"/>
-      <c r="U27" s="55"/>
-      <c r="V27" s="55"/>
-      <c r="W27" s="55"/>
-      <c r="X27" s="55"/>
-      <c r="Y27" s="55"/>
-      <c r="Z27" s="55"/>
-    </row>
-    <row r="28" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="57" t="b">
-        <v>0</v>
-      </c>
-      <c r="B28" s="57" t="s">
-        <v>741</v>
-      </c>
-      <c r="C28" s="57" t="s">
-        <v>742</v>
-      </c>
-      <c r="D28" s="57" t="s">
-        <v>743</v>
-      </c>
-      <c r="E28" s="57" t="s">
-        <v>232</v>
-      </c>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="58"/>
-      <c r="N28" s="58"/>
-      <c r="O28" s="58"/>
-      <c r="P28" s="58"/>
-      <c r="Q28" s="58"/>
-      <c r="R28" s="58"/>
-      <c r="S28" s="58"/>
-      <c r="T28" s="58"/>
-      <c r="U28" s="58"/>
-      <c r="V28" s="58"/>
-      <c r="W28" s="58"/>
-      <c r="X28" s="58"/>
-      <c r="Y28" s="58"/>
-      <c r="Z28" s="58"/>
-    </row>
-    <row r="29" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54" t="s">
-        <v>732</v>
-      </c>
-      <c r="E29" s="54" t="s">
-        <v>733</v>
-      </c>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H29" s="54"/>
-      <c r="I29" s="59" t="s">
-        <v>734</v>
-      </c>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="56"/>
-      <c r="R29" s="55"/>
-      <c r="S29" s="55"/>
-      <c r="T29" s="55"/>
-      <c r="U29" s="55"/>
-      <c r="V29" s="55"/>
-      <c r="W29" s="55"/>
-      <c r="X29" s="55"/>
-      <c r="Y29" s="55"/>
-      <c r="Z29" s="55"/>
-    </row>
-    <row r="30" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
-      <c r="B30" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54" t="s">
-        <v>735</v>
-      </c>
-      <c r="E30" s="54" t="s">
-        <v>736</v>
-      </c>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H30" s="54"/>
-      <c r="I30" s="53" t="s">
-        <v>737</v>
-      </c>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="55"/>
-      <c r="N30" s="55"/>
-      <c r="O30" s="55"/>
-      <c r="P30" s="55"/>
-      <c r="Q30" s="55"/>
-      <c r="R30" s="55"/>
-      <c r="S30" s="55"/>
-      <c r="T30" s="55"/>
-      <c r="U30" s="55"/>
-      <c r="V30" s="55"/>
-      <c r="W30" s="55"/>
-      <c r="X30" s="55"/>
-      <c r="Y30" s="55"/>
-      <c r="Z30" s="55"/>
-    </row>
-    <row r="31" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
-      <c r="B31" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54" t="s">
-        <v>738</v>
-      </c>
-      <c r="E31" s="54" t="s">
-        <v>739</v>
-      </c>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54" t="s">
-        <v>740</v>
-      </c>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
-      <c r="M31" s="54"/>
-      <c r="N31" s="55"/>
-      <c r="O31" s="55"/>
-      <c r="P31" s="55"/>
-      <c r="Q31" s="55"/>
-      <c r="R31" s="55"/>
-      <c r="S31" s="55"/>
-      <c r="T31" s="55"/>
-      <c r="U31" s="55"/>
-      <c r="V31" s="55"/>
-      <c r="W31" s="55"/>
-      <c r="X31" s="55"/>
-      <c r="Y31" s="55"/>
-      <c r="Z31" s="55"/>
-    </row>
-    <row r="32" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54" t="s">
+      <c r="H38" s="46"/>
+      <c r="I38" s="64" t="s">
+        <v>773</v>
+      </c>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="46"/>
+      <c r="O38" s="46"/>
+      <c r="P38" s="46"/>
+      <c r="Q38" s="46"/>
+      <c r="R38" s="46"/>
+      <c r="S38" s="46"/>
+      <c r="T38" s="46"/>
+      <c r="U38" s="46"/>
+      <c r="V38" s="46"/>
+      <c r="W38" s="46"/>
+      <c r="X38" s="46"/>
+      <c r="Y38" s="46"/>
+      <c r="Z38" s="46"/>
+    </row>
+    <row r="39" spans="1:26" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="46"/>
+      <c r="B39" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46" t="s">
+        <v>744</v>
+      </c>
+      <c r="E39" s="46" t="s">
         <v>746</v>
       </c>
-      <c r="E32" s="54" t="s">
-        <v>748</v>
-      </c>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H32" s="54"/>
-      <c r="I32" s="54" t="s">
-        <v>744</v>
-      </c>
-      <c r="J32" s="54"/>
-      <c r="K32" s="54"/>
-      <c r="L32" s="54"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
-      <c r="O32" s="56"/>
-      <c r="P32" s="56"/>
-      <c r="Q32" s="56"/>
-      <c r="R32" s="55"/>
-      <c r="S32" s="55"/>
-      <c r="T32" s="55"/>
-      <c r="U32" s="55"/>
-      <c r="V32" s="55"/>
-      <c r="W32" s="55"/>
-      <c r="X32" s="55"/>
-      <c r="Y32" s="55"/>
-      <c r="Z32" s="55"/>
-    </row>
-    <row r="33" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54" t="s">
-        <v>747</v>
-      </c>
-      <c r="E33" s="54" t="s">
-        <v>749</v>
-      </c>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="H33" s="54"/>
-      <c r="I33" s="54" t="s">
-        <v>745</v>
-      </c>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
-      <c r="T33" s="15"/>
-      <c r="U33" s="15"/>
-      <c r="V33" s="15"/>
-      <c r="W33" s="15"/>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="15"/>
-      <c r="Z33" s="15"/>
-    </row>
-    <row r="34" spans="1:26" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="B34" s="39" t="s">
-        <v>680</v>
-      </c>
-      <c r="C34" s="39" t="s">
-        <v>682</v>
-      </c>
-      <c r="D34" s="39" t="s">
-        <v>680</v>
-      </c>
-      <c r="E34" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="39"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="39"/>
-      <c r="R34" s="39"/>
-      <c r="S34" s="39"/>
-      <c r="T34" s="39"/>
-      <c r="U34" s="39"/>
-      <c r="V34" s="39"/>
-      <c r="W34" s="39"/>
-      <c r="X34" s="39"/>
-      <c r="Y34" s="39"/>
-      <c r="Z34" s="39"/>
-    </row>
-    <row r="35" spans="1:26" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
-      <c r="B35" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46" t="s">
-        <v>750</v>
-      </c>
-      <c r="E35" s="46" t="s">
-        <v>752</v>
-      </c>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46" t="s">
+      <c r="F39" s="46"/>
+      <c r="G39" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="H35" s="46"/>
-      <c r="I35" s="65" t="s">
-        <v>780</v>
-      </c>
-      <c r="J35" s="46"/>
-      <c r="K35" s="46"/>
-      <c r="L35" s="46"/>
-      <c r="M35" s="46"/>
-      <c r="N35" s="46"/>
-      <c r="O35" s="46"/>
-      <c r="P35" s="46"/>
-      <c r="Q35" s="46"/>
-      <c r="R35" s="46"/>
-      <c r="S35" s="46"/>
-      <c r="T35" s="46"/>
-      <c r="U35" s="46"/>
-      <c r="V35" s="46"/>
-      <c r="W35" s="46"/>
-      <c r="X35" s="46"/>
-      <c r="Y35" s="46"/>
-      <c r="Z35" s="46"/>
-    </row>
-    <row r="36" spans="1:26" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
-      <c r="B36" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46" t="s">
-        <v>751</v>
-      </c>
-      <c r="E36" s="46" t="s">
-        <v>753</v>
-      </c>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="H36" s="46"/>
-      <c r="I36" s="65" t="s">
-        <v>780</v>
-      </c>
-      <c r="J36" s="46"/>
-      <c r="K36" s="46"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="46"/>
-      <c r="N36" s="46"/>
-      <c r="O36" s="46"/>
-      <c r="P36" s="46"/>
-      <c r="Q36" s="46"/>
-      <c r="R36" s="46"/>
-      <c r="S36" s="46"/>
-      <c r="T36" s="46"/>
-      <c r="U36" s="46"/>
-      <c r="V36" s="46"/>
-      <c r="W36" s="46"/>
-      <c r="X36" s="46"/>
-      <c r="Y36" s="46"/>
-      <c r="Z36" s="46"/>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
-      <c r="U37" s="15"/>
-      <c r="V37" s="15"/>
-      <c r="W37" s="15"/>
-      <c r="X37" s="15"/>
-      <c r="Y37" s="15"/>
-      <c r="Z37" s="15"/>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
-      <c r="U38" s="15"/>
-      <c r="V38" s="15"/>
-      <c r="W38" s="15"/>
-      <c r="X38" s="15"/>
-      <c r="Y38" s="15"/>
-      <c r="Z38" s="15"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="15"/>
-      <c r="R39" s="15"/>
-      <c r="S39" s="15"/>
-      <c r="T39" s="15"/>
-      <c r="U39" s="15"/>
-      <c r="V39" s="15"/>
-      <c r="W39" s="15"/>
-      <c r="X39" s="15"/>
-      <c r="Y39" s="15"/>
-      <c r="Z39" s="15"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="64" t="s">
+        <v>773</v>
+      </c>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
+      <c r="N39" s="46"/>
+      <c r="O39" s="46"/>
+      <c r="P39" s="46"/>
+      <c r="Q39" s="46"/>
+      <c r="R39" s="46"/>
+      <c r="S39" s="46"/>
+      <c r="T39" s="46"/>
+      <c r="U39" s="46"/>
+      <c r="V39" s="46"/>
+      <c r="W39" s="46"/>
+      <c r="X39" s="46"/>
+      <c r="Y39" s="46"/>
+      <c r="Z39" s="46"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
@@ -8153,8 +8151,8 @@
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
-      <c r="O40" s="41"/>
-      <c r="P40" s="41"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
       <c r="S40" s="15"/>
@@ -8237,8 +8235,8 @@
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
+      <c r="O43" s="41"/>
+      <c r="P43" s="41"/>
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
       <c r="S43" s="15"/>
@@ -8306,7 +8304,7 @@
       <c r="Y45" s="15"/>
       <c r="Z45" s="15"/>
     </row>
-    <row r="46" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -8320,9 +8318,9 @@
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="41"/>
-      <c r="P46" s="41"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
       <c r="S46" s="15"/>
@@ -8390,7 +8388,7 @@
       <c r="Y48" s="15"/>
       <c r="Z48" s="15"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -8404,9 +8402,9 @@
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
-      <c r="N49" s="15"/>
-      <c r="O49" s="15"/>
-      <c r="P49" s="15"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="41"/>
+      <c r="P49" s="41"/>
       <c r="Q49" s="15"/>
       <c r="R49" s="15"/>
       <c r="S49" s="15"/>
@@ -8502,8 +8500,8 @@
       <c r="Y52" s="15"/>
       <c r="Z52" s="15"/>
     </row>
-    <row r="53" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
@@ -8517,8 +8515,8 @@
       <c r="L53" s="15"/>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
-      <c r="O53" s="41"/>
-      <c r="P53" s="41"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
       <c r="Q53" s="15"/>
       <c r="R53" s="15"/>
       <c r="S53" s="15"/>
@@ -8573,8 +8571,8 @@
       <c r="L55" s="15"/>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
-      <c r="O55" s="41"/>
-      <c r="P55" s="41"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
       <c r="S55" s="15"/>
@@ -8586,8 +8584,8 @@
       <c r="Y55" s="15"/>
       <c r="Z55" s="15"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+    <row r="56" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
       <c r="D56" s="15"/>
@@ -8685,8 +8683,8 @@
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
-      <c r="O59" s="15"/>
-      <c r="P59" s="15"/>
+      <c r="O59" s="41"/>
+      <c r="P59" s="41"/>
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
       <c r="S59" s="15"/>
@@ -8713,8 +8711,8 @@
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
       <c r="N60" s="15"/>
-      <c r="O60" s="41"/>
-      <c r="P60" s="41"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="15"/>
       <c r="Q60" s="15"/>
       <c r="R60" s="15"/>
       <c r="S60" s="15"/>
@@ -8741,8 +8739,8 @@
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
       <c r="N61" s="15"/>
-      <c r="O61" s="15"/>
-      <c r="P61" s="15"/>
+      <c r="O61" s="41"/>
+      <c r="P61" s="41"/>
       <c r="Q61" s="15"/>
       <c r="R61" s="15"/>
       <c r="S61" s="15"/>
@@ -8769,8 +8767,8 @@
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
       <c r="N62" s="15"/>
-      <c r="O62" s="41"/>
-      <c r="P62" s="41"/>
+      <c r="O62" s="15"/>
+      <c r="P62" s="15"/>
       <c r="Q62" s="15"/>
       <c r="R62" s="15"/>
       <c r="S62" s="15"/>
@@ -8797,8 +8795,8 @@
       <c r="L63" s="15"/>
       <c r="M63" s="15"/>
       <c r="N63" s="15"/>
-      <c r="O63" s="15"/>
-      <c r="P63" s="15"/>
+      <c r="O63" s="41"/>
+      <c r="P63" s="41"/>
       <c r="Q63" s="15"/>
       <c r="R63" s="15"/>
       <c r="S63" s="15"/>
@@ -8825,8 +8823,8 @@
       <c r="L64" s="15"/>
       <c r="M64" s="15"/>
       <c r="N64" s="15"/>
-      <c r="O64" s="41"/>
-      <c r="P64" s="41"/>
+      <c r="O64" s="15"/>
+      <c r="P64" s="15"/>
       <c r="Q64" s="15"/>
       <c r="R64" s="15"/>
       <c r="S64" s="15"/>
@@ -8853,8 +8851,8 @@
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
       <c r="N65" s="15"/>
-      <c r="O65" s="15"/>
-      <c r="P65" s="15"/>
+      <c r="O65" s="41"/>
+      <c r="P65" s="41"/>
       <c r="Q65" s="15"/>
       <c r="R65" s="15"/>
       <c r="S65" s="15"/>
@@ -8865,6 +8863,90 @@
       <c r="X65" s="15"/>
       <c r="Y65" s="15"/>
       <c r="Z65" s="15"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A66" s="15"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
+      <c r="O66" s="15"/>
+      <c r="P66" s="15"/>
+      <c r="Q66" s="15"/>
+      <c r="R66" s="15"/>
+      <c r="S66" s="15"/>
+      <c r="T66" s="15"/>
+      <c r="U66" s="15"/>
+      <c r="V66" s="15"/>
+      <c r="W66" s="15"/>
+      <c r="X66" s="15"/>
+      <c r="Y66" s="15"/>
+      <c r="Z66" s="15"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A67" s="15"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
+      <c r="O67" s="41"/>
+      <c r="P67" s="41"/>
+      <c r="Q67" s="15"/>
+      <c r="R67" s="15"/>
+      <c r="S67" s="15"/>
+      <c r="T67" s="15"/>
+      <c r="U67" s="15"/>
+      <c r="V67" s="15"/>
+      <c r="W67" s="15"/>
+      <c r="X67" s="15"/>
+      <c r="Y67" s="15"/>
+      <c r="Z67" s="15"/>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A68" s="15"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="15"/>
+      <c r="O68" s="15"/>
+      <c r="P68" s="15"/>
+      <c r="Q68" s="15"/>
+      <c r="R68" s="15"/>
+      <c r="S68" s="15"/>
+      <c r="T68" s="15"/>
+      <c r="U68" s="15"/>
+      <c r="V68" s="15"/>
+      <c r="W68" s="15"/>
+      <c r="X68" s="15"/>
+      <c r="Y68" s="15"/>
+      <c r="Z68" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -8880,7 +8962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -8997,13 +9079,13 @@
     </row>
     <row r="4" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>684</v>
@@ -9030,16 +9112,16 @@
     </row>
     <row r="5" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="E5" s="46" t="s">
         <v>469</v>
@@ -9063,16 +9145,16 @@
     </row>
     <row r="6" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>702</v>
+        <v>696</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
       <c r="E6" s="46" t="s">
         <v>469</v>
@@ -9125,15 +9207,15 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>63</v>
@@ -9154,15 +9236,15 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>708</v>
+        <v>702</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>709</v>
+        <v>703</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>63</v>
@@ -9179,15 +9261,15 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>711</v>
+        <v>705</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>63</v>
@@ -9204,15 +9286,15 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>63</v>
@@ -9229,15 +9311,15 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>63</v>
@@ -9254,60 +9336,60 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
-        <v>756</v>
+        <v>749</v>
       </c>
       <c r="B13" s="22"/>
       <c r="D13" s="46" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="F13" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="60" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="60" t="b">
+      <c r="G13" s="59" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="59" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="60" t="b">
+      <c r="I13" s="59" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>757</v>
+        <v>750</v>
       </c>
       <c r="B14" s="22"/>
       <c r="D14" s="46" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
       <c r="E14" s="46" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="F14" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="60" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="60" t="b">
+      <c r="G14" s="59" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="59" t="b">
         <v>1</v>
       </c>
-      <c r="I14" s="60" t="b">
+      <c r="I14" s="59" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>760</v>
-      </c>
-      <c r="B15" s="53"/>
+        <v>753</v>
+      </c>
+      <c r="B15" s="52"/>
       <c r="C15" s="23"/>
       <c r="D15" s="46" t="s">
-        <v>772</v>
+        <v>765</v>
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="46" t="s">
@@ -9325,14 +9407,14 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>773</v>
+        <v>766</v>
       </c>
       <c r="B16" s="22"/>
       <c r="D16" s="46" t="s">
-        <v>774</v>
+        <v>767</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>790</v>
+        <v>783</v>
       </c>
       <c r="F16" s="46" t="s">
         <v>64</v>
@@ -9349,14 +9431,14 @@
     </row>
     <row r="17" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>781</v>
-      </c>
-      <c r="B17" s="53"/>
+        <v>774</v>
+      </c>
+      <c r="B17" s="52"/>
       <c r="D17" s="46" t="s">
-        <v>782</v>
+        <v>775</v>
       </c>
       <c r="E17" s="46" t="s">
-        <v>787</v>
+        <v>780</v>
       </c>
       <c r="F17" s="46" t="s">
         <v>64</v>
@@ -9373,14 +9455,14 @@
     </row>
     <row r="18" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>783</v>
-      </c>
-      <c r="B18" s="53"/>
+        <v>776</v>
+      </c>
+      <c r="B18" s="52"/>
       <c r="D18" s="46" t="s">
-        <v>784</v>
+        <v>777</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>788</v>
+        <v>781</v>
       </c>
       <c r="F18" s="46" t="s">
         <v>63</v>
@@ -9397,14 +9479,14 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
-        <v>789</v>
+        <v>782</v>
       </c>
       <c r="B19" s="22"/>
       <c r="D19" s="46" t="s">
-        <v>791</v>
+        <v>784</v>
       </c>
       <c r="E19" s="46" t="s">
-        <v>790</v>
+        <v>783</v>
       </c>
       <c r="F19" s="46" t="s">
         <v>64</v>

</xml_diff>